<commit_message>
Adding the recognizer option to the system.
</commit_message>
<xml_diff>
--- a/MasterThesis/experiments/neural.xlsx
+++ b/MasterThesis/experiments/neural.xlsx
@@ -7,14 +7,15 @@
     <workbookView xWindow="120" yWindow="15" windowWidth="18975" windowHeight="11955"/>
   </bookViews>
   <sheets>
-    <sheet name="neural" sheetId="1" r:id="rId1"/>
+    <sheet name="класификация" sheetId="1" r:id="rId1"/>
+    <sheet name="разпознаване" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="22">
   <si>
     <t>Backpropagation, 6 експеримента, 82 обучаващи, 20 верифициращи, 10000 итерации в мрежата</t>
   </si>
@@ -77,6 +78,9 @@
   </si>
   <si>
     <t>20_3</t>
+  </si>
+  <si>
+    <t>Измерения \ Шум</t>
   </si>
 </sst>
 </file>
@@ -240,7 +244,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="30">
+  <fills count="31">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -391,6 +395,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -715,7 +725,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -734,6 +744,20 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="27" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="27" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="27" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="28" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -743,20 +767,10 @@
     <xf numFmtId="0" fontId="0" fillId="28" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="27" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="27" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="27" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Акцент1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -1172,7 +1186,7 @@
   <dimension ref="A1:O27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33:D34"/>
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1185,13 +1199,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="18"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="26"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -1221,7 +1235,7 @@
       </c>
     </row>
     <row r="3" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="19" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="5">
@@ -1236,15 +1250,15 @@
       <c r="E3" s="5">
         <v>0.75829999999999997</v>
       </c>
-      <c r="H3" s="16" t="s">
+      <c r="H3" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="18"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="26"/>
     </row>
     <row r="4" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="20" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="5">
@@ -1273,7 +1287,7 @@
       </c>
     </row>
     <row r="5" spans="1:15">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="8">
@@ -1288,7 +1302,7 @@
       <c r="E5" s="8">
         <v>0.66659999999999997</v>
       </c>
-      <c r="H5" s="25" t="s">
+      <c r="H5" s="19" t="s">
         <v>6</v>
       </c>
       <c r="I5" s="2">
@@ -1302,7 +1316,7 @@
       </c>
     </row>
     <row r="6" spans="1:15">
-      <c r="H6" s="26" t="s">
+      <c r="H6" s="20" t="s">
         <v>8</v>
       </c>
       <c r="I6" s="2">
@@ -1316,7 +1330,7 @@
       </c>
     </row>
     <row r="7" spans="1:15" ht="15.75" thickBot="1">
-      <c r="H7" s="26" t="s">
+      <c r="H7" s="20" t="s">
         <v>11</v>
       </c>
       <c r="I7" s="3">
@@ -1330,13 +1344,13 @@
       </c>
     </row>
     <row r="8" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="18"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="26"/>
     </row>
     <row r="9" spans="1:15" ht="15.75" thickBot="1">
       <c r="A9" s="4" t="s">
@@ -1356,7 +1370,7 @@
       </c>
     </row>
     <row r="10" spans="1:15">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="19" t="s">
         <v>6</v>
       </c>
       <c r="B10" s="5">
@@ -1373,7 +1387,7 @@
       </c>
     </row>
     <row r="11" spans="1:15">
-      <c r="A11" s="26" t="s">
+      <c r="A11" s="20" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="9">
@@ -1390,7 +1404,7 @@
       </c>
     </row>
     <row r="12" spans="1:15">
-      <c r="A12" s="26" t="s">
+      <c r="A12" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="6">
@@ -1408,13 +1422,13 @@
     </row>
     <row r="14" spans="1:15" ht="15.75" thickBot="1"/>
     <row r="15" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A15" s="16" t="s">
+      <c r="A15" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="18"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="26"/>
     </row>
     <row r="16" spans="1:15" ht="15.75" thickBot="1">
       <c r="A16" s="4" t="s">
@@ -1434,7 +1448,7 @@
       </c>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="25" t="s">
+      <c r="A17" s="19" t="s">
         <v>6</v>
       </c>
       <c r="B17" s="6">
@@ -1451,7 +1465,7 @@
       </c>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="26" t="s">
+      <c r="A18" s="20" t="s">
         <v>8</v>
       </c>
       <c r="B18" s="5">
@@ -1468,7 +1482,7 @@
       </c>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="26" t="s">
+      <c r="A19" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B19" s="8">
@@ -1486,13 +1500,13 @@
     </row>
     <row r="22" spans="1:5" ht="15.75" thickBot="1"/>
     <row r="23" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A23" s="19" t="s">
+      <c r="A23" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="20"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="21"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="23"/>
     </row>
     <row r="24" spans="1:5" ht="15.75" thickBot="1">
       <c r="A24" s="4" t="s">
@@ -1512,7 +1526,7 @@
       </c>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="25" t="s">
+      <c r="A25" s="19" t="s">
         <v>6</v>
       </c>
       <c r="B25" s="13">
@@ -1521,7 +1535,7 @@
       <c r="C25" s="12">
         <v>0.87</v>
       </c>
-      <c r="D25" s="22">
+      <c r="D25" s="16">
         <v>0.88500000000000001</v>
       </c>
       <c r="E25" s="5">
@@ -1529,7 +1543,7 @@
       </c>
     </row>
     <row r="26" spans="1:5">
-      <c r="A26" s="26" t="s">
+      <c r="A26" s="20" t="s">
         <v>8</v>
       </c>
       <c r="B26" s="12">
@@ -1541,12 +1555,12 @@
       <c r="D26" s="14">
         <v>0.78500000000000003</v>
       </c>
-      <c r="E26" s="23">
+      <c r="E26" s="17">
         <v>0.79249999999999998</v>
       </c>
     </row>
     <row r="27" spans="1:5">
-      <c r="A27" s="26" t="s">
+      <c r="A27" s="20" t="s">
         <v>11</v>
       </c>
       <c r="B27" s="8">
@@ -1555,7 +1569,7 @@
       <c r="C27" s="8">
         <v>0.86250000000000004</v>
       </c>
-      <c r="D27" s="24">
+      <c r="D27" s="18">
         <v>0.9</v>
       </c>
       <c r="E27" s="15">
@@ -1574,4 +1588,143 @@
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="17.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15.75" thickBot="1"/>
+    <row r="2" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A2" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="30">
+        <v>0.1</v>
+      </c>
+      <c r="C2" s="30">
+        <v>0.2</v>
+      </c>
+      <c r="D2" s="30">
+        <v>0.3</v>
+      </c>
+      <c r="E2" s="30">
+        <v>0.4</v>
+      </c>
+      <c r="F2" s="28">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="19">
+        <v>5</v>
+      </c>
+      <c r="B3" s="3">
+        <v>100</v>
+      </c>
+      <c r="C3" s="3">
+        <v>73.529399999999995</v>
+      </c>
+      <c r="D3" s="3">
+        <v>42.156799999999997</v>
+      </c>
+      <c r="E3" s="3">
+        <v>23.529399999999999</v>
+      </c>
+      <c r="F3" s="3">
+        <v>12.745100000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="20">
+        <v>10</v>
+      </c>
+      <c r="B4" s="29">
+        <v>100</v>
+      </c>
+      <c r="C4" s="29">
+        <v>99.019599999999997</v>
+      </c>
+      <c r="D4" s="29">
+        <v>77.450999999999993</v>
+      </c>
+      <c r="E4" s="29">
+        <v>48.039200000000001</v>
+      </c>
+      <c r="F4" s="29">
+        <v>28.4314</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="20">
+        <v>15</v>
+      </c>
+      <c r="B5" s="29">
+        <v>100</v>
+      </c>
+      <c r="C5" s="29">
+        <v>100</v>
+      </c>
+      <c r="D5" s="29">
+        <v>86.274500000000003</v>
+      </c>
+      <c r="E5" s="29">
+        <v>56.862699999999997</v>
+      </c>
+      <c r="F5" s="29">
+        <v>33.333300000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="20">
+        <v>20</v>
+      </c>
+      <c r="B6" s="29">
+        <v>100</v>
+      </c>
+      <c r="C6" s="29">
+        <v>100</v>
+      </c>
+      <c r="D6" s="29">
+        <v>89.215699999999998</v>
+      </c>
+      <c r="E6" s="29">
+        <v>62.745100000000001</v>
+      </c>
+      <c r="F6" s="29">
+        <v>36.274500000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="20">
+        <v>102</v>
+      </c>
+      <c r="B7" s="29">
+        <v>100</v>
+      </c>
+      <c r="C7" s="29">
+        <v>100</v>
+      </c>
+      <c r="D7" s="29">
+        <v>100</v>
+      </c>
+      <c r="E7" s="29">
+        <v>94.117599999999996</v>
+      </c>
+      <c r="F7" s="29">
+        <v>63.725499999999997</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Committing the results of all nearest neighbour tests.
</commit_message>
<xml_diff>
--- a/MasterThesis/experiments/neural.xlsx
+++ b/MasterThesis/experiments/neural.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="15" windowWidth="18975" windowHeight="11955"/>
+    <workbookView xWindow="120" yWindow="15" windowWidth="18975" windowHeight="11955" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="класификация" sheetId="1" r:id="rId1"/>
     <sheet name="разпознаване" sheetId="2" r:id="rId2"/>
+    <sheet name="Лист1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="27">
   <si>
     <t>Backpropagation, 6 експеримента, 82 обучаващи, 20 верифициращи, 10000 итерации в мрежата</t>
   </si>
@@ -81,6 +82,21 @@
   </si>
   <si>
     <t>Измерения \ Шум</t>
+  </si>
+  <si>
+    <t>Classifier: Nearest neighbor</t>
+  </si>
+  <si>
+    <t>Train set</t>
+  </si>
+  <si>
+    <t>Classifier: Weighted nn</t>
+  </si>
+  <si>
+    <t>Classifier: Correlated nn</t>
+  </si>
+  <si>
+    <t>MAX</t>
   </si>
 </sst>
 </file>
@@ -244,7 +260,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="31">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -404,8 +420,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="22">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -680,6 +708,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -725,7 +762,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -749,6 +786,10 @@
     <xf numFmtId="9" fontId="0" fillId="27" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="29" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="29" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="28" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -767,10 +808,17 @@
     <xf numFmtId="0" fontId="0" fillId="28" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Акцент1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -886,8 +934,8 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
     <mruColors>
+      <color rgb="FFFFFF99"/>
       <color rgb="FFFFFFCC"/>
-      <color rgb="FFFFFF99"/>
       <color rgb="FFFFCC99"/>
       <color rgb="FF9966FF"/>
       <color rgb="FF993366"/>
@@ -1185,7 +1233,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
@@ -1199,13 +1247,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="26"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="30"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -1250,12 +1298,12 @@
       <c r="E3" s="5">
         <v>0.75829999999999997</v>
       </c>
-      <c r="H3" s="24" t="s">
+      <c r="H3" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="26"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="30"/>
     </row>
     <row r="4" spans="1:15" ht="15.75" thickBot="1">
       <c r="A4" s="20" t="s">
@@ -1344,13 +1392,13 @@
       </c>
     </row>
     <row r="8" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="25"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="26"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="30"/>
     </row>
     <row r="9" spans="1:15" ht="15.75" thickBot="1">
       <c r="A9" s="4" t="s">
@@ -1422,13 +1470,13 @@
     </row>
     <row r="14" spans="1:15" ht="15.75" thickBot="1"/>
     <row r="15" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A15" s="24" t="s">
+      <c r="A15" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="25"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="26"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="30"/>
     </row>
     <row r="16" spans="1:15" ht="15.75" thickBot="1">
       <c r="A16" s="4" t="s">
@@ -1500,13 +1548,13 @@
     </row>
     <row r="22" spans="1:5" ht="15.75" thickBot="1"/>
     <row r="23" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A23" s="21" t="s">
+      <c r="A23" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="22"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="22"/>
-      <c r="E23" s="23"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="26"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="27"/>
     </row>
     <row r="24" spans="1:5" ht="15.75" thickBot="1">
       <c r="A24" s="4" t="s">
@@ -1605,22 +1653,22 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1"/>
     <row r="2" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="30">
+      <c r="B2" s="24">
         <v>0.1</v>
       </c>
-      <c r="C2" s="30">
+      <c r="C2" s="24">
         <v>0.2</v>
       </c>
-      <c r="D2" s="30">
+      <c r="D2" s="24">
         <v>0.3</v>
       </c>
-      <c r="E2" s="30">
+      <c r="E2" s="24">
         <v>0.4</v>
       </c>
-      <c r="F2" s="28">
+      <c r="F2" s="22">
         <v>0.5</v>
       </c>
     </row>
@@ -1648,19 +1696,19 @@
       <c r="A4" s="20">
         <v>10</v>
       </c>
-      <c r="B4" s="29">
+      <c r="B4" s="23">
         <v>100</v>
       </c>
-      <c r="C4" s="29">
+      <c r="C4" s="23">
         <v>99.019599999999997</v>
       </c>
-      <c r="D4" s="29">
+      <c r="D4" s="23">
         <v>77.450999999999993</v>
       </c>
-      <c r="E4" s="29">
+      <c r="E4" s="23">
         <v>48.039200000000001</v>
       </c>
-      <c r="F4" s="29">
+      <c r="F4" s="23">
         <v>28.4314</v>
       </c>
     </row>
@@ -1668,19 +1716,19 @@
       <c r="A5" s="20">
         <v>15</v>
       </c>
-      <c r="B5" s="29">
+      <c r="B5" s="23">
         <v>100</v>
       </c>
-      <c r="C5" s="29">
+      <c r="C5" s="23">
         <v>100</v>
       </c>
-      <c r="D5" s="29">
+      <c r="D5" s="23">
         <v>86.274500000000003</v>
       </c>
-      <c r="E5" s="29">
+      <c r="E5" s="23">
         <v>56.862699999999997</v>
       </c>
-      <c r="F5" s="29">
+      <c r="F5" s="23">
         <v>33.333300000000001</v>
       </c>
     </row>
@@ -1688,19 +1736,19 @@
       <c r="A6" s="20">
         <v>20</v>
       </c>
-      <c r="B6" s="29">
+      <c r="B6" s="23">
         <v>100</v>
       </c>
-      <c r="C6" s="29">
+      <c r="C6" s="23">
         <v>100</v>
       </c>
-      <c r="D6" s="29">
+      <c r="D6" s="23">
         <v>89.215699999999998</v>
       </c>
-      <c r="E6" s="29">
+      <c r="E6" s="23">
         <v>62.745100000000001</v>
       </c>
-      <c r="F6" s="29">
+      <c r="F6" s="23">
         <v>36.274500000000003</v>
       </c>
     </row>
@@ -1708,23 +1756,3819 @@
       <c r="A7" s="20">
         <v>102</v>
       </c>
-      <c r="B7" s="29">
+      <c r="B7" s="23">
         <v>100</v>
       </c>
-      <c r="C7" s="29">
+      <c r="C7" s="23">
         <v>100</v>
       </c>
-      <c r="D7" s="29">
+      <c r="D7" s="23">
         <v>100</v>
       </c>
-      <c r="E7" s="29">
+      <c r="E7" s="23">
         <v>94.117599999999996</v>
       </c>
-      <c r="F7" s="29">
+      <c r="F7" s="23">
         <v>63.725499999999997</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:CY17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="CW6" sqref="CW6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:103">
+      <c r="A1" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+    </row>
+    <row r="2" spans="1:103">
+      <c r="A2" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="31">
+        <v>1</v>
+      </c>
+      <c r="C2" s="31">
+        <v>2</v>
+      </c>
+      <c r="D2" s="31">
+        <v>3</v>
+      </c>
+      <c r="E2" s="31">
+        <v>4</v>
+      </c>
+      <c r="F2" s="31">
+        <v>5</v>
+      </c>
+      <c r="G2" s="31">
+        <v>6</v>
+      </c>
+      <c r="H2" s="31">
+        <v>7</v>
+      </c>
+      <c r="I2" s="31">
+        <v>8</v>
+      </c>
+      <c r="J2" s="31">
+        <v>9</v>
+      </c>
+      <c r="K2" s="31">
+        <v>10</v>
+      </c>
+      <c r="L2" s="31">
+        <v>11</v>
+      </c>
+      <c r="M2" s="31">
+        <v>12</v>
+      </c>
+      <c r="N2" s="31">
+        <v>13</v>
+      </c>
+      <c r="O2" s="31">
+        <v>14</v>
+      </c>
+      <c r="P2" s="31">
+        <v>15</v>
+      </c>
+      <c r="Q2" s="31">
+        <v>16</v>
+      </c>
+      <c r="R2" s="31">
+        <v>17</v>
+      </c>
+      <c r="S2" s="31">
+        <v>18</v>
+      </c>
+      <c r="T2" s="31">
+        <v>19</v>
+      </c>
+      <c r="U2" s="31">
+        <v>20</v>
+      </c>
+      <c r="V2" s="31">
+        <v>21</v>
+      </c>
+      <c r="W2" s="31">
+        <v>22</v>
+      </c>
+      <c r="X2" s="31">
+        <v>23</v>
+      </c>
+      <c r="Y2" s="31">
+        <v>24</v>
+      </c>
+      <c r="Z2" s="31">
+        <v>25</v>
+      </c>
+      <c r="AA2" s="31">
+        <v>26</v>
+      </c>
+      <c r="AB2" s="31">
+        <v>27</v>
+      </c>
+      <c r="AC2" s="31">
+        <v>28</v>
+      </c>
+      <c r="AD2" s="31">
+        <v>29</v>
+      </c>
+      <c r="AE2" s="31">
+        <v>30</v>
+      </c>
+      <c r="AF2" s="31">
+        <v>31</v>
+      </c>
+      <c r="AG2" s="31">
+        <v>32</v>
+      </c>
+      <c r="AH2" s="31">
+        <v>33</v>
+      </c>
+      <c r="AI2" s="31">
+        <v>34</v>
+      </c>
+      <c r="AJ2" s="31">
+        <v>35</v>
+      </c>
+      <c r="AK2" s="31">
+        <v>36</v>
+      </c>
+      <c r="AL2" s="31">
+        <v>37</v>
+      </c>
+      <c r="AM2" s="31">
+        <v>38</v>
+      </c>
+      <c r="AN2" s="31">
+        <v>39</v>
+      </c>
+      <c r="AO2" s="31">
+        <v>40</v>
+      </c>
+      <c r="AP2" s="31">
+        <v>41</v>
+      </c>
+      <c r="AQ2" s="31">
+        <v>42</v>
+      </c>
+      <c r="AR2" s="31">
+        <v>43</v>
+      </c>
+      <c r="AS2" s="31">
+        <v>44</v>
+      </c>
+      <c r="AT2" s="31">
+        <v>45</v>
+      </c>
+      <c r="AU2" s="31">
+        <v>46</v>
+      </c>
+      <c r="AV2" s="31">
+        <v>47</v>
+      </c>
+      <c r="AW2" s="31">
+        <v>48</v>
+      </c>
+      <c r="AX2" s="31">
+        <v>49</v>
+      </c>
+      <c r="AY2" s="31">
+        <v>50</v>
+      </c>
+      <c r="AZ2" s="31">
+        <v>51</v>
+      </c>
+      <c r="BA2" s="31">
+        <v>52</v>
+      </c>
+      <c r="BB2" s="31">
+        <v>53</v>
+      </c>
+      <c r="BC2" s="31">
+        <v>54</v>
+      </c>
+      <c r="BD2" s="31">
+        <v>55</v>
+      </c>
+      <c r="BE2" s="31">
+        <v>56</v>
+      </c>
+      <c r="BF2" s="31">
+        <v>57</v>
+      </c>
+      <c r="BG2" s="31">
+        <v>58</v>
+      </c>
+      <c r="BH2" s="31">
+        <v>59</v>
+      </c>
+      <c r="BI2" s="31">
+        <v>60</v>
+      </c>
+      <c r="BJ2" s="31">
+        <v>61</v>
+      </c>
+      <c r="BK2" s="31">
+        <v>62</v>
+      </c>
+      <c r="BL2" s="31">
+        <v>63</v>
+      </c>
+      <c r="BM2" s="31">
+        <v>64</v>
+      </c>
+      <c r="BN2" s="31">
+        <v>65</v>
+      </c>
+      <c r="BO2" s="31">
+        <v>66</v>
+      </c>
+      <c r="BP2" s="31">
+        <v>67</v>
+      </c>
+      <c r="BQ2" s="31">
+        <v>68</v>
+      </c>
+      <c r="BR2" s="31">
+        <v>69</v>
+      </c>
+      <c r="BS2" s="31">
+        <v>70</v>
+      </c>
+      <c r="BT2" s="31">
+        <v>71</v>
+      </c>
+      <c r="BU2" s="31">
+        <v>72</v>
+      </c>
+      <c r="BV2" s="31">
+        <v>73</v>
+      </c>
+      <c r="BW2" s="31">
+        <v>74</v>
+      </c>
+      <c r="BX2" s="31">
+        <v>75</v>
+      </c>
+      <c r="BY2" s="31">
+        <v>76</v>
+      </c>
+      <c r="BZ2" s="31">
+        <v>77</v>
+      </c>
+      <c r="CA2" s="31">
+        <v>78</v>
+      </c>
+      <c r="CB2" s="31">
+        <v>79</v>
+      </c>
+      <c r="CC2" s="31">
+        <v>80</v>
+      </c>
+      <c r="CD2" s="31">
+        <v>81</v>
+      </c>
+      <c r="CE2" s="31">
+        <v>82</v>
+      </c>
+      <c r="CF2" s="31">
+        <v>83</v>
+      </c>
+      <c r="CG2" s="31">
+        <v>84</v>
+      </c>
+      <c r="CH2" s="31">
+        <v>85</v>
+      </c>
+      <c r="CI2" s="31">
+        <v>86</v>
+      </c>
+      <c r="CJ2" s="31">
+        <v>87</v>
+      </c>
+      <c r="CK2" s="31">
+        <v>88</v>
+      </c>
+      <c r="CL2" s="31">
+        <v>89</v>
+      </c>
+      <c r="CM2" s="31">
+        <v>90</v>
+      </c>
+      <c r="CN2" s="31">
+        <v>91</v>
+      </c>
+      <c r="CO2" s="31">
+        <v>92</v>
+      </c>
+      <c r="CP2" s="31">
+        <v>93</v>
+      </c>
+      <c r="CQ2" s="31">
+        <v>94</v>
+      </c>
+      <c r="CR2" s="31">
+        <v>95</v>
+      </c>
+      <c r="CS2" s="31">
+        <v>96</v>
+      </c>
+      <c r="CT2" s="31">
+        <v>97</v>
+      </c>
+      <c r="CU2" s="31">
+        <v>98</v>
+      </c>
+      <c r="CV2" s="31">
+        <v>99</v>
+      </c>
+      <c r="CW2" s="31">
+        <v>100</v>
+      </c>
+      <c r="CX2" s="31">
+        <v>101</v>
+      </c>
+      <c r="CY2" s="34" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:103">
+      <c r="A3" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="23">
+        <v>54.333300000000001</v>
+      </c>
+      <c r="C3" s="23">
+        <v>56.916699999999999</v>
+      </c>
+      <c r="D3" s="23">
+        <v>56.083300000000001</v>
+      </c>
+      <c r="E3" s="23">
+        <v>50.75</v>
+      </c>
+      <c r="F3" s="23">
+        <v>53.333300000000001</v>
+      </c>
+      <c r="G3" s="23">
+        <v>52.083300000000001</v>
+      </c>
+      <c r="H3" s="23">
+        <v>50.5</v>
+      </c>
+      <c r="I3" s="23">
+        <v>51.25</v>
+      </c>
+      <c r="J3" s="23">
+        <v>50.833300000000001</v>
+      </c>
+      <c r="K3" s="23">
+        <v>47.666699999999999</v>
+      </c>
+      <c r="L3" s="23">
+        <v>48.416699999999999</v>
+      </c>
+      <c r="M3" s="23">
+        <v>49.166699999999999</v>
+      </c>
+      <c r="N3" s="23">
+        <v>49.583300000000001</v>
+      </c>
+      <c r="O3" s="23">
+        <v>48.833300000000001</v>
+      </c>
+      <c r="P3" s="23">
+        <v>48.583300000000001</v>
+      </c>
+      <c r="Q3" s="23">
+        <v>49.083300000000001</v>
+      </c>
+      <c r="R3" s="23">
+        <v>49.166699999999999</v>
+      </c>
+      <c r="S3" s="23">
+        <v>48</v>
+      </c>
+      <c r="T3" s="23">
+        <v>48.666699999999999</v>
+      </c>
+      <c r="U3" s="23">
+        <v>48.916699999999999</v>
+      </c>
+      <c r="V3" s="23">
+        <v>47.333300000000001</v>
+      </c>
+      <c r="W3" s="23">
+        <v>47.416699999999999</v>
+      </c>
+      <c r="X3" s="23">
+        <v>47.416699999999999</v>
+      </c>
+      <c r="Y3" s="23">
+        <v>48.666699999999999</v>
+      </c>
+      <c r="Z3" s="23">
+        <v>48.75</v>
+      </c>
+      <c r="AA3" s="23">
+        <v>49</v>
+      </c>
+      <c r="AB3" s="23">
+        <v>49.166699999999999</v>
+      </c>
+      <c r="AC3" s="23">
+        <v>49.166699999999999</v>
+      </c>
+      <c r="AD3" s="23">
+        <v>49.333300000000001</v>
+      </c>
+      <c r="AE3" s="23">
+        <v>49.083300000000001</v>
+      </c>
+      <c r="AF3" s="23">
+        <v>48.75</v>
+      </c>
+      <c r="AG3" s="23">
+        <v>49.833300000000001</v>
+      </c>
+      <c r="AH3" s="23">
+        <v>51.916699999999999</v>
+      </c>
+      <c r="AI3" s="23">
+        <v>50.083300000000001</v>
+      </c>
+      <c r="AJ3" s="23">
+        <v>49.75</v>
+      </c>
+      <c r="AK3" s="23">
+        <v>49.5</v>
+      </c>
+      <c r="AL3" s="23">
+        <v>49.083300000000001</v>
+      </c>
+      <c r="AM3" s="23">
+        <v>48.75</v>
+      </c>
+      <c r="AN3" s="23">
+        <v>48.666699999999999</v>
+      </c>
+      <c r="AO3" s="23">
+        <v>48.916699999999999</v>
+      </c>
+      <c r="AP3" s="23">
+        <v>48.833300000000001</v>
+      </c>
+      <c r="AQ3" s="23">
+        <v>48.916699999999999</v>
+      </c>
+      <c r="AR3" s="23">
+        <v>48.5</v>
+      </c>
+      <c r="AS3" s="23">
+        <v>48.916699999999999</v>
+      </c>
+      <c r="AT3" s="23">
+        <v>49</v>
+      </c>
+      <c r="AU3" s="23">
+        <v>48.416699999999999</v>
+      </c>
+      <c r="AV3" s="23">
+        <v>48.75</v>
+      </c>
+      <c r="AW3" s="23">
+        <v>48.916699999999999</v>
+      </c>
+      <c r="AX3" s="23">
+        <v>49.416699999999999</v>
+      </c>
+      <c r="AY3" s="23">
+        <v>49.166699999999999</v>
+      </c>
+      <c r="AZ3" s="23">
+        <v>50.333300000000001</v>
+      </c>
+      <c r="BA3" s="23">
+        <v>49.75</v>
+      </c>
+      <c r="BB3" s="23">
+        <v>49.416699999999999</v>
+      </c>
+      <c r="BC3" s="23">
+        <v>49.333300000000001</v>
+      </c>
+      <c r="BD3" s="23">
+        <v>49.666699999999999</v>
+      </c>
+      <c r="BE3" s="23">
+        <v>49.75</v>
+      </c>
+      <c r="BF3" s="23">
+        <v>49.166699999999999</v>
+      </c>
+      <c r="BG3" s="23">
+        <v>48.5</v>
+      </c>
+      <c r="BH3" s="23">
+        <v>49.5</v>
+      </c>
+      <c r="BI3" s="23">
+        <v>49.583300000000001</v>
+      </c>
+      <c r="BJ3" s="23">
+        <v>49.416699999999999</v>
+      </c>
+      <c r="BK3" s="23">
+        <v>50.25</v>
+      </c>
+      <c r="BL3" s="23">
+        <v>48.75</v>
+      </c>
+      <c r="BM3" s="23">
+        <v>49.083300000000001</v>
+      </c>
+      <c r="BN3" s="23">
+        <v>49.75</v>
+      </c>
+      <c r="BO3" s="23">
+        <v>49.333300000000001</v>
+      </c>
+      <c r="BP3" s="23">
+        <v>49.5</v>
+      </c>
+      <c r="BQ3" s="23">
+        <v>49.333300000000001</v>
+      </c>
+      <c r="BR3" s="23">
+        <v>48.666699999999999</v>
+      </c>
+      <c r="BS3" s="23">
+        <v>48.333300000000001</v>
+      </c>
+      <c r="BT3" s="23">
+        <v>48.5</v>
+      </c>
+      <c r="BU3" s="23">
+        <v>49.083300000000001</v>
+      </c>
+      <c r="BV3" s="23">
+        <v>49.166699999999999</v>
+      </c>
+      <c r="BW3" s="23">
+        <v>48.5</v>
+      </c>
+      <c r="BX3" s="23">
+        <v>48.583300000000001</v>
+      </c>
+      <c r="BY3" s="23">
+        <v>48.333300000000001</v>
+      </c>
+      <c r="BZ3" s="23">
+        <v>48.75</v>
+      </c>
+      <c r="CA3" s="23">
+        <v>48.583300000000001</v>
+      </c>
+      <c r="CB3" s="23">
+        <v>48.083300000000001</v>
+      </c>
+      <c r="CC3" s="23">
+        <v>48.5</v>
+      </c>
+      <c r="CD3" s="23">
+        <v>48</v>
+      </c>
+      <c r="CE3" s="23">
+        <v>48.833300000000001</v>
+      </c>
+      <c r="CF3" s="23">
+        <v>48.25</v>
+      </c>
+      <c r="CG3" s="23">
+        <v>48.583300000000001</v>
+      </c>
+      <c r="CH3" s="23">
+        <v>48.75</v>
+      </c>
+      <c r="CI3" s="23">
+        <v>47.75</v>
+      </c>
+      <c r="CJ3" s="23">
+        <v>47.75</v>
+      </c>
+      <c r="CK3" s="23">
+        <v>48.166699999999999</v>
+      </c>
+      <c r="CL3" s="23">
+        <v>47.5</v>
+      </c>
+      <c r="CM3" s="23">
+        <v>48.166699999999999</v>
+      </c>
+      <c r="CN3" s="23">
+        <v>47.75</v>
+      </c>
+      <c r="CO3" s="23">
+        <v>48.166699999999999</v>
+      </c>
+      <c r="CP3" s="23">
+        <v>49.166699999999999</v>
+      </c>
+      <c r="CQ3" s="23">
+        <v>48.75</v>
+      </c>
+      <c r="CR3" s="23">
+        <v>48.833300000000001</v>
+      </c>
+      <c r="CS3" s="23">
+        <v>48.5</v>
+      </c>
+      <c r="CT3" s="23">
+        <v>48.083300000000001</v>
+      </c>
+      <c r="CU3" s="23">
+        <v>48.25</v>
+      </c>
+      <c r="CV3" s="23">
+        <v>47.916699999999999</v>
+      </c>
+      <c r="CW3" s="23">
+        <v>48</v>
+      </c>
+      <c r="CX3" s="23">
+        <v>48.083300000000001</v>
+      </c>
+      <c r="CY3" s="23">
+        <f>MAX(B3:CX3)</f>
+        <v>56.916699999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:103">
+      <c r="A4" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="23">
+        <v>79.666700000000006</v>
+      </c>
+      <c r="C4" s="23">
+        <v>79.75</v>
+      </c>
+      <c r="D4" s="23">
+        <v>79.666700000000006</v>
+      </c>
+      <c r="E4" s="23">
+        <v>82.583299999999994</v>
+      </c>
+      <c r="F4" s="23">
+        <v>81.583299999999994</v>
+      </c>
+      <c r="G4" s="23">
+        <v>82.833299999999994</v>
+      </c>
+      <c r="H4" s="23">
+        <v>82.583299999999994</v>
+      </c>
+      <c r="I4" s="23">
+        <v>82.916700000000006</v>
+      </c>
+      <c r="J4" s="23">
+        <v>81.583299999999994</v>
+      </c>
+      <c r="K4" s="23">
+        <v>83.083299999999994</v>
+      </c>
+      <c r="L4" s="23">
+        <v>82.666700000000006</v>
+      </c>
+      <c r="M4" s="23">
+        <v>82.333299999999994</v>
+      </c>
+      <c r="N4" s="23">
+        <v>81.75</v>
+      </c>
+      <c r="O4" s="23">
+        <v>81.916700000000006</v>
+      </c>
+      <c r="P4" s="23">
+        <v>82</v>
+      </c>
+      <c r="Q4" s="23">
+        <v>81.5</v>
+      </c>
+      <c r="R4" s="23">
+        <v>81.166700000000006</v>
+      </c>
+      <c r="S4" s="23">
+        <v>82.083299999999994</v>
+      </c>
+      <c r="T4" s="23">
+        <v>82.25</v>
+      </c>
+      <c r="U4" s="23">
+        <v>81.916700000000006</v>
+      </c>
+      <c r="V4" s="23">
+        <v>82</v>
+      </c>
+      <c r="W4" s="23">
+        <v>81.833299999999994</v>
+      </c>
+      <c r="X4" s="23">
+        <v>81.75</v>
+      </c>
+      <c r="Y4" s="23">
+        <v>81.25</v>
+      </c>
+      <c r="Z4" s="23">
+        <v>81.416700000000006</v>
+      </c>
+      <c r="AA4" s="23">
+        <v>81.916700000000006</v>
+      </c>
+      <c r="AB4" s="23">
+        <v>81.25</v>
+      </c>
+      <c r="AC4" s="23">
+        <v>80.416700000000006</v>
+      </c>
+      <c r="AD4" s="23">
+        <v>81.166700000000006</v>
+      </c>
+      <c r="AE4" s="23">
+        <v>82.166700000000006</v>
+      </c>
+      <c r="AF4" s="23">
+        <v>80</v>
+      </c>
+      <c r="AG4" s="23">
+        <v>80.5</v>
+      </c>
+      <c r="AH4" s="23">
+        <v>81.416700000000006</v>
+      </c>
+      <c r="AI4" s="23">
+        <v>81.166700000000006</v>
+      </c>
+      <c r="AJ4" s="23">
+        <v>81.166700000000006</v>
+      </c>
+      <c r="AK4" s="23">
+        <v>80.5</v>
+      </c>
+      <c r="AL4" s="23">
+        <v>80.916700000000006</v>
+      </c>
+      <c r="AM4" s="23">
+        <v>81.5</v>
+      </c>
+      <c r="AN4" s="23">
+        <v>81.083299999999994</v>
+      </c>
+      <c r="AO4" s="23">
+        <v>81.333299999999994</v>
+      </c>
+      <c r="AP4" s="23">
+        <v>81.083299999999994</v>
+      </c>
+      <c r="AQ4" s="23">
+        <v>80.833299999999994</v>
+      </c>
+      <c r="AR4" s="23">
+        <v>80.416700000000006</v>
+      </c>
+      <c r="AS4" s="23">
+        <v>80.166700000000006</v>
+      </c>
+      <c r="AT4" s="23">
+        <v>80.583299999999994</v>
+      </c>
+      <c r="AU4" s="23">
+        <v>80</v>
+      </c>
+      <c r="AV4" s="23">
+        <v>80.5</v>
+      </c>
+      <c r="AW4" s="23">
+        <v>80.416700000000006</v>
+      </c>
+      <c r="AX4" s="23">
+        <v>80.416700000000006</v>
+      </c>
+      <c r="AY4" s="23">
+        <v>79.916700000000006</v>
+      </c>
+      <c r="AZ4" s="23">
+        <v>80.416700000000006</v>
+      </c>
+      <c r="BA4" s="23">
+        <v>81.5</v>
+      </c>
+      <c r="BB4" s="23">
+        <v>81.583299999999994</v>
+      </c>
+      <c r="BC4" s="23">
+        <v>81.916700000000006</v>
+      </c>
+      <c r="BD4" s="23">
+        <v>81.5</v>
+      </c>
+      <c r="BE4" s="23">
+        <v>80.833299999999994</v>
+      </c>
+      <c r="BF4" s="23">
+        <v>80.583299999999994</v>
+      </c>
+      <c r="BG4" s="23">
+        <v>80.916700000000006</v>
+      </c>
+      <c r="BH4" s="23">
+        <v>80.333299999999994</v>
+      </c>
+      <c r="BI4" s="23">
+        <v>80.916700000000006</v>
+      </c>
+      <c r="BJ4" s="23">
+        <v>81.75</v>
+      </c>
+      <c r="BK4" s="23">
+        <v>81.083299999999994</v>
+      </c>
+      <c r="BL4" s="23">
+        <v>81</v>
+      </c>
+      <c r="BM4" s="23">
+        <v>81</v>
+      </c>
+      <c r="BN4" s="23">
+        <v>82.25</v>
+      </c>
+      <c r="BO4" s="23">
+        <v>81.833299999999994</v>
+      </c>
+      <c r="BP4" s="23">
+        <v>82</v>
+      </c>
+      <c r="BQ4" s="23">
+        <v>82</v>
+      </c>
+      <c r="BR4" s="23">
+        <v>81.666700000000006</v>
+      </c>
+      <c r="BS4" s="23">
+        <v>81.75</v>
+      </c>
+      <c r="BT4" s="23">
+        <v>82.166700000000006</v>
+      </c>
+      <c r="BU4" s="23">
+        <v>81.666700000000006</v>
+      </c>
+      <c r="BV4" s="23">
+        <v>82.25</v>
+      </c>
+      <c r="BW4" s="23">
+        <v>82.416700000000006</v>
+      </c>
+      <c r="BX4" s="23">
+        <v>82.166700000000006</v>
+      </c>
+      <c r="BY4" s="23">
+        <v>82.25</v>
+      </c>
+      <c r="BZ4" s="23">
+        <v>82</v>
+      </c>
+      <c r="CA4" s="23">
+        <v>81.5</v>
+      </c>
+      <c r="CB4" s="23">
+        <v>81.666700000000006</v>
+      </c>
+      <c r="CC4" s="23">
+        <v>81.25</v>
+      </c>
+      <c r="CD4" s="23">
+        <v>81.333299999999994</v>
+      </c>
+      <c r="CE4" s="23">
+        <v>81.333299999999994</v>
+      </c>
+      <c r="CF4" s="23">
+        <v>80.5</v>
+      </c>
+      <c r="CG4" s="23">
+        <v>79.166700000000006</v>
+      </c>
+      <c r="CH4" s="23">
+        <v>79.166700000000006</v>
+      </c>
+      <c r="CI4" s="23">
+        <v>79.416700000000006</v>
+      </c>
+      <c r="CJ4" s="23">
+        <v>79.583299999999994</v>
+      </c>
+      <c r="CK4" s="23">
+        <v>78.833299999999994</v>
+      </c>
+      <c r="CL4" s="23">
+        <v>78.916700000000006</v>
+      </c>
+      <c r="CM4" s="23">
+        <v>78.833299999999994</v>
+      </c>
+      <c r="CN4" s="23">
+        <v>79.083299999999994</v>
+      </c>
+      <c r="CO4" s="23">
+        <v>78.916700000000006</v>
+      </c>
+      <c r="CP4" s="23">
+        <v>79.916700000000006</v>
+      </c>
+      <c r="CQ4" s="23">
+        <v>79.833299999999994</v>
+      </c>
+      <c r="CR4" s="23">
+        <v>79.416700000000006</v>
+      </c>
+      <c r="CS4" s="23">
+        <v>79.5</v>
+      </c>
+      <c r="CT4" s="23">
+        <v>79.916700000000006</v>
+      </c>
+      <c r="CU4" s="23">
+        <v>79.916700000000006</v>
+      </c>
+      <c r="CV4" s="23">
+        <v>80.75</v>
+      </c>
+      <c r="CW4" s="23">
+        <v>80.833299999999994</v>
+      </c>
+      <c r="CX4" s="23">
+        <v>80.916700000000006</v>
+      </c>
+      <c r="CY4" s="23">
+        <f t="shared" ref="CY4:CY17" si="0">MAX(B4:CX4)</f>
+        <v>83.083299999999994</v>
+      </c>
+    </row>
+    <row r="5" spans="1:103">
+      <c r="A5" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="23">
+        <v>72.333299999999994</v>
+      </c>
+      <c r="C5" s="23">
+        <v>73.333299999999994</v>
+      </c>
+      <c r="D5" s="23">
+        <v>80.833299999999994</v>
+      </c>
+      <c r="E5" s="23">
+        <v>83.666700000000006</v>
+      </c>
+      <c r="F5" s="23">
+        <v>83.333299999999994</v>
+      </c>
+      <c r="G5" s="23">
+        <v>82.583299999999994</v>
+      </c>
+      <c r="H5" s="23">
+        <v>83.666700000000006</v>
+      </c>
+      <c r="I5" s="23">
+        <v>83.583299999999994</v>
+      </c>
+      <c r="J5" s="23">
+        <v>84.166700000000006</v>
+      </c>
+      <c r="K5" s="23">
+        <v>84.333299999999994</v>
+      </c>
+      <c r="L5" s="23">
+        <v>84.416700000000006</v>
+      </c>
+      <c r="M5" s="23">
+        <v>84.333299999999994</v>
+      </c>
+      <c r="N5" s="23">
+        <v>84.25</v>
+      </c>
+      <c r="O5" s="23">
+        <v>83.75</v>
+      </c>
+      <c r="P5" s="23">
+        <v>84</v>
+      </c>
+      <c r="Q5" s="23">
+        <v>84.833299999999994</v>
+      </c>
+      <c r="R5" s="23">
+        <v>84.583299999999994</v>
+      </c>
+      <c r="S5" s="23">
+        <v>84.583299999999994</v>
+      </c>
+      <c r="T5" s="23">
+        <v>83.666700000000006</v>
+      </c>
+      <c r="U5" s="23">
+        <v>83.583299999999994</v>
+      </c>
+      <c r="V5" s="23">
+        <v>83.583299999999994</v>
+      </c>
+      <c r="W5" s="23">
+        <v>83</v>
+      </c>
+      <c r="X5" s="23">
+        <v>83.5</v>
+      </c>
+      <c r="Y5" s="23">
+        <v>83.25</v>
+      </c>
+      <c r="Z5" s="23">
+        <v>83.5</v>
+      </c>
+      <c r="AA5" s="23">
+        <v>83.75</v>
+      </c>
+      <c r="AB5" s="23">
+        <v>83.666700000000006</v>
+      </c>
+      <c r="AC5" s="23">
+        <v>83.416700000000006</v>
+      </c>
+      <c r="AD5" s="23">
+        <v>83.833299999999994</v>
+      </c>
+      <c r="AE5" s="23">
+        <v>84.166700000000006</v>
+      </c>
+      <c r="AF5" s="23">
+        <v>84.416700000000006</v>
+      </c>
+      <c r="AG5" s="23">
+        <v>84.5</v>
+      </c>
+      <c r="AH5" s="23">
+        <v>84.333299999999994</v>
+      </c>
+      <c r="AI5" s="23">
+        <v>84.583299999999994</v>
+      </c>
+      <c r="AJ5" s="23">
+        <v>84.166700000000006</v>
+      </c>
+      <c r="AK5" s="23">
+        <v>84.666700000000006</v>
+      </c>
+      <c r="AL5" s="23">
+        <v>84.416700000000006</v>
+      </c>
+      <c r="AM5" s="23">
+        <v>84.25</v>
+      </c>
+      <c r="AN5" s="23">
+        <v>84.25</v>
+      </c>
+      <c r="AO5" s="23">
+        <v>84.75</v>
+      </c>
+      <c r="AP5" s="23">
+        <v>84.583299999999994</v>
+      </c>
+      <c r="AQ5" s="23">
+        <v>84.916700000000006</v>
+      </c>
+      <c r="AR5" s="23">
+        <v>84.583299999999994</v>
+      </c>
+      <c r="AS5" s="23">
+        <v>84.916700000000006</v>
+      </c>
+      <c r="AT5" s="23">
+        <v>84.916700000000006</v>
+      </c>
+      <c r="AU5" s="23">
+        <v>84.833299999999994</v>
+      </c>
+      <c r="AV5" s="23">
+        <v>84.666700000000006</v>
+      </c>
+      <c r="AW5" s="23">
+        <v>84.583299999999994</v>
+      </c>
+      <c r="AX5" s="23">
+        <v>84.583299999999994</v>
+      </c>
+      <c r="AY5" s="23">
+        <v>84.416700000000006</v>
+      </c>
+      <c r="AZ5" s="23">
+        <v>84.75</v>
+      </c>
+      <c r="BA5" s="23">
+        <v>84.416700000000006</v>
+      </c>
+      <c r="BB5" s="23">
+        <v>84.416700000000006</v>
+      </c>
+      <c r="BC5" s="23">
+        <v>84.416700000000006</v>
+      </c>
+      <c r="BD5" s="23">
+        <v>84.25</v>
+      </c>
+      <c r="BE5" s="23">
+        <v>84.333299999999994</v>
+      </c>
+      <c r="BF5" s="23">
+        <v>84</v>
+      </c>
+      <c r="BG5" s="23">
+        <v>83.833299999999994</v>
+      </c>
+      <c r="BH5" s="23">
+        <v>84.083299999999994</v>
+      </c>
+      <c r="BI5" s="23">
+        <v>85.25</v>
+      </c>
+      <c r="BJ5" s="23">
+        <v>85.166700000000006</v>
+      </c>
+      <c r="BK5" s="23">
+        <v>85</v>
+      </c>
+      <c r="BL5" s="23">
+        <v>84.583299999999994</v>
+      </c>
+      <c r="BM5" s="23">
+        <v>84.666700000000006</v>
+      </c>
+      <c r="BN5" s="23">
+        <v>85.083299999999994</v>
+      </c>
+      <c r="BO5" s="23">
+        <v>85.083299999999994</v>
+      </c>
+      <c r="BP5" s="23">
+        <v>84.916700000000006</v>
+      </c>
+      <c r="BQ5" s="23">
+        <v>85</v>
+      </c>
+      <c r="BR5" s="23">
+        <v>85.083299999999994</v>
+      </c>
+      <c r="BS5" s="23">
+        <v>85.083299999999994</v>
+      </c>
+      <c r="BT5" s="23">
+        <v>84.833299999999994</v>
+      </c>
+      <c r="BU5" s="23">
+        <v>84.833299999999994</v>
+      </c>
+      <c r="BV5" s="23">
+        <v>84.916700000000006</v>
+      </c>
+      <c r="BW5" s="23">
+        <v>84.916700000000006</v>
+      </c>
+      <c r="BX5" s="23">
+        <v>84.75</v>
+      </c>
+      <c r="BY5" s="23">
+        <v>84.5</v>
+      </c>
+      <c r="BZ5" s="23">
+        <v>84.5</v>
+      </c>
+      <c r="CA5" s="23">
+        <v>84.666700000000006</v>
+      </c>
+      <c r="CB5" s="23">
+        <v>84.666700000000006</v>
+      </c>
+      <c r="CC5" s="23">
+        <v>84.333299999999994</v>
+      </c>
+      <c r="CD5" s="23">
+        <v>84.333299999999994</v>
+      </c>
+      <c r="CE5" s="23">
+        <v>84.833299999999994</v>
+      </c>
+      <c r="CF5" s="23">
+        <v>84.75</v>
+      </c>
+      <c r="CG5" s="23">
+        <v>84.833299999999994</v>
+      </c>
+      <c r="CH5" s="23">
+        <v>84.833299999999994</v>
+      </c>
+      <c r="CI5" s="23">
+        <v>84.833299999999994</v>
+      </c>
+      <c r="CJ5" s="23">
+        <v>84.916700000000006</v>
+      </c>
+      <c r="CK5" s="23">
+        <v>84.916700000000006</v>
+      </c>
+      <c r="CL5" s="23">
+        <v>84.833299999999994</v>
+      </c>
+      <c r="CM5" s="23">
+        <v>84.583299999999994</v>
+      </c>
+      <c r="CN5" s="23">
+        <v>84.583299999999994</v>
+      </c>
+      <c r="CO5" s="23">
+        <v>84.5</v>
+      </c>
+      <c r="CP5" s="23">
+        <v>84.5</v>
+      </c>
+      <c r="CQ5" s="23">
+        <v>84.666700000000006</v>
+      </c>
+      <c r="CR5" s="23">
+        <v>84.666700000000006</v>
+      </c>
+      <c r="CS5" s="23">
+        <v>84.666700000000006</v>
+      </c>
+      <c r="CT5" s="23">
+        <v>84.666700000000006</v>
+      </c>
+      <c r="CU5" s="23">
+        <v>84.75</v>
+      </c>
+      <c r="CV5" s="23">
+        <v>85</v>
+      </c>
+      <c r="CW5" s="23">
+        <v>84.833299999999994</v>
+      </c>
+      <c r="CX5" s="23">
+        <v>84.666700000000006</v>
+      </c>
+      <c r="CY5" s="23">
+        <f t="shared" si="0"/>
+        <v>85.25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:103">
+      <c r="CY6" s="35"/>
+    </row>
+    <row r="7" spans="1:103">
+      <c r="A7" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="33"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="CY7" s="35"/>
+    </row>
+    <row r="8" spans="1:103">
+      <c r="A8" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="31">
+        <v>1</v>
+      </c>
+      <c r="C8" s="31">
+        <v>2</v>
+      </c>
+      <c r="D8" s="31">
+        <v>3</v>
+      </c>
+      <c r="E8" s="31">
+        <v>4</v>
+      </c>
+      <c r="F8" s="31">
+        <v>5</v>
+      </c>
+      <c r="G8" s="31">
+        <v>6</v>
+      </c>
+      <c r="H8" s="31">
+        <v>7</v>
+      </c>
+      <c r="I8" s="31">
+        <v>8</v>
+      </c>
+      <c r="J8" s="31">
+        <v>9</v>
+      </c>
+      <c r="K8" s="31">
+        <v>10</v>
+      </c>
+      <c r="L8" s="31">
+        <v>11</v>
+      </c>
+      <c r="M8" s="31">
+        <v>12</v>
+      </c>
+      <c r="N8" s="31">
+        <v>13</v>
+      </c>
+      <c r="O8" s="31">
+        <v>14</v>
+      </c>
+      <c r="P8" s="31">
+        <v>15</v>
+      </c>
+      <c r="Q8" s="31">
+        <v>16</v>
+      </c>
+      <c r="R8" s="31">
+        <v>17</v>
+      </c>
+      <c r="S8" s="31">
+        <v>18</v>
+      </c>
+      <c r="T8" s="31">
+        <v>19</v>
+      </c>
+      <c r="U8" s="31">
+        <v>20</v>
+      </c>
+      <c r="V8" s="31">
+        <v>21</v>
+      </c>
+      <c r="W8" s="31">
+        <v>22</v>
+      </c>
+      <c r="X8" s="31">
+        <v>23</v>
+      </c>
+      <c r="Y8" s="31">
+        <v>24</v>
+      </c>
+      <c r="Z8" s="31">
+        <v>25</v>
+      </c>
+      <c r="AA8" s="31">
+        <v>26</v>
+      </c>
+      <c r="AB8" s="31">
+        <v>27</v>
+      </c>
+      <c r="AC8" s="31">
+        <v>28</v>
+      </c>
+      <c r="AD8" s="31">
+        <v>29</v>
+      </c>
+      <c r="AE8" s="31">
+        <v>30</v>
+      </c>
+      <c r="AF8" s="31">
+        <v>31</v>
+      </c>
+      <c r="AG8" s="31">
+        <v>32</v>
+      </c>
+      <c r="AH8" s="31">
+        <v>33</v>
+      </c>
+      <c r="AI8" s="31">
+        <v>34</v>
+      </c>
+      <c r="AJ8" s="31">
+        <v>35</v>
+      </c>
+      <c r="AK8" s="31">
+        <v>36</v>
+      </c>
+      <c r="AL8" s="31">
+        <v>37</v>
+      </c>
+      <c r="AM8" s="31">
+        <v>38</v>
+      </c>
+      <c r="AN8" s="31">
+        <v>39</v>
+      </c>
+      <c r="AO8" s="31">
+        <v>40</v>
+      </c>
+      <c r="AP8" s="31">
+        <v>41</v>
+      </c>
+      <c r="AQ8" s="31">
+        <v>42</v>
+      </c>
+      <c r="AR8" s="31">
+        <v>43</v>
+      </c>
+      <c r="AS8" s="31">
+        <v>44</v>
+      </c>
+      <c r="AT8" s="31">
+        <v>45</v>
+      </c>
+      <c r="AU8" s="31">
+        <v>46</v>
+      </c>
+      <c r="AV8" s="31">
+        <v>47</v>
+      </c>
+      <c r="AW8" s="31">
+        <v>48</v>
+      </c>
+      <c r="AX8" s="31">
+        <v>49</v>
+      </c>
+      <c r="AY8" s="31">
+        <v>50</v>
+      </c>
+      <c r="AZ8" s="31">
+        <v>51</v>
+      </c>
+      <c r="BA8" s="31">
+        <v>52</v>
+      </c>
+      <c r="BB8" s="31">
+        <v>53</v>
+      </c>
+      <c r="BC8" s="31">
+        <v>54</v>
+      </c>
+      <c r="BD8" s="31">
+        <v>55</v>
+      </c>
+      <c r="BE8" s="31">
+        <v>56</v>
+      </c>
+      <c r="BF8" s="31">
+        <v>57</v>
+      </c>
+      <c r="BG8" s="31">
+        <v>58</v>
+      </c>
+      <c r="BH8" s="31">
+        <v>59</v>
+      </c>
+      <c r="BI8" s="31">
+        <v>60</v>
+      </c>
+      <c r="BJ8" s="31">
+        <v>61</v>
+      </c>
+      <c r="BK8" s="31">
+        <v>62</v>
+      </c>
+      <c r="BL8" s="31">
+        <v>63</v>
+      </c>
+      <c r="BM8" s="31">
+        <v>64</v>
+      </c>
+      <c r="BN8" s="31">
+        <v>65</v>
+      </c>
+      <c r="BO8" s="31">
+        <v>66</v>
+      </c>
+      <c r="BP8" s="31">
+        <v>67</v>
+      </c>
+      <c r="BQ8" s="31">
+        <v>68</v>
+      </c>
+      <c r="BR8" s="31">
+        <v>69</v>
+      </c>
+      <c r="BS8" s="31">
+        <v>70</v>
+      </c>
+      <c r="BT8" s="31">
+        <v>71</v>
+      </c>
+      <c r="BU8" s="31">
+        <v>72</v>
+      </c>
+      <c r="BV8" s="31">
+        <v>73</v>
+      </c>
+      <c r="BW8" s="31">
+        <v>74</v>
+      </c>
+      <c r="BX8" s="31">
+        <v>75</v>
+      </c>
+      <c r="BY8" s="31">
+        <v>76</v>
+      </c>
+      <c r="BZ8" s="31">
+        <v>77</v>
+      </c>
+      <c r="CA8" s="31">
+        <v>78</v>
+      </c>
+      <c r="CB8" s="31">
+        <v>79</v>
+      </c>
+      <c r="CC8" s="31">
+        <v>80</v>
+      </c>
+      <c r="CD8" s="31">
+        <v>81</v>
+      </c>
+      <c r="CE8" s="31">
+        <v>82</v>
+      </c>
+      <c r="CF8" s="31">
+        <v>83</v>
+      </c>
+      <c r="CG8" s="31">
+        <v>84</v>
+      </c>
+      <c r="CH8" s="31">
+        <v>85</v>
+      </c>
+      <c r="CI8" s="31">
+        <v>86</v>
+      </c>
+      <c r="CJ8" s="31">
+        <v>87</v>
+      </c>
+      <c r="CK8" s="31">
+        <v>88</v>
+      </c>
+      <c r="CL8" s="31">
+        <v>89</v>
+      </c>
+      <c r="CM8" s="31">
+        <v>90</v>
+      </c>
+      <c r="CN8" s="31">
+        <v>91</v>
+      </c>
+      <c r="CO8" s="31">
+        <v>92</v>
+      </c>
+      <c r="CP8" s="31">
+        <v>93</v>
+      </c>
+      <c r="CQ8" s="31">
+        <v>94</v>
+      </c>
+      <c r="CR8" s="31">
+        <v>95</v>
+      </c>
+      <c r="CS8" s="31">
+        <v>96</v>
+      </c>
+      <c r="CT8" s="31">
+        <v>97</v>
+      </c>
+      <c r="CU8" s="31">
+        <v>98</v>
+      </c>
+      <c r="CV8" s="31">
+        <v>99</v>
+      </c>
+      <c r="CW8" s="31">
+        <v>100</v>
+      </c>
+      <c r="CX8" s="31">
+        <v>101</v>
+      </c>
+      <c r="CY8" s="34" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:103">
+      <c r="A9" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="23">
+        <v>56.083300000000001</v>
+      </c>
+      <c r="C9" s="23">
+        <v>55.666699999999999</v>
+      </c>
+      <c r="D9" s="23">
+        <v>56.583300000000001</v>
+      </c>
+      <c r="E9" s="23">
+        <v>55.416699999999999</v>
+      </c>
+      <c r="F9" s="23">
+        <v>56</v>
+      </c>
+      <c r="G9" s="23">
+        <v>55.333300000000001</v>
+      </c>
+      <c r="H9" s="23">
+        <v>52.75</v>
+      </c>
+      <c r="I9" s="23">
+        <v>53.75</v>
+      </c>
+      <c r="J9" s="23">
+        <v>54.666699999999999</v>
+      </c>
+      <c r="K9" s="23">
+        <v>52.75</v>
+      </c>
+      <c r="L9" s="23">
+        <v>53.166699999999999</v>
+      </c>
+      <c r="M9" s="23">
+        <v>55.166699999999999</v>
+      </c>
+      <c r="N9" s="23">
+        <v>53.5</v>
+      </c>
+      <c r="O9" s="23">
+        <v>53.416699999999999</v>
+      </c>
+      <c r="P9" s="23">
+        <v>53.5</v>
+      </c>
+      <c r="Q9" s="23">
+        <v>53.583300000000001</v>
+      </c>
+      <c r="R9" s="23">
+        <v>55</v>
+      </c>
+      <c r="S9" s="23">
+        <v>53.666699999999999</v>
+      </c>
+      <c r="T9" s="23">
+        <v>52.083300000000001</v>
+      </c>
+      <c r="U9" s="23">
+        <v>52.5</v>
+      </c>
+      <c r="V9" s="23">
+        <v>51.333300000000001</v>
+      </c>
+      <c r="W9" s="23">
+        <v>51.583300000000001</v>
+      </c>
+      <c r="X9" s="23">
+        <v>50.333300000000001</v>
+      </c>
+      <c r="Y9" s="23">
+        <v>51</v>
+      </c>
+      <c r="Z9" s="23">
+        <v>51</v>
+      </c>
+      <c r="AA9" s="23">
+        <v>51.833300000000001</v>
+      </c>
+      <c r="AB9" s="23">
+        <v>50.333300000000001</v>
+      </c>
+      <c r="AC9" s="23">
+        <v>51.833300000000001</v>
+      </c>
+      <c r="AD9" s="23">
+        <v>51.583300000000001</v>
+      </c>
+      <c r="AE9" s="23">
+        <v>52.666699999999999</v>
+      </c>
+      <c r="AF9" s="23">
+        <v>52.166699999999999</v>
+      </c>
+      <c r="AG9" s="23">
+        <v>52.666699999999999</v>
+      </c>
+      <c r="AH9" s="23">
+        <v>53.416699999999999</v>
+      </c>
+      <c r="AI9" s="23">
+        <v>52.416699999999999</v>
+      </c>
+      <c r="AJ9" s="23">
+        <v>52.666699999999999</v>
+      </c>
+      <c r="AK9" s="23">
+        <v>53.083300000000001</v>
+      </c>
+      <c r="AL9" s="23">
+        <v>52.916699999999999</v>
+      </c>
+      <c r="AM9" s="23">
+        <v>52.666699999999999</v>
+      </c>
+      <c r="AN9" s="23">
+        <v>52.166699999999999</v>
+      </c>
+      <c r="AO9" s="23">
+        <v>51.75</v>
+      </c>
+      <c r="AP9" s="23">
+        <v>51.916699999999999</v>
+      </c>
+      <c r="AQ9" s="23">
+        <v>51.583300000000001</v>
+      </c>
+      <c r="AR9" s="23">
+        <v>51.416699999999999</v>
+      </c>
+      <c r="AS9" s="23">
+        <v>50.916699999999999</v>
+      </c>
+      <c r="AT9" s="23">
+        <v>52.083300000000001</v>
+      </c>
+      <c r="AU9" s="23">
+        <v>51.583300000000001</v>
+      </c>
+      <c r="AV9" s="23">
+        <v>52.916699999999999</v>
+      </c>
+      <c r="AW9" s="23">
+        <v>52.416699999999999</v>
+      </c>
+      <c r="AX9" s="23">
+        <v>52.916699999999999</v>
+      </c>
+      <c r="AY9" s="23">
+        <v>52.166699999999999</v>
+      </c>
+      <c r="AZ9" s="23">
+        <v>53.083300000000001</v>
+      </c>
+      <c r="BA9" s="23">
+        <v>53.5</v>
+      </c>
+      <c r="BB9" s="23">
+        <v>52.833300000000001</v>
+      </c>
+      <c r="BC9" s="23">
+        <v>53</v>
+      </c>
+      <c r="BD9" s="23">
+        <v>53.666699999999999</v>
+      </c>
+      <c r="BE9" s="23">
+        <v>53.75</v>
+      </c>
+      <c r="BF9" s="23">
+        <v>53.166699999999999</v>
+      </c>
+      <c r="BG9" s="23">
+        <v>52.416699999999999</v>
+      </c>
+      <c r="BH9" s="23">
+        <v>52.083300000000001</v>
+      </c>
+      <c r="BI9" s="23">
+        <v>52.833300000000001</v>
+      </c>
+      <c r="BJ9" s="23">
+        <v>53.833300000000001</v>
+      </c>
+      <c r="BK9" s="23">
+        <v>52.583300000000001</v>
+      </c>
+      <c r="BL9" s="23">
+        <v>53.083300000000001</v>
+      </c>
+      <c r="BM9" s="23">
+        <v>52.666699999999999</v>
+      </c>
+      <c r="BN9" s="23">
+        <v>52.416699999999999</v>
+      </c>
+      <c r="BO9" s="23">
+        <v>52.083300000000001</v>
+      </c>
+      <c r="BP9" s="23">
+        <v>52.583300000000001</v>
+      </c>
+      <c r="BQ9" s="23">
+        <v>52.916699999999999</v>
+      </c>
+      <c r="BR9" s="23">
+        <v>51.583300000000001</v>
+      </c>
+      <c r="BS9" s="23">
+        <v>51.583300000000001</v>
+      </c>
+      <c r="BT9" s="23">
+        <v>51.916699999999999</v>
+      </c>
+      <c r="BU9" s="23">
+        <v>52.583300000000001</v>
+      </c>
+      <c r="BV9" s="23">
+        <v>51.833300000000001</v>
+      </c>
+      <c r="BW9" s="23">
+        <v>52</v>
+      </c>
+      <c r="BX9" s="23">
+        <v>52.25</v>
+      </c>
+      <c r="BY9" s="23">
+        <v>51.833300000000001</v>
+      </c>
+      <c r="BZ9" s="23">
+        <v>51.666699999999999</v>
+      </c>
+      <c r="CA9" s="23">
+        <v>51.583300000000001</v>
+      </c>
+      <c r="CB9" s="23">
+        <v>52.25</v>
+      </c>
+      <c r="CC9" s="23">
+        <v>51.916699999999999</v>
+      </c>
+      <c r="CD9" s="23">
+        <v>52.166699999999999</v>
+      </c>
+      <c r="CE9" s="23">
+        <v>51.916699999999999</v>
+      </c>
+      <c r="CF9" s="23">
+        <v>52</v>
+      </c>
+      <c r="CG9" s="23">
+        <v>52.333300000000001</v>
+      </c>
+      <c r="CH9" s="23">
+        <v>52.416699999999999</v>
+      </c>
+      <c r="CI9" s="23">
+        <v>52.25</v>
+      </c>
+      <c r="CJ9" s="23">
+        <v>52.583300000000001</v>
+      </c>
+      <c r="CK9" s="23">
+        <v>52.583300000000001</v>
+      </c>
+      <c r="CL9" s="23">
+        <v>52.083300000000001</v>
+      </c>
+      <c r="CM9" s="23">
+        <v>51.75</v>
+      </c>
+      <c r="CN9" s="23">
+        <v>51.666699999999999</v>
+      </c>
+      <c r="CO9" s="23">
+        <v>51.916699999999999</v>
+      </c>
+      <c r="CP9" s="23">
+        <v>52.333300000000001</v>
+      </c>
+      <c r="CQ9" s="23">
+        <v>52.166699999999999</v>
+      </c>
+      <c r="CR9" s="23">
+        <v>52.583300000000001</v>
+      </c>
+      <c r="CS9" s="23">
+        <v>52.166699999999999</v>
+      </c>
+      <c r="CT9" s="23">
+        <v>52.083300000000001</v>
+      </c>
+      <c r="CU9" s="23">
+        <v>52</v>
+      </c>
+      <c r="CV9" s="23">
+        <v>52</v>
+      </c>
+      <c r="CW9" s="23">
+        <v>52.166699999999999</v>
+      </c>
+      <c r="CX9" s="23">
+        <v>52.083300000000001</v>
+      </c>
+      <c r="CY9" s="23">
+        <f t="shared" si="0"/>
+        <v>56.583300000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:103">
+      <c r="A10" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="23">
+        <v>76.583299999999994</v>
+      </c>
+      <c r="C10" s="23">
+        <v>78.5</v>
+      </c>
+      <c r="D10" s="23">
+        <v>81.25</v>
+      </c>
+      <c r="E10" s="23">
+        <v>82.833299999999994</v>
+      </c>
+      <c r="F10" s="23">
+        <v>82.75</v>
+      </c>
+      <c r="G10" s="23">
+        <v>83.75</v>
+      </c>
+      <c r="H10" s="23">
+        <v>82.916700000000006</v>
+      </c>
+      <c r="I10" s="23">
+        <v>82.75</v>
+      </c>
+      <c r="J10" s="23">
+        <v>82.583299999999994</v>
+      </c>
+      <c r="K10" s="23">
+        <v>82.666700000000006</v>
+      </c>
+      <c r="L10" s="23">
+        <v>83.166700000000006</v>
+      </c>
+      <c r="M10" s="23">
+        <v>82.833299999999994</v>
+      </c>
+      <c r="N10" s="23">
+        <v>82.25</v>
+      </c>
+      <c r="O10" s="23">
+        <v>81.583299999999994</v>
+      </c>
+      <c r="P10" s="23">
+        <v>82.583299999999994</v>
+      </c>
+      <c r="Q10" s="23">
+        <v>82.75</v>
+      </c>
+      <c r="R10" s="23">
+        <v>82.666700000000006</v>
+      </c>
+      <c r="S10" s="23">
+        <v>83.583299999999994</v>
+      </c>
+      <c r="T10" s="23">
+        <v>83.75</v>
+      </c>
+      <c r="U10" s="23">
+        <v>83.75</v>
+      </c>
+      <c r="V10" s="23">
+        <v>83.083299999999994</v>
+      </c>
+      <c r="W10" s="23">
+        <v>83.5</v>
+      </c>
+      <c r="X10" s="23">
+        <v>82.5</v>
+      </c>
+      <c r="Y10" s="23">
+        <v>83.083299999999994</v>
+      </c>
+      <c r="Z10" s="23">
+        <v>82.25</v>
+      </c>
+      <c r="AA10" s="23">
+        <v>82</v>
+      </c>
+      <c r="AB10" s="23">
+        <v>82.75</v>
+      </c>
+      <c r="AC10" s="23">
+        <v>82.25</v>
+      </c>
+      <c r="AD10" s="23">
+        <v>82.583299999999994</v>
+      </c>
+      <c r="AE10" s="23">
+        <v>83</v>
+      </c>
+      <c r="AF10" s="23">
+        <v>82.333299999999994</v>
+      </c>
+      <c r="AG10" s="23">
+        <v>82.333299999999994</v>
+      </c>
+      <c r="AH10" s="23">
+        <v>82.666700000000006</v>
+      </c>
+      <c r="AI10" s="23">
+        <v>82.916700000000006</v>
+      </c>
+      <c r="AJ10" s="23">
+        <v>82.666700000000006</v>
+      </c>
+      <c r="AK10" s="23">
+        <v>82.916700000000006</v>
+      </c>
+      <c r="AL10" s="23">
+        <v>82.666700000000006</v>
+      </c>
+      <c r="AM10" s="23">
+        <v>83</v>
+      </c>
+      <c r="AN10" s="23">
+        <v>82.75</v>
+      </c>
+      <c r="AO10" s="23">
+        <v>82.5</v>
+      </c>
+      <c r="AP10" s="23">
+        <v>82.416700000000006</v>
+      </c>
+      <c r="AQ10" s="23">
+        <v>83</v>
+      </c>
+      <c r="AR10" s="23">
+        <v>82.666700000000006</v>
+      </c>
+      <c r="AS10" s="23">
+        <v>82.666700000000006</v>
+      </c>
+      <c r="AT10" s="23">
+        <v>82.916700000000006</v>
+      </c>
+      <c r="AU10" s="23">
+        <v>83.166700000000006</v>
+      </c>
+      <c r="AV10" s="23">
+        <v>82.416700000000006</v>
+      </c>
+      <c r="AW10" s="23">
+        <v>82.416700000000006</v>
+      </c>
+      <c r="AX10" s="23">
+        <v>82.25</v>
+      </c>
+      <c r="AY10" s="23">
+        <v>82.166700000000006</v>
+      </c>
+      <c r="AZ10" s="23">
+        <v>82.333299999999994</v>
+      </c>
+      <c r="BA10" s="23">
+        <v>82.583299999999994</v>
+      </c>
+      <c r="BB10" s="23">
+        <v>83.083299999999994</v>
+      </c>
+      <c r="BC10" s="23">
+        <v>83.416700000000006</v>
+      </c>
+      <c r="BD10" s="23">
+        <v>83.5</v>
+      </c>
+      <c r="BE10" s="23">
+        <v>83</v>
+      </c>
+      <c r="BF10" s="23">
+        <v>82.833299999999994</v>
+      </c>
+      <c r="BG10" s="23">
+        <v>83</v>
+      </c>
+      <c r="BH10" s="23">
+        <v>82.75</v>
+      </c>
+      <c r="BI10" s="23">
+        <v>82.75</v>
+      </c>
+      <c r="BJ10" s="23">
+        <v>82.666700000000006</v>
+      </c>
+      <c r="BK10" s="23">
+        <v>82.416700000000006</v>
+      </c>
+      <c r="BL10" s="23">
+        <v>82.5</v>
+      </c>
+      <c r="BM10" s="23">
+        <v>82.666700000000006</v>
+      </c>
+      <c r="BN10" s="23">
+        <v>82.666700000000006</v>
+      </c>
+      <c r="BO10" s="23">
+        <v>82.583299999999994</v>
+      </c>
+      <c r="BP10" s="23">
+        <v>82.583299999999994</v>
+      </c>
+      <c r="BQ10" s="23">
+        <v>82.833299999999994</v>
+      </c>
+      <c r="BR10" s="23">
+        <v>83</v>
+      </c>
+      <c r="BS10" s="23">
+        <v>82.75</v>
+      </c>
+      <c r="BT10" s="23">
+        <v>83.333299999999994</v>
+      </c>
+      <c r="BU10" s="23">
+        <v>83.083299999999994</v>
+      </c>
+      <c r="BV10" s="23">
+        <v>82.833299999999994</v>
+      </c>
+      <c r="BW10" s="23">
+        <v>82.833299999999994</v>
+      </c>
+      <c r="BX10" s="23">
+        <v>83.166700000000006</v>
+      </c>
+      <c r="BY10" s="23">
+        <v>83.333299999999994</v>
+      </c>
+      <c r="BZ10" s="23">
+        <v>83.5</v>
+      </c>
+      <c r="CA10" s="23">
+        <v>83.25</v>
+      </c>
+      <c r="CB10" s="23">
+        <v>83.333299999999994</v>
+      </c>
+      <c r="CC10" s="23">
+        <v>83.083299999999994</v>
+      </c>
+      <c r="CD10" s="23">
+        <v>83.083299999999994</v>
+      </c>
+      <c r="CE10" s="23">
+        <v>83.166700000000006</v>
+      </c>
+      <c r="CF10" s="23">
+        <v>82.833299999999994</v>
+      </c>
+      <c r="CG10" s="23">
+        <v>82.666700000000006</v>
+      </c>
+      <c r="CH10" s="23">
+        <v>82.916700000000006</v>
+      </c>
+      <c r="CI10" s="23">
+        <v>82.5</v>
+      </c>
+      <c r="CJ10" s="23">
+        <v>82.583299999999994</v>
+      </c>
+      <c r="CK10" s="23">
+        <v>82.666700000000006</v>
+      </c>
+      <c r="CL10" s="23">
+        <v>82.666700000000006</v>
+      </c>
+      <c r="CM10" s="23">
+        <v>82.666700000000006</v>
+      </c>
+      <c r="CN10" s="23">
+        <v>82.916700000000006</v>
+      </c>
+      <c r="CO10" s="23">
+        <v>82.916700000000006</v>
+      </c>
+      <c r="CP10" s="23">
+        <v>82.666700000000006</v>
+      </c>
+      <c r="CQ10" s="23">
+        <v>82.333299999999994</v>
+      </c>
+      <c r="CR10" s="23">
+        <v>82.416700000000006</v>
+      </c>
+      <c r="CS10" s="23">
+        <v>81.833299999999994</v>
+      </c>
+      <c r="CT10" s="23">
+        <v>82.166700000000006</v>
+      </c>
+      <c r="CU10" s="23">
+        <v>81.833299999999994</v>
+      </c>
+      <c r="CV10" s="23">
+        <v>81.916700000000006</v>
+      </c>
+      <c r="CW10" s="23">
+        <v>81.916700000000006</v>
+      </c>
+      <c r="CX10" s="23">
+        <v>82</v>
+      </c>
+      <c r="CY10" s="23">
+        <f t="shared" si="0"/>
+        <v>83.75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:103">
+      <c r="A11" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="23">
+        <v>68.5</v>
+      </c>
+      <c r="C11" s="23">
+        <v>72.5</v>
+      </c>
+      <c r="D11" s="23">
+        <v>82.416700000000006</v>
+      </c>
+      <c r="E11" s="23">
+        <v>84.916700000000006</v>
+      </c>
+      <c r="F11" s="23">
+        <v>84.25</v>
+      </c>
+      <c r="G11" s="23">
+        <v>84.166700000000006</v>
+      </c>
+      <c r="H11" s="23">
+        <v>84.5</v>
+      </c>
+      <c r="I11" s="23">
+        <v>84.75</v>
+      </c>
+      <c r="J11" s="23">
+        <v>85.166700000000006</v>
+      </c>
+      <c r="K11" s="23">
+        <v>85.416700000000006</v>
+      </c>
+      <c r="L11" s="23">
+        <v>85.166700000000006</v>
+      </c>
+      <c r="M11" s="23">
+        <v>85.5</v>
+      </c>
+      <c r="N11" s="23">
+        <v>85.25</v>
+      </c>
+      <c r="O11" s="23">
+        <v>85.083299999999994</v>
+      </c>
+      <c r="P11" s="23">
+        <v>85.583299999999994</v>
+      </c>
+      <c r="Q11" s="23">
+        <v>85</v>
+      </c>
+      <c r="R11" s="23">
+        <v>85</v>
+      </c>
+      <c r="S11" s="23">
+        <v>85.333299999999994</v>
+      </c>
+      <c r="T11" s="23">
+        <v>84.666700000000006</v>
+      </c>
+      <c r="U11" s="23">
+        <v>84.583299999999994</v>
+      </c>
+      <c r="V11" s="23">
+        <v>84.416700000000006</v>
+      </c>
+      <c r="W11" s="23">
+        <v>84.666700000000006</v>
+      </c>
+      <c r="X11" s="23">
+        <v>84.75</v>
+      </c>
+      <c r="Y11" s="23">
+        <v>84.416700000000006</v>
+      </c>
+      <c r="Z11" s="23">
+        <v>84.416700000000006</v>
+      </c>
+      <c r="AA11" s="23">
+        <v>84.583299999999994</v>
+      </c>
+      <c r="AB11" s="23">
+        <v>84.416700000000006</v>
+      </c>
+      <c r="AC11" s="23">
+        <v>84.75</v>
+      </c>
+      <c r="AD11" s="23">
+        <v>85.083299999999994</v>
+      </c>
+      <c r="AE11" s="23">
+        <v>84.666700000000006</v>
+      </c>
+      <c r="AF11" s="23">
+        <v>84.666700000000006</v>
+      </c>
+      <c r="AG11" s="23">
+        <v>85.083299999999994</v>
+      </c>
+      <c r="AH11" s="23">
+        <v>85.333299999999994</v>
+      </c>
+      <c r="AI11" s="23">
+        <v>85.166700000000006</v>
+      </c>
+      <c r="AJ11" s="23">
+        <v>85.5</v>
+      </c>
+      <c r="AK11" s="23">
+        <v>85</v>
+      </c>
+      <c r="AL11" s="23">
+        <v>85.25</v>
+      </c>
+      <c r="AM11" s="23">
+        <v>85.666700000000006</v>
+      </c>
+      <c r="AN11" s="23">
+        <v>85.333299999999994</v>
+      </c>
+      <c r="AO11" s="23">
+        <v>85.5</v>
+      </c>
+      <c r="AP11" s="23">
+        <v>85.416700000000006</v>
+      </c>
+      <c r="AQ11" s="23">
+        <v>85.416700000000006</v>
+      </c>
+      <c r="AR11" s="23">
+        <v>85.333299999999994</v>
+      </c>
+      <c r="AS11" s="23">
+        <v>85.75</v>
+      </c>
+      <c r="AT11" s="23">
+        <v>85.666700000000006</v>
+      </c>
+      <c r="AU11" s="23">
+        <v>85.25</v>
+      </c>
+      <c r="AV11" s="23">
+        <v>85.333299999999994</v>
+      </c>
+      <c r="AW11" s="23">
+        <v>85.666700000000006</v>
+      </c>
+      <c r="AX11" s="23">
+        <v>85.166700000000006</v>
+      </c>
+      <c r="AY11" s="23">
+        <v>85</v>
+      </c>
+      <c r="AZ11" s="23">
+        <v>85.5</v>
+      </c>
+      <c r="BA11" s="23">
+        <v>84.75</v>
+      </c>
+      <c r="BB11" s="23">
+        <v>84.583299999999994</v>
+      </c>
+      <c r="BC11" s="23">
+        <v>84.666700000000006</v>
+      </c>
+      <c r="BD11" s="23">
+        <v>84.75</v>
+      </c>
+      <c r="BE11" s="23">
+        <v>84.916700000000006</v>
+      </c>
+      <c r="BF11" s="23">
+        <v>84.416700000000006</v>
+      </c>
+      <c r="BG11" s="23">
+        <v>84.333299999999994</v>
+      </c>
+      <c r="BH11" s="23">
+        <v>84.583299999999994</v>
+      </c>
+      <c r="BI11" s="23">
+        <v>84.583299999999994</v>
+      </c>
+      <c r="BJ11" s="23">
+        <v>84.416700000000006</v>
+      </c>
+      <c r="BK11" s="23">
+        <v>84.5</v>
+      </c>
+      <c r="BL11" s="23">
+        <v>84.416700000000006</v>
+      </c>
+      <c r="BM11" s="23">
+        <v>84.166700000000006</v>
+      </c>
+      <c r="BN11" s="23">
+        <v>84.416700000000006</v>
+      </c>
+      <c r="BO11" s="23">
+        <v>84.333299999999994</v>
+      </c>
+      <c r="BP11" s="23">
+        <v>84.5</v>
+      </c>
+      <c r="BQ11" s="23">
+        <v>84.25</v>
+      </c>
+      <c r="BR11" s="23">
+        <v>84.25</v>
+      </c>
+      <c r="BS11" s="23">
+        <v>84.5</v>
+      </c>
+      <c r="BT11" s="23">
+        <v>84.583299999999994</v>
+      </c>
+      <c r="BU11" s="23">
+        <v>84.583299999999994</v>
+      </c>
+      <c r="BV11" s="23">
+        <v>84.5</v>
+      </c>
+      <c r="BW11" s="23">
+        <v>85</v>
+      </c>
+      <c r="BX11" s="23">
+        <v>85.166700000000006</v>
+      </c>
+      <c r="BY11" s="23">
+        <v>85.25</v>
+      </c>
+      <c r="BZ11" s="23">
+        <v>85.083299999999994</v>
+      </c>
+      <c r="CA11" s="23">
+        <v>85.333299999999994</v>
+      </c>
+      <c r="CB11" s="23">
+        <v>85.083299999999994</v>
+      </c>
+      <c r="CC11" s="23">
+        <v>85</v>
+      </c>
+      <c r="CD11" s="23">
+        <v>85.25</v>
+      </c>
+      <c r="CE11" s="23">
+        <v>85</v>
+      </c>
+      <c r="CF11" s="23">
+        <v>85.166700000000006</v>
+      </c>
+      <c r="CG11" s="23">
+        <v>84.333299999999994</v>
+      </c>
+      <c r="CH11" s="23">
+        <v>84.5</v>
+      </c>
+      <c r="CI11" s="23">
+        <v>84.5</v>
+      </c>
+      <c r="CJ11" s="23">
+        <v>84.666700000000006</v>
+      </c>
+      <c r="CK11" s="23">
+        <v>84.916700000000006</v>
+      </c>
+      <c r="CL11" s="23">
+        <v>84.833299999999994</v>
+      </c>
+      <c r="CM11" s="23">
+        <v>84.916700000000006</v>
+      </c>
+      <c r="CN11" s="23">
+        <v>85</v>
+      </c>
+      <c r="CO11" s="23">
+        <v>85.083299999999994</v>
+      </c>
+      <c r="CP11" s="23">
+        <v>85.083299999999994</v>
+      </c>
+      <c r="CQ11" s="23">
+        <v>85.166700000000006</v>
+      </c>
+      <c r="CR11" s="23">
+        <v>85</v>
+      </c>
+      <c r="CS11" s="23">
+        <v>84.833299999999994</v>
+      </c>
+      <c r="CT11" s="23">
+        <v>84.833299999999994</v>
+      </c>
+      <c r="CU11" s="23">
+        <v>84.833299999999994</v>
+      </c>
+      <c r="CV11" s="23">
+        <v>84.833299999999994</v>
+      </c>
+      <c r="CW11" s="23">
+        <v>84.916700000000006</v>
+      </c>
+      <c r="CX11" s="23">
+        <v>85.083299999999994</v>
+      </c>
+      <c r="CY11" s="23">
+        <f t="shared" si="0"/>
+        <v>85.75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:103">
+      <c r="CY12" s="35"/>
+    </row>
+    <row r="13" spans="1:103">
+      <c r="A13" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="33"/>
+      <c r="C13" s="33"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="33"/>
+      <c r="CY13" s="35"/>
+    </row>
+    <row r="14" spans="1:103">
+      <c r="A14" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="31">
+        <v>1</v>
+      </c>
+      <c r="C14" s="31">
+        <v>2</v>
+      </c>
+      <c r="D14" s="31">
+        <v>3</v>
+      </c>
+      <c r="E14" s="31">
+        <v>4</v>
+      </c>
+      <c r="F14" s="31">
+        <v>5</v>
+      </c>
+      <c r="G14" s="31">
+        <v>6</v>
+      </c>
+      <c r="H14" s="31">
+        <v>7</v>
+      </c>
+      <c r="I14" s="31">
+        <v>8</v>
+      </c>
+      <c r="J14" s="31">
+        <v>9</v>
+      </c>
+      <c r="K14" s="31">
+        <v>10</v>
+      </c>
+      <c r="L14" s="31">
+        <v>11</v>
+      </c>
+      <c r="M14" s="31">
+        <v>12</v>
+      </c>
+      <c r="N14" s="31">
+        <v>13</v>
+      </c>
+      <c r="O14" s="31">
+        <v>14</v>
+      </c>
+      <c r="P14" s="31">
+        <v>15</v>
+      </c>
+      <c r="Q14" s="31">
+        <v>16</v>
+      </c>
+      <c r="R14" s="31">
+        <v>17</v>
+      </c>
+      <c r="S14" s="31">
+        <v>18</v>
+      </c>
+      <c r="T14" s="31">
+        <v>19</v>
+      </c>
+      <c r="U14" s="31">
+        <v>20</v>
+      </c>
+      <c r="V14" s="31">
+        <v>21</v>
+      </c>
+      <c r="W14" s="31">
+        <v>22</v>
+      </c>
+      <c r="X14" s="31">
+        <v>23</v>
+      </c>
+      <c r="Y14" s="31">
+        <v>24</v>
+      </c>
+      <c r="Z14" s="31">
+        <v>25</v>
+      </c>
+      <c r="AA14" s="31">
+        <v>26</v>
+      </c>
+      <c r="AB14" s="31">
+        <v>27</v>
+      </c>
+      <c r="AC14" s="31">
+        <v>28</v>
+      </c>
+      <c r="AD14" s="31">
+        <v>29</v>
+      </c>
+      <c r="AE14" s="31">
+        <v>30</v>
+      </c>
+      <c r="AF14" s="31">
+        <v>31</v>
+      </c>
+      <c r="AG14" s="31">
+        <v>32</v>
+      </c>
+      <c r="AH14" s="31">
+        <v>33</v>
+      </c>
+      <c r="AI14" s="31">
+        <v>34</v>
+      </c>
+      <c r="AJ14" s="31">
+        <v>35</v>
+      </c>
+      <c r="AK14" s="31">
+        <v>36</v>
+      </c>
+      <c r="AL14" s="31">
+        <v>37</v>
+      </c>
+      <c r="AM14" s="31">
+        <v>38</v>
+      </c>
+      <c r="AN14" s="31">
+        <v>39</v>
+      </c>
+      <c r="AO14" s="31">
+        <v>40</v>
+      </c>
+      <c r="AP14" s="31">
+        <v>41</v>
+      </c>
+      <c r="AQ14" s="31">
+        <v>42</v>
+      </c>
+      <c r="AR14" s="31">
+        <v>43</v>
+      </c>
+      <c r="AS14" s="31">
+        <v>44</v>
+      </c>
+      <c r="AT14" s="31">
+        <v>45</v>
+      </c>
+      <c r="AU14" s="31">
+        <v>46</v>
+      </c>
+      <c r="AV14" s="31">
+        <v>47</v>
+      </c>
+      <c r="AW14" s="31">
+        <v>48</v>
+      </c>
+      <c r="AX14" s="31">
+        <v>49</v>
+      </c>
+      <c r="AY14" s="31">
+        <v>50</v>
+      </c>
+      <c r="AZ14" s="31">
+        <v>51</v>
+      </c>
+      <c r="BA14" s="31">
+        <v>52</v>
+      </c>
+      <c r="BB14" s="31">
+        <v>53</v>
+      </c>
+      <c r="BC14" s="31">
+        <v>54</v>
+      </c>
+      <c r="BD14" s="31">
+        <v>55</v>
+      </c>
+      <c r="BE14" s="31">
+        <v>56</v>
+      </c>
+      <c r="BF14" s="31">
+        <v>57</v>
+      </c>
+      <c r="BG14" s="31">
+        <v>58</v>
+      </c>
+      <c r="BH14" s="31">
+        <v>59</v>
+      </c>
+      <c r="BI14" s="31">
+        <v>60</v>
+      </c>
+      <c r="BJ14" s="31">
+        <v>61</v>
+      </c>
+      <c r="BK14" s="31">
+        <v>62</v>
+      </c>
+      <c r="BL14" s="31">
+        <v>63</v>
+      </c>
+      <c r="BM14" s="31">
+        <v>64</v>
+      </c>
+      <c r="BN14" s="31">
+        <v>65</v>
+      </c>
+      <c r="BO14" s="31">
+        <v>66</v>
+      </c>
+      <c r="BP14" s="31">
+        <v>67</v>
+      </c>
+      <c r="BQ14" s="31">
+        <v>68</v>
+      </c>
+      <c r="BR14" s="31">
+        <v>69</v>
+      </c>
+      <c r="BS14" s="31">
+        <v>70</v>
+      </c>
+      <c r="BT14" s="31">
+        <v>71</v>
+      </c>
+      <c r="BU14" s="31">
+        <v>72</v>
+      </c>
+      <c r="BV14" s="31">
+        <v>73</v>
+      </c>
+      <c r="BW14" s="31">
+        <v>74</v>
+      </c>
+      <c r="BX14" s="31">
+        <v>75</v>
+      </c>
+      <c r="BY14" s="31">
+        <v>76</v>
+      </c>
+      <c r="BZ14" s="31">
+        <v>77</v>
+      </c>
+      <c r="CA14" s="31">
+        <v>78</v>
+      </c>
+      <c r="CB14" s="31">
+        <v>79</v>
+      </c>
+      <c r="CC14" s="31">
+        <v>80</v>
+      </c>
+      <c r="CD14" s="31">
+        <v>81</v>
+      </c>
+      <c r="CE14" s="31">
+        <v>82</v>
+      </c>
+      <c r="CF14" s="31">
+        <v>83</v>
+      </c>
+      <c r="CG14" s="31">
+        <v>84</v>
+      </c>
+      <c r="CH14" s="31">
+        <v>85</v>
+      </c>
+      <c r="CI14" s="31">
+        <v>86</v>
+      </c>
+      <c r="CJ14" s="31">
+        <v>87</v>
+      </c>
+      <c r="CK14" s="31">
+        <v>88</v>
+      </c>
+      <c r="CL14" s="31">
+        <v>89</v>
+      </c>
+      <c r="CM14" s="31">
+        <v>90</v>
+      </c>
+      <c r="CN14" s="31">
+        <v>91</v>
+      </c>
+      <c r="CO14" s="31">
+        <v>92</v>
+      </c>
+      <c r="CP14" s="31">
+        <v>93</v>
+      </c>
+      <c r="CQ14" s="31">
+        <v>94</v>
+      </c>
+      <c r="CR14" s="31">
+        <v>95</v>
+      </c>
+      <c r="CS14" s="31">
+        <v>96</v>
+      </c>
+      <c r="CT14" s="31">
+        <v>97</v>
+      </c>
+      <c r="CU14" s="31">
+        <v>98</v>
+      </c>
+      <c r="CV14" s="31">
+        <v>99</v>
+      </c>
+      <c r="CW14" s="31">
+        <v>100</v>
+      </c>
+      <c r="CX14" s="31">
+        <v>101</v>
+      </c>
+      <c r="CY14" s="34" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:103">
+      <c r="A15" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="23">
+        <v>48</v>
+      </c>
+      <c r="C15" s="23">
+        <v>53.75</v>
+      </c>
+      <c r="D15" s="23">
+        <v>53.333300000000001</v>
+      </c>
+      <c r="E15" s="23">
+        <v>48.833300000000001</v>
+      </c>
+      <c r="F15" s="23">
+        <v>51.666699999999999</v>
+      </c>
+      <c r="G15" s="23">
+        <v>50.416699999999999</v>
+      </c>
+      <c r="H15" s="23">
+        <v>50.666699999999999</v>
+      </c>
+      <c r="I15" s="23">
+        <v>50.083300000000001</v>
+      </c>
+      <c r="J15" s="23">
+        <v>51.166699999999999</v>
+      </c>
+      <c r="K15" s="23">
+        <v>47.916699999999999</v>
+      </c>
+      <c r="L15" s="23">
+        <v>50.583300000000001</v>
+      </c>
+      <c r="M15" s="23">
+        <v>49.416699999999999</v>
+      </c>
+      <c r="N15" s="23">
+        <v>49.75</v>
+      </c>
+      <c r="O15" s="23">
+        <v>48.833300000000001</v>
+      </c>
+      <c r="P15" s="23">
+        <v>51.166699999999999</v>
+      </c>
+      <c r="Q15" s="23">
+        <v>49</v>
+      </c>
+      <c r="R15" s="23">
+        <v>49.666699999999999</v>
+      </c>
+      <c r="S15" s="23">
+        <v>49.666699999999999</v>
+      </c>
+      <c r="T15" s="23">
+        <v>50.416699999999999</v>
+      </c>
+      <c r="U15" s="23">
+        <v>50</v>
+      </c>
+      <c r="V15" s="23">
+        <v>49.416699999999999</v>
+      </c>
+      <c r="W15" s="23">
+        <v>49.916699999999999</v>
+      </c>
+      <c r="X15" s="23">
+        <v>50.083300000000001</v>
+      </c>
+      <c r="Y15" s="23">
+        <v>50</v>
+      </c>
+      <c r="Z15" s="23">
+        <v>51.166699999999999</v>
+      </c>
+      <c r="AA15" s="23">
+        <v>51.666699999999999</v>
+      </c>
+      <c r="AB15" s="23">
+        <v>50.333300000000001</v>
+      </c>
+      <c r="AC15" s="23">
+        <v>51.25</v>
+      </c>
+      <c r="AD15" s="23">
+        <v>50.083300000000001</v>
+      </c>
+      <c r="AE15" s="23">
+        <v>50.166699999999999</v>
+      </c>
+      <c r="AF15" s="23">
+        <v>50.166699999999999</v>
+      </c>
+      <c r="AG15" s="23">
+        <v>49.833300000000001</v>
+      </c>
+      <c r="AH15" s="23">
+        <v>50</v>
+      </c>
+      <c r="AI15" s="23">
+        <v>50</v>
+      </c>
+      <c r="AJ15" s="23">
+        <v>50.416699999999999</v>
+      </c>
+      <c r="AK15" s="23">
+        <v>49.666699999999999</v>
+      </c>
+      <c r="AL15" s="23">
+        <v>50.25</v>
+      </c>
+      <c r="AM15" s="23">
+        <v>49.666699999999999</v>
+      </c>
+      <c r="AN15" s="23">
+        <v>50.083300000000001</v>
+      </c>
+      <c r="AO15" s="23">
+        <v>51</v>
+      </c>
+      <c r="AP15" s="23">
+        <v>51.25</v>
+      </c>
+      <c r="AQ15" s="23">
+        <v>50</v>
+      </c>
+      <c r="AR15" s="23">
+        <v>51.166699999999999</v>
+      </c>
+      <c r="AS15" s="23">
+        <v>51</v>
+      </c>
+      <c r="AT15" s="23">
+        <v>49.75</v>
+      </c>
+      <c r="AU15" s="23">
+        <v>50.25</v>
+      </c>
+      <c r="AV15" s="23">
+        <v>49.5</v>
+      </c>
+      <c r="AW15" s="23">
+        <v>49.5</v>
+      </c>
+      <c r="AX15" s="23">
+        <v>50</v>
+      </c>
+      <c r="AY15" s="23">
+        <v>50.25</v>
+      </c>
+      <c r="AZ15" s="23">
+        <v>50.166699999999999</v>
+      </c>
+      <c r="BA15" s="23">
+        <v>51</v>
+      </c>
+      <c r="BB15" s="23">
+        <v>49.666699999999999</v>
+      </c>
+      <c r="BC15" s="23">
+        <v>49.833300000000001</v>
+      </c>
+      <c r="BD15" s="23">
+        <v>49.833300000000001</v>
+      </c>
+      <c r="BE15" s="23">
+        <v>49.5</v>
+      </c>
+      <c r="BF15" s="23">
+        <v>51.416699999999999</v>
+      </c>
+      <c r="BG15" s="23">
+        <v>50.75</v>
+      </c>
+      <c r="BH15" s="23">
+        <v>50.916699999999999</v>
+      </c>
+      <c r="BI15" s="23">
+        <v>50.666699999999999</v>
+      </c>
+      <c r="BJ15" s="23">
+        <v>50.166699999999999</v>
+      </c>
+      <c r="BK15" s="23">
+        <v>50.333300000000001</v>
+      </c>
+      <c r="BL15" s="23">
+        <v>50.583300000000001</v>
+      </c>
+      <c r="BM15" s="23">
+        <v>50.75</v>
+      </c>
+      <c r="BN15" s="23">
+        <v>50.083300000000001</v>
+      </c>
+      <c r="BO15" s="23">
+        <v>50.25</v>
+      </c>
+      <c r="BP15" s="23">
+        <v>50.333300000000001</v>
+      </c>
+      <c r="BQ15" s="23">
+        <v>49.583300000000001</v>
+      </c>
+      <c r="BR15" s="23">
+        <v>50.166699999999999</v>
+      </c>
+      <c r="BS15" s="23">
+        <v>50.666699999999999</v>
+      </c>
+      <c r="BT15" s="23">
+        <v>50</v>
+      </c>
+      <c r="BU15" s="23">
+        <v>49.833300000000001</v>
+      </c>
+      <c r="BV15" s="23">
+        <v>49.833300000000001</v>
+      </c>
+      <c r="BW15" s="23">
+        <v>49.083300000000001</v>
+      </c>
+      <c r="BX15" s="23">
+        <v>48.083300000000001</v>
+      </c>
+      <c r="BY15" s="23">
+        <v>48.833300000000001</v>
+      </c>
+      <c r="BZ15" s="23">
+        <v>49.583300000000001</v>
+      </c>
+      <c r="CA15" s="23">
+        <v>49.083300000000001</v>
+      </c>
+      <c r="CB15" s="23">
+        <v>49.583300000000001</v>
+      </c>
+      <c r="CC15" s="23">
+        <v>49</v>
+      </c>
+      <c r="CD15" s="23">
+        <v>48.916699999999999</v>
+      </c>
+      <c r="CE15" s="23">
+        <v>49.583300000000001</v>
+      </c>
+      <c r="CF15" s="23">
+        <v>50</v>
+      </c>
+      <c r="CG15" s="23">
+        <v>50.333300000000001</v>
+      </c>
+      <c r="CH15" s="23">
+        <v>50.166699999999999</v>
+      </c>
+      <c r="CI15" s="23">
+        <v>51</v>
+      </c>
+      <c r="CJ15" s="23">
+        <v>50.25</v>
+      </c>
+      <c r="CK15" s="23">
+        <v>50.166699999999999</v>
+      </c>
+      <c r="CL15" s="23">
+        <v>50.25</v>
+      </c>
+      <c r="CM15" s="23">
+        <v>49.333300000000001</v>
+      </c>
+      <c r="CN15" s="23">
+        <v>48.833300000000001</v>
+      </c>
+      <c r="CO15" s="23">
+        <v>49.75</v>
+      </c>
+      <c r="CP15" s="23">
+        <v>50.25</v>
+      </c>
+      <c r="CQ15" s="23">
+        <v>50</v>
+      </c>
+      <c r="CR15" s="23">
+        <v>50.333300000000001</v>
+      </c>
+      <c r="CS15" s="23">
+        <v>51.083300000000001</v>
+      </c>
+      <c r="CT15" s="23">
+        <v>50.916699999999999</v>
+      </c>
+      <c r="CU15" s="23">
+        <v>50.916699999999999</v>
+      </c>
+      <c r="CV15" s="23">
+        <v>51.583300000000001</v>
+      </c>
+      <c r="CW15" s="23">
+        <v>50.916699999999999</v>
+      </c>
+      <c r="CX15" s="23">
+        <v>50.833300000000001</v>
+      </c>
+      <c r="CY15" s="23">
+        <f t="shared" si="0"/>
+        <v>53.75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:103">
+      <c r="A16" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="23">
+        <v>65.75</v>
+      </c>
+      <c r="C16" s="23">
+        <v>77.583299999999994</v>
+      </c>
+      <c r="D16" s="23">
+        <v>77.416700000000006</v>
+      </c>
+      <c r="E16" s="23">
+        <v>77.083299999999994</v>
+      </c>
+      <c r="F16" s="23">
+        <v>76.916700000000006</v>
+      </c>
+      <c r="G16" s="23">
+        <v>76.833299999999994</v>
+      </c>
+      <c r="H16" s="23">
+        <v>77.25</v>
+      </c>
+      <c r="I16" s="23">
+        <v>76.5</v>
+      </c>
+      <c r="J16" s="23">
+        <v>76.5</v>
+      </c>
+      <c r="K16" s="23">
+        <v>76.333299999999994</v>
+      </c>
+      <c r="L16" s="23">
+        <v>76.333299999999994</v>
+      </c>
+      <c r="M16" s="23">
+        <v>77</v>
+      </c>
+      <c r="N16" s="23">
+        <v>76.583299999999994</v>
+      </c>
+      <c r="O16" s="23">
+        <v>76.25</v>
+      </c>
+      <c r="P16" s="23">
+        <v>76.25</v>
+      </c>
+      <c r="Q16" s="23">
+        <v>76.166700000000006</v>
+      </c>
+      <c r="R16" s="23">
+        <v>76.916700000000006</v>
+      </c>
+      <c r="S16" s="23">
+        <v>76.75</v>
+      </c>
+      <c r="T16" s="23">
+        <v>76.416700000000006</v>
+      </c>
+      <c r="U16" s="23">
+        <v>76.416700000000006</v>
+      </c>
+      <c r="V16" s="23">
+        <v>76.083299999999994</v>
+      </c>
+      <c r="W16" s="23">
+        <v>76.083299999999994</v>
+      </c>
+      <c r="X16" s="23">
+        <v>76.25</v>
+      </c>
+      <c r="Y16" s="23">
+        <v>76.416700000000006</v>
+      </c>
+      <c r="Z16" s="23">
+        <v>76.583299999999994</v>
+      </c>
+      <c r="AA16" s="23">
+        <v>76.416700000000006</v>
+      </c>
+      <c r="AB16" s="23">
+        <v>76.75</v>
+      </c>
+      <c r="AC16" s="23">
+        <v>76.75</v>
+      </c>
+      <c r="AD16" s="23">
+        <v>76.916700000000006</v>
+      </c>
+      <c r="AE16" s="23">
+        <v>77.333299999999994</v>
+      </c>
+      <c r="AF16" s="23">
+        <v>77.166700000000006</v>
+      </c>
+      <c r="AG16" s="23">
+        <v>77.083299999999994</v>
+      </c>
+      <c r="AH16" s="23">
+        <v>75.833299999999994</v>
+      </c>
+      <c r="AI16" s="23">
+        <v>75.5</v>
+      </c>
+      <c r="AJ16" s="23">
+        <v>75.166700000000006</v>
+      </c>
+      <c r="AK16" s="23">
+        <v>75.166700000000006</v>
+      </c>
+      <c r="AL16" s="23">
+        <v>75.166700000000006</v>
+      </c>
+      <c r="AM16" s="23">
+        <v>75.333299999999994</v>
+      </c>
+      <c r="AN16" s="23">
+        <v>75.333299999999994</v>
+      </c>
+      <c r="AO16" s="23">
+        <v>75.5</v>
+      </c>
+      <c r="AP16" s="23">
+        <v>76.166700000000006</v>
+      </c>
+      <c r="AQ16" s="23">
+        <v>76.083299999999994</v>
+      </c>
+      <c r="AR16" s="23">
+        <v>76</v>
+      </c>
+      <c r="AS16" s="23">
+        <v>76.75</v>
+      </c>
+      <c r="AT16" s="23">
+        <v>76.5</v>
+      </c>
+      <c r="AU16" s="23">
+        <v>76.583299999999994</v>
+      </c>
+      <c r="AV16" s="23">
+        <v>76.416700000000006</v>
+      </c>
+      <c r="AW16" s="23">
+        <v>76.083299999999994</v>
+      </c>
+      <c r="AX16" s="23">
+        <v>76.166700000000006</v>
+      </c>
+      <c r="AY16" s="23">
+        <v>76.833299999999994</v>
+      </c>
+      <c r="AZ16" s="23">
+        <v>76.5</v>
+      </c>
+      <c r="BA16" s="23">
+        <v>76.583299999999994</v>
+      </c>
+      <c r="BB16" s="23">
+        <v>76.583299999999994</v>
+      </c>
+      <c r="BC16" s="23">
+        <v>76.583299999999994</v>
+      </c>
+      <c r="BD16" s="23">
+        <v>76.5</v>
+      </c>
+      <c r="BE16" s="23">
+        <v>76.5</v>
+      </c>
+      <c r="BF16" s="23">
+        <v>76.833299999999994</v>
+      </c>
+      <c r="BG16" s="23">
+        <v>76.583299999999994</v>
+      </c>
+      <c r="BH16" s="23">
+        <v>76.75</v>
+      </c>
+      <c r="BI16" s="23">
+        <v>76.833299999999994</v>
+      </c>
+      <c r="BJ16" s="23">
+        <v>76.75</v>
+      </c>
+      <c r="BK16" s="23">
+        <v>76.833299999999994</v>
+      </c>
+      <c r="BL16" s="23">
+        <v>76.833299999999994</v>
+      </c>
+      <c r="BM16" s="23">
+        <v>77.416700000000006</v>
+      </c>
+      <c r="BN16" s="23">
+        <v>77.166700000000006</v>
+      </c>
+      <c r="BO16" s="23">
+        <v>77.166700000000006</v>
+      </c>
+      <c r="BP16" s="23">
+        <v>77.25</v>
+      </c>
+      <c r="BQ16" s="23">
+        <v>77.25</v>
+      </c>
+      <c r="BR16" s="23">
+        <v>77.416700000000006</v>
+      </c>
+      <c r="BS16" s="23">
+        <v>77.416700000000006</v>
+      </c>
+      <c r="BT16" s="23">
+        <v>77.416700000000006</v>
+      </c>
+      <c r="BU16" s="23">
+        <v>77.25</v>
+      </c>
+      <c r="BV16" s="23">
+        <v>77.416700000000006</v>
+      </c>
+      <c r="BW16" s="23">
+        <v>77.416700000000006</v>
+      </c>
+      <c r="BX16" s="23">
+        <v>77.25</v>
+      </c>
+      <c r="BY16" s="23">
+        <v>77.25</v>
+      </c>
+      <c r="BZ16" s="23">
+        <v>77.25</v>
+      </c>
+      <c r="CA16" s="23">
+        <v>77.25</v>
+      </c>
+      <c r="CB16" s="23">
+        <v>77.25</v>
+      </c>
+      <c r="CC16" s="23">
+        <v>77.083299999999994</v>
+      </c>
+      <c r="CD16" s="23">
+        <v>77.083299999999994</v>
+      </c>
+      <c r="CE16" s="23">
+        <v>77.083299999999994</v>
+      </c>
+      <c r="CF16" s="23">
+        <v>77.083299999999994</v>
+      </c>
+      <c r="CG16" s="23">
+        <v>77.083299999999994</v>
+      </c>
+      <c r="CH16" s="23">
+        <v>77.083299999999994</v>
+      </c>
+      <c r="CI16" s="23">
+        <v>77.083299999999994</v>
+      </c>
+      <c r="CJ16" s="23">
+        <v>77.25</v>
+      </c>
+      <c r="CK16" s="23">
+        <v>77.25</v>
+      </c>
+      <c r="CL16" s="23">
+        <v>77.25</v>
+      </c>
+      <c r="CM16" s="23">
+        <v>77.25</v>
+      </c>
+      <c r="CN16" s="23">
+        <v>77.25</v>
+      </c>
+      <c r="CO16" s="23">
+        <v>77.25</v>
+      </c>
+      <c r="CP16" s="23">
+        <v>77.25</v>
+      </c>
+      <c r="CQ16" s="23">
+        <v>77.25</v>
+      </c>
+      <c r="CR16" s="23">
+        <v>77.25</v>
+      </c>
+      <c r="CS16" s="23">
+        <v>77.25</v>
+      </c>
+      <c r="CT16" s="23">
+        <v>77.25</v>
+      </c>
+      <c r="CU16" s="23">
+        <v>77.25</v>
+      </c>
+      <c r="CV16" s="23">
+        <v>77.25</v>
+      </c>
+      <c r="CW16" s="23">
+        <v>77.25</v>
+      </c>
+      <c r="CX16" s="23">
+        <v>77.25</v>
+      </c>
+      <c r="CY16" s="23">
+        <f t="shared" si="0"/>
+        <v>77.583299999999994</v>
+      </c>
+    </row>
+    <row r="17" spans="1:103">
+      <c r="A17" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="23">
+        <v>49.916699999999999</v>
+      </c>
+      <c r="C17" s="23">
+        <v>40.916699999999999</v>
+      </c>
+      <c r="D17" s="23">
+        <v>35.5</v>
+      </c>
+      <c r="E17" s="23">
+        <v>24.5</v>
+      </c>
+      <c r="F17" s="23">
+        <v>26</v>
+      </c>
+      <c r="G17" s="23">
+        <v>30.833300000000001</v>
+      </c>
+      <c r="H17" s="23">
+        <v>35.666699999999999</v>
+      </c>
+      <c r="I17" s="23">
+        <v>35.75</v>
+      </c>
+      <c r="J17" s="23">
+        <v>31.916699999999999</v>
+      </c>
+      <c r="K17" s="23">
+        <v>32</v>
+      </c>
+      <c r="L17" s="23">
+        <v>32.083300000000001</v>
+      </c>
+      <c r="M17" s="23">
+        <v>30.083300000000001</v>
+      </c>
+      <c r="N17" s="23">
+        <v>33.083300000000001</v>
+      </c>
+      <c r="O17" s="23">
+        <v>34.666699999999999</v>
+      </c>
+      <c r="P17" s="23">
+        <v>32.5</v>
+      </c>
+      <c r="Q17" s="23">
+        <v>34.5</v>
+      </c>
+      <c r="R17" s="23">
+        <v>34.5</v>
+      </c>
+      <c r="S17" s="23">
+        <v>35.5</v>
+      </c>
+      <c r="T17" s="23">
+        <v>34.333300000000001</v>
+      </c>
+      <c r="U17" s="23">
+        <v>33.5</v>
+      </c>
+      <c r="V17" s="23">
+        <v>34.083300000000001</v>
+      </c>
+      <c r="W17" s="23">
+        <v>35.5</v>
+      </c>
+      <c r="X17" s="23">
+        <v>34.166699999999999</v>
+      </c>
+      <c r="Y17" s="23">
+        <v>33.583300000000001</v>
+      </c>
+      <c r="Z17" s="23">
+        <v>34.416699999999999</v>
+      </c>
+      <c r="AA17" s="23">
+        <v>34.166699999999999</v>
+      </c>
+      <c r="AB17" s="23">
+        <v>34.333300000000001</v>
+      </c>
+      <c r="AC17" s="23">
+        <v>35.666699999999999</v>
+      </c>
+      <c r="AD17" s="23">
+        <v>35.166699999999999</v>
+      </c>
+      <c r="AE17" s="23">
+        <v>34.416699999999999</v>
+      </c>
+      <c r="AF17" s="23">
+        <v>36.833300000000001</v>
+      </c>
+      <c r="AG17" s="23">
+        <v>38.583300000000001</v>
+      </c>
+      <c r="AH17" s="23">
+        <v>37.583300000000001</v>
+      </c>
+      <c r="AI17" s="23">
+        <v>37.583300000000001</v>
+      </c>
+      <c r="AJ17" s="23">
+        <v>37</v>
+      </c>
+      <c r="AK17" s="23">
+        <v>36.833300000000001</v>
+      </c>
+      <c r="AL17" s="23">
+        <v>36.833300000000001</v>
+      </c>
+      <c r="AM17" s="23">
+        <v>36.166699999999999</v>
+      </c>
+      <c r="AN17" s="23">
+        <v>37.083300000000001</v>
+      </c>
+      <c r="AO17" s="23">
+        <v>36.166699999999999</v>
+      </c>
+      <c r="AP17" s="23">
+        <v>37.083300000000001</v>
+      </c>
+      <c r="AQ17" s="23">
+        <v>36.166699999999999</v>
+      </c>
+      <c r="AR17" s="23">
+        <v>35.583300000000001</v>
+      </c>
+      <c r="AS17" s="23">
+        <v>35.25</v>
+      </c>
+      <c r="AT17" s="23">
+        <v>35.916699999999999</v>
+      </c>
+      <c r="AU17" s="23">
+        <v>36.833300000000001</v>
+      </c>
+      <c r="AV17" s="23">
+        <v>35.166699999999999</v>
+      </c>
+      <c r="AW17" s="23">
+        <v>34.916699999999999</v>
+      </c>
+      <c r="AX17" s="23">
+        <v>33.333300000000001</v>
+      </c>
+      <c r="AY17" s="23">
+        <v>32.5</v>
+      </c>
+      <c r="AZ17" s="23">
+        <v>33</v>
+      </c>
+      <c r="BA17" s="23">
+        <v>32.833300000000001</v>
+      </c>
+      <c r="BB17" s="23">
+        <v>34.666699999999999</v>
+      </c>
+      <c r="BC17" s="23">
+        <v>33.333300000000001</v>
+      </c>
+      <c r="BD17" s="23">
+        <v>32.333300000000001</v>
+      </c>
+      <c r="BE17" s="23">
+        <v>32.75</v>
+      </c>
+      <c r="BF17" s="23">
+        <v>33.5</v>
+      </c>
+      <c r="BG17" s="23">
+        <v>32.75</v>
+      </c>
+      <c r="BH17" s="23">
+        <v>32</v>
+      </c>
+      <c r="BI17" s="23">
+        <v>32.583300000000001</v>
+      </c>
+      <c r="BJ17" s="23">
+        <v>33.333300000000001</v>
+      </c>
+      <c r="BK17" s="23">
+        <v>33.666699999999999</v>
+      </c>
+      <c r="BL17" s="23">
+        <v>35.25</v>
+      </c>
+      <c r="BM17" s="23">
+        <v>34.75</v>
+      </c>
+      <c r="BN17" s="23">
+        <v>34.75</v>
+      </c>
+      <c r="BO17" s="23">
+        <v>33.666699999999999</v>
+      </c>
+      <c r="BP17" s="23">
+        <v>33.333300000000001</v>
+      </c>
+      <c r="BQ17" s="23">
+        <v>34.416699999999999</v>
+      </c>
+      <c r="BR17" s="23">
+        <v>34.916699999999999</v>
+      </c>
+      <c r="BS17" s="23">
+        <v>35.083300000000001</v>
+      </c>
+      <c r="BT17" s="23">
+        <v>34.25</v>
+      </c>
+      <c r="BU17" s="23">
+        <v>35.416699999999999</v>
+      </c>
+      <c r="BV17" s="23">
+        <v>35.25</v>
+      </c>
+      <c r="BW17" s="23">
+        <v>34.5</v>
+      </c>
+      <c r="BX17" s="23">
+        <v>34.5</v>
+      </c>
+      <c r="BY17" s="23">
+        <v>34.416699999999999</v>
+      </c>
+      <c r="BZ17" s="23">
+        <v>34.25</v>
+      </c>
+      <c r="CA17" s="23">
+        <v>34.5</v>
+      </c>
+      <c r="CB17" s="23">
+        <v>34.666699999999999</v>
+      </c>
+      <c r="CC17" s="23">
+        <v>34.083300000000001</v>
+      </c>
+      <c r="CD17" s="23">
+        <v>34</v>
+      </c>
+      <c r="CE17" s="23">
+        <v>34.5</v>
+      </c>
+      <c r="CF17" s="23">
+        <v>33.833300000000001</v>
+      </c>
+      <c r="CG17" s="23">
+        <v>34</v>
+      </c>
+      <c r="CH17" s="23">
+        <v>34.416699999999999</v>
+      </c>
+      <c r="CI17" s="23">
+        <v>34.583300000000001</v>
+      </c>
+      <c r="CJ17" s="23">
+        <v>34.583300000000001</v>
+      </c>
+      <c r="CK17" s="23">
+        <v>34.5</v>
+      </c>
+      <c r="CL17" s="23">
+        <v>32.916699999999999</v>
+      </c>
+      <c r="CM17" s="23">
+        <v>32.416699999999999</v>
+      </c>
+      <c r="CN17" s="23">
+        <v>32.833300000000001</v>
+      </c>
+      <c r="CO17" s="23">
+        <v>32.75</v>
+      </c>
+      <c r="CP17" s="23">
+        <v>32.75</v>
+      </c>
+      <c r="CQ17" s="23">
+        <v>33.166699999999999</v>
+      </c>
+      <c r="CR17" s="23">
+        <v>32.666699999999999</v>
+      </c>
+      <c r="CS17" s="23">
+        <v>32.666699999999999</v>
+      </c>
+      <c r="CT17" s="23">
+        <v>32.666699999999999</v>
+      </c>
+      <c r="CU17" s="23">
+        <v>32.5</v>
+      </c>
+      <c r="CV17" s="23">
+        <v>33.833300000000001</v>
+      </c>
+      <c r="CW17" s="23">
+        <v>33.5</v>
+      </c>
+      <c r="CX17" s="23">
+        <v>32.916699999999999</v>
+      </c>
+      <c r="CY17" s="23">
+        <f t="shared" si="0"/>
+        <v>49.916699999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="A13:E13"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adding random classifier. Adding the images used in the thesis document
</commit_message>
<xml_diff>
--- a/MasterThesis/experiments/neural.xlsx
+++ b/MasterThesis/experiments/neural.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="28">
   <si>
     <t>Backpropagation, 6 експеримента, 82 обучаващи, 20 верифициращи, 10000 итерации в мрежата</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>MAX</t>
+  </si>
+  <si>
+    <t>Classifier: Neural network</t>
   </si>
 </sst>
 </file>
@@ -762,7 +765,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -790,6 +793,11 @@
     <xf numFmtId="0" fontId="0" fillId="30" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="30" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="28" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -808,7 +816,6 @@
     <xf numFmtId="0" fontId="0" fillId="28" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="31" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="28" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -816,9 +823,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="32" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Акцент1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -1234,7 +1240,7 @@
   <dimension ref="A1:O27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1247,13 +1253,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="30"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="33"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -1298,12 +1304,12 @@
       <c r="E3" s="5">
         <v>0.75829999999999997</v>
       </c>
-      <c r="H3" s="28" t="s">
+      <c r="H3" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="30"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="33"/>
     </row>
     <row r="4" spans="1:15" ht="15.75" thickBot="1">
       <c r="A4" s="20" t="s">
@@ -1392,13 +1398,13 @@
       </c>
     </row>
     <row r="8" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="29"/>
-      <c r="C8" s="29"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="30"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="33"/>
     </row>
     <row r="9" spans="1:15" ht="15.75" thickBot="1">
       <c r="A9" s="4" t="s">
@@ -1470,13 +1476,13 @@
     </row>
     <row r="14" spans="1:15" ht="15.75" thickBot="1"/>
     <row r="15" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A15" s="28" t="s">
+      <c r="A15" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="29"/>
-      <c r="C15" s="29"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="30"/>
+      <c r="B15" s="32"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="33"/>
     </row>
     <row r="16" spans="1:15" ht="15.75" thickBot="1">
       <c r="A16" s="4" t="s">
@@ -1548,13 +1554,13 @@
     </row>
     <row r="22" spans="1:5" ht="15.75" thickBot="1"/>
     <row r="23" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A23" s="25" t="s">
+      <c r="A23" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="26"/>
-      <c r="C23" s="26"/>
-      <c r="D23" s="26"/>
-      <c r="E23" s="27"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="30"/>
     </row>
     <row r="24" spans="1:5" ht="15.75" thickBot="1">
       <c r="A24" s="4" t="s">
@@ -1779,331 +1785,331 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:CY17"/>
+  <dimension ref="A1:CY24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="CW6" sqref="CW6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="AZ26" sqref="AZ26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:103">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
     </row>
     <row r="2" spans="1:103">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="31">
+      <c r="B2" s="25">
         <v>1</v>
       </c>
-      <c r="C2" s="31">
+      <c r="C2" s="25">
         <v>2</v>
       </c>
-      <c r="D2" s="31">
+      <c r="D2" s="25">
         <v>3</v>
       </c>
-      <c r="E2" s="31">
+      <c r="E2" s="25">
         <v>4</v>
       </c>
-      <c r="F2" s="31">
+      <c r="F2" s="25">
         <v>5</v>
       </c>
-      <c r="G2" s="31">
+      <c r="G2" s="25">
         <v>6</v>
       </c>
-      <c r="H2" s="31">
+      <c r="H2" s="25">
         <v>7</v>
       </c>
-      <c r="I2" s="31">
+      <c r="I2" s="25">
         <v>8</v>
       </c>
-      <c r="J2" s="31">
+      <c r="J2" s="25">
         <v>9</v>
       </c>
-      <c r="K2" s="31">
+      <c r="K2" s="25">
         <v>10</v>
       </c>
-      <c r="L2" s="31">
+      <c r="L2" s="25">
         <v>11</v>
       </c>
-      <c r="M2" s="31">
+      <c r="M2" s="25">
         <v>12</v>
       </c>
-      <c r="N2" s="31">
+      <c r="N2" s="25">
         <v>13</v>
       </c>
-      <c r="O2" s="31">
+      <c r="O2" s="25">
         <v>14</v>
       </c>
-      <c r="P2" s="31">
+      <c r="P2" s="25">
         <v>15</v>
       </c>
-      <c r="Q2" s="31">
+      <c r="Q2" s="25">
         <v>16</v>
       </c>
-      <c r="R2" s="31">
+      <c r="R2" s="25">
         <v>17</v>
       </c>
-      <c r="S2" s="31">
+      <c r="S2" s="25">
         <v>18</v>
       </c>
-      <c r="T2" s="31">
+      <c r="T2" s="25">
         <v>19</v>
       </c>
-      <c r="U2" s="31">
+      <c r="U2" s="25">
         <v>20</v>
       </c>
-      <c r="V2" s="31">
+      <c r="V2" s="25">
         <v>21</v>
       </c>
-      <c r="W2" s="31">
+      <c r="W2" s="25">
         <v>22</v>
       </c>
-      <c r="X2" s="31">
+      <c r="X2" s="25">
         <v>23</v>
       </c>
-      <c r="Y2" s="31">
+      <c r="Y2" s="25">
         <v>24</v>
       </c>
-      <c r="Z2" s="31">
+      <c r="Z2" s="25">
         <v>25</v>
       </c>
-      <c r="AA2" s="31">
+      <c r="AA2" s="25">
         <v>26</v>
       </c>
-      <c r="AB2" s="31">
+      <c r="AB2" s="25">
         <v>27</v>
       </c>
-      <c r="AC2" s="31">
+      <c r="AC2" s="25">
         <v>28</v>
       </c>
-      <c r="AD2" s="31">
+      <c r="AD2" s="25">
         <v>29</v>
       </c>
-      <c r="AE2" s="31">
+      <c r="AE2" s="25">
         <v>30</v>
       </c>
-      <c r="AF2" s="31">
+      <c r="AF2" s="25">
         <v>31</v>
       </c>
-      <c r="AG2" s="31">
+      <c r="AG2" s="25">
         <v>32</v>
       </c>
-      <c r="AH2" s="31">
+      <c r="AH2" s="25">
         <v>33</v>
       </c>
-      <c r="AI2" s="31">
+      <c r="AI2" s="25">
         <v>34</v>
       </c>
-      <c r="AJ2" s="31">
+      <c r="AJ2" s="25">
         <v>35</v>
       </c>
-      <c r="AK2" s="31">
+      <c r="AK2" s="25">
         <v>36</v>
       </c>
-      <c r="AL2" s="31">
+      <c r="AL2" s="25">
         <v>37</v>
       </c>
-      <c r="AM2" s="31">
+      <c r="AM2" s="25">
         <v>38</v>
       </c>
-      <c r="AN2" s="31">
+      <c r="AN2" s="25">
         <v>39</v>
       </c>
-      <c r="AO2" s="31">
+      <c r="AO2" s="25">
         <v>40</v>
       </c>
-      <c r="AP2" s="31">
+      <c r="AP2" s="25">
         <v>41</v>
       </c>
-      <c r="AQ2" s="31">
+      <c r="AQ2" s="25">
         <v>42</v>
       </c>
-      <c r="AR2" s="31">
+      <c r="AR2" s="25">
         <v>43</v>
       </c>
-      <c r="AS2" s="31">
+      <c r="AS2" s="25">
         <v>44</v>
       </c>
-      <c r="AT2" s="31">
+      <c r="AT2" s="25">
         <v>45</v>
       </c>
-      <c r="AU2" s="31">
+      <c r="AU2" s="25">
         <v>46</v>
       </c>
-      <c r="AV2" s="31">
+      <c r="AV2" s="25">
         <v>47</v>
       </c>
-      <c r="AW2" s="31">
+      <c r="AW2" s="25">
         <v>48</v>
       </c>
-      <c r="AX2" s="31">
+      <c r="AX2" s="25">
         <v>49</v>
       </c>
-      <c r="AY2" s="31">
+      <c r="AY2" s="25">
         <v>50</v>
       </c>
-      <c r="AZ2" s="31">
+      <c r="AZ2" s="25">
         <v>51</v>
       </c>
-      <c r="BA2" s="31">
+      <c r="BA2" s="25">
         <v>52</v>
       </c>
-      <c r="BB2" s="31">
+      <c r="BB2" s="25">
         <v>53</v>
       </c>
-      <c r="BC2" s="31">
+      <c r="BC2" s="25">
         <v>54</v>
       </c>
-      <c r="BD2" s="31">
+      <c r="BD2" s="25">
         <v>55</v>
       </c>
-      <c r="BE2" s="31">
+      <c r="BE2" s="25">
         <v>56</v>
       </c>
-      <c r="BF2" s="31">
+      <c r="BF2" s="25">
         <v>57</v>
       </c>
-      <c r="BG2" s="31">
+      <c r="BG2" s="25">
         <v>58</v>
       </c>
-      <c r="BH2" s="31">
+      <c r="BH2" s="25">
         <v>59</v>
       </c>
-      <c r="BI2" s="31">
+      <c r="BI2" s="25">
         <v>60</v>
       </c>
-      <c r="BJ2" s="31">
+      <c r="BJ2" s="25">
         <v>61</v>
       </c>
-      <c r="BK2" s="31">
+      <c r="BK2" s="25">
         <v>62</v>
       </c>
-      <c r="BL2" s="31">
+      <c r="BL2" s="25">
         <v>63</v>
       </c>
-      <c r="BM2" s="31">
+      <c r="BM2" s="25">
         <v>64</v>
       </c>
-      <c r="BN2" s="31">
+      <c r="BN2" s="25">
         <v>65</v>
       </c>
-      <c r="BO2" s="31">
+      <c r="BO2" s="25">
         <v>66</v>
       </c>
-      <c r="BP2" s="31">
+      <c r="BP2" s="25">
         <v>67</v>
       </c>
-      <c r="BQ2" s="31">
+      <c r="BQ2" s="25">
         <v>68</v>
       </c>
-      <c r="BR2" s="31">
+      <c r="BR2" s="25">
         <v>69</v>
       </c>
-      <c r="BS2" s="31">
+      <c r="BS2" s="25">
         <v>70</v>
       </c>
-      <c r="BT2" s="31">
+      <c r="BT2" s="25">
         <v>71</v>
       </c>
-      <c r="BU2" s="31">
+      <c r="BU2" s="25">
         <v>72</v>
       </c>
-      <c r="BV2" s="31">
+      <c r="BV2" s="25">
         <v>73</v>
       </c>
-      <c r="BW2" s="31">
+      <c r="BW2" s="25">
         <v>74</v>
       </c>
-      <c r="BX2" s="31">
+      <c r="BX2" s="25">
         <v>75</v>
       </c>
-      <c r="BY2" s="31">
+      <c r="BY2" s="25">
         <v>76</v>
       </c>
-      <c r="BZ2" s="31">
+      <c r="BZ2" s="25">
         <v>77</v>
       </c>
-      <c r="CA2" s="31">
+      <c r="CA2" s="25">
         <v>78</v>
       </c>
-      <c r="CB2" s="31">
+      <c r="CB2" s="25">
         <v>79</v>
       </c>
-      <c r="CC2" s="31">
+      <c r="CC2" s="25">
         <v>80</v>
       </c>
-      <c r="CD2" s="31">
+      <c r="CD2" s="25">
         <v>81</v>
       </c>
-      <c r="CE2" s="31">
+      <c r="CE2" s="25">
         <v>82</v>
       </c>
-      <c r="CF2" s="31">
+      <c r="CF2" s="25">
         <v>83</v>
       </c>
-      <c r="CG2" s="31">
+      <c r="CG2" s="25">
         <v>84</v>
       </c>
-      <c r="CH2" s="31">
+      <c r="CH2" s="25">
         <v>85</v>
       </c>
-      <c r="CI2" s="31">
+      <c r="CI2" s="25">
         <v>86</v>
       </c>
-      <c r="CJ2" s="31">
+      <c r="CJ2" s="25">
         <v>87</v>
       </c>
-      <c r="CK2" s="31">
+      <c r="CK2" s="25">
         <v>88</v>
       </c>
-      <c r="CL2" s="31">
+      <c r="CL2" s="25">
         <v>89</v>
       </c>
-      <c r="CM2" s="31">
+      <c r="CM2" s="25">
         <v>90</v>
       </c>
-      <c r="CN2" s="31">
+      <c r="CN2" s="25">
         <v>91</v>
       </c>
-      <c r="CO2" s="31">
+      <c r="CO2" s="25">
         <v>92</v>
       </c>
-      <c r="CP2" s="31">
+      <c r="CP2" s="25">
         <v>93</v>
       </c>
-      <c r="CQ2" s="31">
+      <c r="CQ2" s="25">
         <v>94</v>
       </c>
-      <c r="CR2" s="31">
+      <c r="CR2" s="25">
         <v>95</v>
       </c>
-      <c r="CS2" s="31">
+      <c r="CS2" s="25">
         <v>96</v>
       </c>
-      <c r="CT2" s="31">
+      <c r="CT2" s="25">
         <v>97</v>
       </c>
-      <c r="CU2" s="31">
+      <c r="CU2" s="25">
         <v>98</v>
       </c>
-      <c r="CV2" s="31">
+      <c r="CV2" s="25">
         <v>99</v>
       </c>
-      <c r="CW2" s="31">
+      <c r="CW2" s="25">
         <v>100</v>
       </c>
-      <c r="CX2" s="31">
+      <c r="CX2" s="25">
         <v>101</v>
       </c>
-      <c r="CY2" s="34" t="s">
+      <c r="CY2" s="26" t="s">
         <v>26</v>
       </c>
     </row>
@@ -3044,326 +3050,326 @@
       </c>
     </row>
     <row r="6" spans="1:103">
-      <c r="CY6" s="35"/>
+      <c r="CY6" s="27"/>
     </row>
     <row r="7" spans="1:103">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="33"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="CY7" s="35"/>
+      <c r="B7" s="35"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
+      <c r="CY7" s="27"/>
     </row>
     <row r="8" spans="1:103">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="31">
+      <c r="B8" s="25">
         <v>1</v>
       </c>
-      <c r="C8" s="31">
+      <c r="C8" s="25">
         <v>2</v>
       </c>
-      <c r="D8" s="31">
+      <c r="D8" s="25">
         <v>3</v>
       </c>
-      <c r="E8" s="31">
+      <c r="E8" s="25">
         <v>4</v>
       </c>
-      <c r="F8" s="31">
+      <c r="F8" s="25">
         <v>5</v>
       </c>
-      <c r="G8" s="31">
+      <c r="G8" s="25">
         <v>6</v>
       </c>
-      <c r="H8" s="31">
+      <c r="H8" s="25">
         <v>7</v>
       </c>
-      <c r="I8" s="31">
+      <c r="I8" s="25">
         <v>8</v>
       </c>
-      <c r="J8" s="31">
+      <c r="J8" s="25">
         <v>9</v>
       </c>
-      <c r="K8" s="31">
+      <c r="K8" s="25">
         <v>10</v>
       </c>
-      <c r="L8" s="31">
+      <c r="L8" s="25">
         <v>11</v>
       </c>
-      <c r="M8" s="31">
+      <c r="M8" s="25">
         <v>12</v>
       </c>
-      <c r="N8" s="31">
+      <c r="N8" s="25">
         <v>13</v>
       </c>
-      <c r="O8" s="31">
+      <c r="O8" s="25">
         <v>14</v>
       </c>
-      <c r="P8" s="31">
+      <c r="P8" s="25">
         <v>15</v>
       </c>
-      <c r="Q8" s="31">
+      <c r="Q8" s="25">
         <v>16</v>
       </c>
-      <c r="R8" s="31">
+      <c r="R8" s="25">
         <v>17</v>
       </c>
-      <c r="S8" s="31">
+      <c r="S8" s="25">
         <v>18</v>
       </c>
-      <c r="T8" s="31">
+      <c r="T8" s="25">
         <v>19</v>
       </c>
-      <c r="U8" s="31">
+      <c r="U8" s="25">
         <v>20</v>
       </c>
-      <c r="V8" s="31">
+      <c r="V8" s="25">
         <v>21</v>
       </c>
-      <c r="W8" s="31">
+      <c r="W8" s="25">
         <v>22</v>
       </c>
-      <c r="X8" s="31">
+      <c r="X8" s="25">
         <v>23</v>
       </c>
-      <c r="Y8" s="31">
+      <c r="Y8" s="25">
         <v>24</v>
       </c>
-      <c r="Z8" s="31">
+      <c r="Z8" s="25">
         <v>25</v>
       </c>
-      <c r="AA8" s="31">
+      <c r="AA8" s="25">
         <v>26</v>
       </c>
-      <c r="AB8" s="31">
+      <c r="AB8" s="25">
         <v>27</v>
       </c>
-      <c r="AC8" s="31">
+      <c r="AC8" s="25">
         <v>28</v>
       </c>
-      <c r="AD8" s="31">
+      <c r="AD8" s="25">
         <v>29</v>
       </c>
-      <c r="AE8" s="31">
+      <c r="AE8" s="25">
         <v>30</v>
       </c>
-      <c r="AF8" s="31">
+      <c r="AF8" s="25">
         <v>31</v>
       </c>
-      <c r="AG8" s="31">
+      <c r="AG8" s="25">
         <v>32</v>
       </c>
-      <c r="AH8" s="31">
+      <c r="AH8" s="25">
         <v>33</v>
       </c>
-      <c r="AI8" s="31">
+      <c r="AI8" s="25">
         <v>34</v>
       </c>
-      <c r="AJ8" s="31">
+      <c r="AJ8" s="25">
         <v>35</v>
       </c>
-      <c r="AK8" s="31">
+      <c r="AK8" s="25">
         <v>36</v>
       </c>
-      <c r="AL8" s="31">
+      <c r="AL8" s="25">
         <v>37</v>
       </c>
-      <c r="AM8" s="31">
+      <c r="AM8" s="25">
         <v>38</v>
       </c>
-      <c r="AN8" s="31">
+      <c r="AN8" s="25">
         <v>39</v>
       </c>
-      <c r="AO8" s="31">
+      <c r="AO8" s="25">
         <v>40</v>
       </c>
-      <c r="AP8" s="31">
+      <c r="AP8" s="25">
         <v>41</v>
       </c>
-      <c r="AQ8" s="31">
+      <c r="AQ8" s="25">
         <v>42</v>
       </c>
-      <c r="AR8" s="31">
+      <c r="AR8" s="25">
         <v>43</v>
       </c>
-      <c r="AS8" s="31">
+      <c r="AS8" s="25">
         <v>44</v>
       </c>
-      <c r="AT8" s="31">
+      <c r="AT8" s="25">
         <v>45</v>
       </c>
-      <c r="AU8" s="31">
+      <c r="AU8" s="25">
         <v>46</v>
       </c>
-      <c r="AV8" s="31">
+      <c r="AV8" s="25">
         <v>47</v>
       </c>
-      <c r="AW8" s="31">
+      <c r="AW8" s="25">
         <v>48</v>
       </c>
-      <c r="AX8" s="31">
+      <c r="AX8" s="25">
         <v>49</v>
       </c>
-      <c r="AY8" s="31">
+      <c r="AY8" s="25">
         <v>50</v>
       </c>
-      <c r="AZ8" s="31">
+      <c r="AZ8" s="25">
         <v>51</v>
       </c>
-      <c r="BA8" s="31">
+      <c r="BA8" s="25">
         <v>52</v>
       </c>
-      <c r="BB8" s="31">
+      <c r="BB8" s="25">
         <v>53</v>
       </c>
-      <c r="BC8" s="31">
+      <c r="BC8" s="25">
         <v>54</v>
       </c>
-      <c r="BD8" s="31">
+      <c r="BD8" s="25">
         <v>55</v>
       </c>
-      <c r="BE8" s="31">
+      <c r="BE8" s="25">
         <v>56</v>
       </c>
-      <c r="BF8" s="31">
+      <c r="BF8" s="25">
         <v>57</v>
       </c>
-      <c r="BG8" s="31">
+      <c r="BG8" s="25">
         <v>58</v>
       </c>
-      <c r="BH8" s="31">
+      <c r="BH8" s="25">
         <v>59</v>
       </c>
-      <c r="BI8" s="31">
+      <c r="BI8" s="25">
         <v>60</v>
       </c>
-      <c r="BJ8" s="31">
+      <c r="BJ8" s="25">
         <v>61</v>
       </c>
-      <c r="BK8" s="31">
+      <c r="BK8" s="25">
         <v>62</v>
       </c>
-      <c r="BL8" s="31">
+      <c r="BL8" s="25">
         <v>63</v>
       </c>
-      <c r="BM8" s="31">
+      <c r="BM8" s="25">
         <v>64</v>
       </c>
-      <c r="BN8" s="31">
+      <c r="BN8" s="25">
         <v>65</v>
       </c>
-      <c r="BO8" s="31">
+      <c r="BO8" s="25">
         <v>66</v>
       </c>
-      <c r="BP8" s="31">
+      <c r="BP8" s="25">
         <v>67</v>
       </c>
-      <c r="BQ8" s="31">
+      <c r="BQ8" s="25">
         <v>68</v>
       </c>
-      <c r="BR8" s="31">
+      <c r="BR8" s="25">
         <v>69</v>
       </c>
-      <c r="BS8" s="31">
+      <c r="BS8" s="25">
         <v>70</v>
       </c>
-      <c r="BT8" s="31">
+      <c r="BT8" s="25">
         <v>71</v>
       </c>
-      <c r="BU8" s="31">
+      <c r="BU8" s="25">
         <v>72</v>
       </c>
-      <c r="BV8" s="31">
+      <c r="BV8" s="25">
         <v>73</v>
       </c>
-      <c r="BW8" s="31">
+      <c r="BW8" s="25">
         <v>74</v>
       </c>
-      <c r="BX8" s="31">
+      <c r="BX8" s="25">
         <v>75</v>
       </c>
-      <c r="BY8" s="31">
+      <c r="BY8" s="25">
         <v>76</v>
       </c>
-      <c r="BZ8" s="31">
+      <c r="BZ8" s="25">
         <v>77</v>
       </c>
-      <c r="CA8" s="31">
+      <c r="CA8" s="25">
         <v>78</v>
       </c>
-      <c r="CB8" s="31">
+      <c r="CB8" s="25">
         <v>79</v>
       </c>
-      <c r="CC8" s="31">
+      <c r="CC8" s="25">
         <v>80</v>
       </c>
-      <c r="CD8" s="31">
+      <c r="CD8" s="25">
         <v>81</v>
       </c>
-      <c r="CE8" s="31">
+      <c r="CE8" s="25">
         <v>82</v>
       </c>
-      <c r="CF8" s="31">
+      <c r="CF8" s="25">
         <v>83</v>
       </c>
-      <c r="CG8" s="31">
+      <c r="CG8" s="25">
         <v>84</v>
       </c>
-      <c r="CH8" s="31">
+      <c r="CH8" s="25">
         <v>85</v>
       </c>
-      <c r="CI8" s="31">
+      <c r="CI8" s="25">
         <v>86</v>
       </c>
-      <c r="CJ8" s="31">
+      <c r="CJ8" s="25">
         <v>87</v>
       </c>
-      <c r="CK8" s="31">
+      <c r="CK8" s="25">
         <v>88</v>
       </c>
-      <c r="CL8" s="31">
+      <c r="CL8" s="25">
         <v>89</v>
       </c>
-      <c r="CM8" s="31">
+      <c r="CM8" s="25">
         <v>90</v>
       </c>
-      <c r="CN8" s="31">
+      <c r="CN8" s="25">
         <v>91</v>
       </c>
-      <c r="CO8" s="31">
+      <c r="CO8" s="25">
         <v>92</v>
       </c>
-      <c r="CP8" s="31">
+      <c r="CP8" s="25">
         <v>93</v>
       </c>
-      <c r="CQ8" s="31">
+      <c r="CQ8" s="25">
         <v>94</v>
       </c>
-      <c r="CR8" s="31">
+      <c r="CR8" s="25">
         <v>95</v>
       </c>
-      <c r="CS8" s="31">
+      <c r="CS8" s="25">
         <v>96</v>
       </c>
-      <c r="CT8" s="31">
+      <c r="CT8" s="25">
         <v>97</v>
       </c>
-      <c r="CU8" s="31">
+      <c r="CU8" s="25">
         <v>98</v>
       </c>
-      <c r="CV8" s="31">
+      <c r="CV8" s="25">
         <v>99</v>
       </c>
-      <c r="CW8" s="31">
+      <c r="CW8" s="25">
         <v>100</v>
       </c>
-      <c r="CX8" s="31">
+      <c r="CX8" s="25">
         <v>101</v>
       </c>
-      <c r="CY8" s="34" t="s">
+      <c r="CY8" s="26" t="s">
         <v>26</v>
       </c>
     </row>
@@ -4304,326 +4310,326 @@
       </c>
     </row>
     <row r="12" spans="1:103">
-      <c r="CY12" s="35"/>
+      <c r="CY12" s="27"/>
     </row>
     <row r="13" spans="1:103">
-      <c r="A13" s="33" t="s">
+      <c r="A13" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="33"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="33"/>
-      <c r="CY13" s="35"/>
+      <c r="B13" s="35"/>
+      <c r="C13" s="35"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="35"/>
+      <c r="CY13" s="27"/>
     </row>
     <row r="14" spans="1:103">
-      <c r="A14" s="31" t="s">
+      <c r="A14" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="31">
+      <c r="B14" s="25">
         <v>1</v>
       </c>
-      <c r="C14" s="31">
+      <c r="C14" s="25">
         <v>2</v>
       </c>
-      <c r="D14" s="31">
+      <c r="D14" s="25">
         <v>3</v>
       </c>
-      <c r="E14" s="31">
+      <c r="E14" s="25">
         <v>4</v>
       </c>
-      <c r="F14" s="31">
+      <c r="F14" s="25">
         <v>5</v>
       </c>
-      <c r="G14" s="31">
+      <c r="G14" s="25">
         <v>6</v>
       </c>
-      <c r="H14" s="31">
+      <c r="H14" s="25">
         <v>7</v>
       </c>
-      <c r="I14" s="31">
+      <c r="I14" s="25">
         <v>8</v>
       </c>
-      <c r="J14" s="31">
+      <c r="J14" s="25">
         <v>9</v>
       </c>
-      <c r="K14" s="31">
+      <c r="K14" s="25">
         <v>10</v>
       </c>
-      <c r="L14" s="31">
+      <c r="L14" s="25">
         <v>11</v>
       </c>
-      <c r="M14" s="31">
+      <c r="M14" s="25">
         <v>12</v>
       </c>
-      <c r="N14" s="31">
+      <c r="N14" s="25">
         <v>13</v>
       </c>
-      <c r="O14" s="31">
+      <c r="O14" s="25">
         <v>14</v>
       </c>
-      <c r="P14" s="31">
+      <c r="P14" s="25">
         <v>15</v>
       </c>
-      <c r="Q14" s="31">
+      <c r="Q14" s="25">
         <v>16</v>
       </c>
-      <c r="R14" s="31">
+      <c r="R14" s="25">
         <v>17</v>
       </c>
-      <c r="S14" s="31">
+      <c r="S14" s="25">
         <v>18</v>
       </c>
-      <c r="T14" s="31">
+      <c r="T14" s="25">
         <v>19</v>
       </c>
-      <c r="U14" s="31">
+      <c r="U14" s="25">
         <v>20</v>
       </c>
-      <c r="V14" s="31">
+      <c r="V14" s="25">
         <v>21</v>
       </c>
-      <c r="W14" s="31">
+      <c r="W14" s="25">
         <v>22</v>
       </c>
-      <c r="X14" s="31">
+      <c r="X14" s="25">
         <v>23</v>
       </c>
-      <c r="Y14" s="31">
+      <c r="Y14" s="25">
         <v>24</v>
       </c>
-      <c r="Z14" s="31">
+      <c r="Z14" s="25">
         <v>25</v>
       </c>
-      <c r="AA14" s="31">
+      <c r="AA14" s="25">
         <v>26</v>
       </c>
-      <c r="AB14" s="31">
+      <c r="AB14" s="25">
         <v>27</v>
       </c>
-      <c r="AC14" s="31">
+      <c r="AC14" s="25">
         <v>28</v>
       </c>
-      <c r="AD14" s="31">
+      <c r="AD14" s="25">
         <v>29</v>
       </c>
-      <c r="AE14" s="31">
+      <c r="AE14" s="25">
         <v>30</v>
       </c>
-      <c r="AF14" s="31">
+      <c r="AF14" s="25">
         <v>31</v>
       </c>
-      <c r="AG14" s="31">
+      <c r="AG14" s="25">
         <v>32</v>
       </c>
-      <c r="AH14" s="31">
+      <c r="AH14" s="25">
         <v>33</v>
       </c>
-      <c r="AI14" s="31">
+      <c r="AI14" s="25">
         <v>34</v>
       </c>
-      <c r="AJ14" s="31">
+      <c r="AJ14" s="25">
         <v>35</v>
       </c>
-      <c r="AK14" s="31">
+      <c r="AK14" s="25">
         <v>36</v>
       </c>
-      <c r="AL14" s="31">
+      <c r="AL14" s="25">
         <v>37</v>
       </c>
-      <c r="AM14" s="31">
+      <c r="AM14" s="25">
         <v>38</v>
       </c>
-      <c r="AN14" s="31">
+      <c r="AN14" s="25">
         <v>39</v>
       </c>
-      <c r="AO14" s="31">
+      <c r="AO14" s="25">
         <v>40</v>
       </c>
-      <c r="AP14" s="31">
+      <c r="AP14" s="25">
         <v>41</v>
       </c>
-      <c r="AQ14" s="31">
+      <c r="AQ14" s="25">
         <v>42</v>
       </c>
-      <c r="AR14" s="31">
+      <c r="AR14" s="25">
         <v>43</v>
       </c>
-      <c r="AS14" s="31">
+      <c r="AS14" s="25">
         <v>44</v>
       </c>
-      <c r="AT14" s="31">
+      <c r="AT14" s="25">
         <v>45</v>
       </c>
-      <c r="AU14" s="31">
+      <c r="AU14" s="25">
         <v>46</v>
       </c>
-      <c r="AV14" s="31">
+      <c r="AV14" s="25">
         <v>47</v>
       </c>
-      <c r="AW14" s="31">
+      <c r="AW14" s="25">
         <v>48</v>
       </c>
-      <c r="AX14" s="31">
+      <c r="AX14" s="25">
         <v>49</v>
       </c>
-      <c r="AY14" s="31">
+      <c r="AY14" s="25">
         <v>50</v>
       </c>
-      <c r="AZ14" s="31">
+      <c r="AZ14" s="25">
         <v>51</v>
       </c>
-      <c r="BA14" s="31">
+      <c r="BA14" s="25">
         <v>52</v>
       </c>
-      <c r="BB14" s="31">
+      <c r="BB14" s="25">
         <v>53</v>
       </c>
-      <c r="BC14" s="31">
+      <c r="BC14" s="25">
         <v>54</v>
       </c>
-      <c r="BD14" s="31">
+      <c r="BD14" s="25">
         <v>55</v>
       </c>
-      <c r="BE14" s="31">
+      <c r="BE14" s="25">
         <v>56</v>
       </c>
-      <c r="BF14" s="31">
+      <c r="BF14" s="25">
         <v>57</v>
       </c>
-      <c r="BG14" s="31">
+      <c r="BG14" s="25">
         <v>58</v>
       </c>
-      <c r="BH14" s="31">
+      <c r="BH14" s="25">
         <v>59</v>
       </c>
-      <c r="BI14" s="31">
+      <c r="BI14" s="25">
         <v>60</v>
       </c>
-      <c r="BJ14" s="31">
+      <c r="BJ14" s="25">
         <v>61</v>
       </c>
-      <c r="BK14" s="31">
+      <c r="BK14" s="25">
         <v>62</v>
       </c>
-      <c r="BL14" s="31">
+      <c r="BL14" s="25">
         <v>63</v>
       </c>
-      <c r="BM14" s="31">
+      <c r="BM14" s="25">
         <v>64</v>
       </c>
-      <c r="BN14" s="31">
+      <c r="BN14" s="25">
         <v>65</v>
       </c>
-      <c r="BO14" s="31">
+      <c r="BO14" s="25">
         <v>66</v>
       </c>
-      <c r="BP14" s="31">
+      <c r="BP14" s="25">
         <v>67</v>
       </c>
-      <c r="BQ14" s="31">
+      <c r="BQ14" s="25">
         <v>68</v>
       </c>
-      <c r="BR14" s="31">
+      <c r="BR14" s="25">
         <v>69</v>
       </c>
-      <c r="BS14" s="31">
+      <c r="BS14" s="25">
         <v>70</v>
       </c>
-      <c r="BT14" s="31">
+      <c r="BT14" s="25">
         <v>71</v>
       </c>
-      <c r="BU14" s="31">
+      <c r="BU14" s="25">
         <v>72</v>
       </c>
-      <c r="BV14" s="31">
+      <c r="BV14" s="25">
         <v>73</v>
       </c>
-      <c r="BW14" s="31">
+      <c r="BW14" s="25">
         <v>74</v>
       </c>
-      <c r="BX14" s="31">
+      <c r="BX14" s="25">
         <v>75</v>
       </c>
-      <c r="BY14" s="31">
+      <c r="BY14" s="25">
         <v>76</v>
       </c>
-      <c r="BZ14" s="31">
+      <c r="BZ14" s="25">
         <v>77</v>
       </c>
-      <c r="CA14" s="31">
+      <c r="CA14" s="25">
         <v>78</v>
       </c>
-      <c r="CB14" s="31">
+      <c r="CB14" s="25">
         <v>79</v>
       </c>
-      <c r="CC14" s="31">
+      <c r="CC14" s="25">
         <v>80</v>
       </c>
-      <c r="CD14" s="31">
+      <c r="CD14" s="25">
         <v>81</v>
       </c>
-      <c r="CE14" s="31">
+      <c r="CE14" s="25">
         <v>82</v>
       </c>
-      <c r="CF14" s="31">
+      <c r="CF14" s="25">
         <v>83</v>
       </c>
-      <c r="CG14" s="31">
+      <c r="CG14" s="25">
         <v>84</v>
       </c>
-      <c r="CH14" s="31">
+      <c r="CH14" s="25">
         <v>85</v>
       </c>
-      <c r="CI14" s="31">
+      <c r="CI14" s="25">
         <v>86</v>
       </c>
-      <c r="CJ14" s="31">
+      <c r="CJ14" s="25">
         <v>87</v>
       </c>
-      <c r="CK14" s="31">
+      <c r="CK14" s="25">
         <v>88</v>
       </c>
-      <c r="CL14" s="31">
+      <c r="CL14" s="25">
         <v>89</v>
       </c>
-      <c r="CM14" s="31">
+      <c r="CM14" s="25">
         <v>90</v>
       </c>
-      <c r="CN14" s="31">
+      <c r="CN14" s="25">
         <v>91</v>
       </c>
-      <c r="CO14" s="31">
+      <c r="CO14" s="25">
         <v>92</v>
       </c>
-      <c r="CP14" s="31">
+      <c r="CP14" s="25">
         <v>93</v>
       </c>
-      <c r="CQ14" s="31">
+      <c r="CQ14" s="25">
         <v>94</v>
       </c>
-      <c r="CR14" s="31">
+      <c r="CR14" s="25">
         <v>95</v>
       </c>
-      <c r="CS14" s="31">
+      <c r="CS14" s="25">
         <v>96</v>
       </c>
-      <c r="CT14" s="31">
+      <c r="CT14" s="25">
         <v>97</v>
       </c>
-      <c r="CU14" s="31">
+      <c r="CU14" s="25">
         <v>98</v>
       </c>
-      <c r="CV14" s="31">
+      <c r="CV14" s="25">
         <v>99</v>
       </c>
-      <c r="CW14" s="31">
+      <c r="CW14" s="25">
         <v>100</v>
       </c>
-      <c r="CX14" s="31">
+      <c r="CX14" s="25">
         <v>101</v>
       </c>
-      <c r="CY14" s="34" t="s">
+      <c r="CY14" s="26" t="s">
         <v>26</v>
       </c>
     </row>
@@ -5563,11 +5569,680 @@
         <v>49.916699999999999</v>
       </c>
     </row>
+    <row r="20" spans="1:103">
+      <c r="A20" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="35"/>
+      <c r="C20" s="35"/>
+      <c r="D20" s="35"/>
+      <c r="E20" s="35"/>
+    </row>
+    <row r="21" spans="1:103">
+      <c r="A21" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="25">
+        <v>1</v>
+      </c>
+      <c r="C21" s="25">
+        <v>2</v>
+      </c>
+      <c r="D21" s="25">
+        <v>3</v>
+      </c>
+      <c r="E21" s="25">
+        <v>4</v>
+      </c>
+      <c r="F21" s="25">
+        <v>5</v>
+      </c>
+      <c r="G21" s="25">
+        <v>6</v>
+      </c>
+      <c r="H21" s="25">
+        <v>7</v>
+      </c>
+      <c r="I21" s="25">
+        <v>8</v>
+      </c>
+      <c r="J21" s="25">
+        <v>9</v>
+      </c>
+      <c r="K21" s="25">
+        <v>10</v>
+      </c>
+      <c r="L21" s="25">
+        <v>11</v>
+      </c>
+      <c r="M21" s="25">
+        <v>20</v>
+      </c>
+      <c r="N21" s="25">
+        <v>21</v>
+      </c>
+      <c r="O21" s="25">
+        <v>22</v>
+      </c>
+      <c r="P21" s="25">
+        <v>23</v>
+      </c>
+      <c r="Q21" s="25">
+        <v>24</v>
+      </c>
+      <c r="R21" s="25">
+        <v>25</v>
+      </c>
+      <c r="S21" s="25">
+        <v>26</v>
+      </c>
+      <c r="T21" s="25">
+        <v>27</v>
+      </c>
+      <c r="U21" s="25">
+        <v>28</v>
+      </c>
+      <c r="V21" s="25">
+        <v>29</v>
+      </c>
+      <c r="W21" s="25">
+        <v>30</v>
+      </c>
+      <c r="X21" s="25">
+        <v>31</v>
+      </c>
+      <c r="Y21" s="25">
+        <v>32</v>
+      </c>
+      <c r="Z21" s="25">
+        <v>33</v>
+      </c>
+      <c r="AA21" s="25">
+        <v>34</v>
+      </c>
+      <c r="AB21" s="25">
+        <v>35</v>
+      </c>
+      <c r="AC21" s="25">
+        <v>36</v>
+      </c>
+      <c r="AD21" s="25">
+        <v>37</v>
+      </c>
+      <c r="AE21" s="25">
+        <v>38</v>
+      </c>
+      <c r="AF21" s="25">
+        <v>39</v>
+      </c>
+      <c r="AG21" s="25">
+        <v>40</v>
+      </c>
+      <c r="AH21" s="25">
+        <v>41</v>
+      </c>
+      <c r="AI21" s="25">
+        <v>42</v>
+      </c>
+      <c r="AJ21" s="25">
+        <v>43</v>
+      </c>
+      <c r="AK21" s="25">
+        <v>44</v>
+      </c>
+      <c r="AL21" s="25">
+        <v>45</v>
+      </c>
+      <c r="AM21" s="25">
+        <v>46</v>
+      </c>
+      <c r="AN21" s="25">
+        <v>47</v>
+      </c>
+      <c r="AO21" s="25">
+        <v>48</v>
+      </c>
+      <c r="AP21" s="25">
+        <v>49</v>
+      </c>
+      <c r="AQ21" s="25">
+        <v>50</v>
+      </c>
+      <c r="AR21" s="25">
+        <v>51</v>
+      </c>
+      <c r="AS21" s="25">
+        <v>52</v>
+      </c>
+      <c r="AT21" s="25">
+        <v>53</v>
+      </c>
+      <c r="AU21" s="25">
+        <v>54</v>
+      </c>
+      <c r="AV21" s="25">
+        <v>55</v>
+      </c>
+      <c r="AW21" s="25">
+        <v>56</v>
+      </c>
+      <c r="AX21" s="25">
+        <v>57</v>
+      </c>
+      <c r="AY21" s="25">
+        <v>58</v>
+      </c>
+      <c r="AZ21" s="25">
+        <v>59</v>
+      </c>
+      <c r="BA21" s="25">
+        <v>60</v>
+      </c>
+      <c r="BB21" s="36" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:103">
+      <c r="A22" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="23">
+        <v>58</v>
+      </c>
+      <c r="C22" s="23">
+        <v>55.125</v>
+      </c>
+      <c r="D22" s="23">
+        <v>55.5</v>
+      </c>
+      <c r="E22" s="23">
+        <v>54.5</v>
+      </c>
+      <c r="F22" s="23">
+        <v>54.875</v>
+      </c>
+      <c r="G22" s="23">
+        <v>56.5</v>
+      </c>
+      <c r="H22" s="23">
+        <v>57.75</v>
+      </c>
+      <c r="I22" s="23">
+        <v>61.875</v>
+      </c>
+      <c r="J22" s="23">
+        <v>62.125</v>
+      </c>
+      <c r="K22" s="23">
+        <v>63.375</v>
+      </c>
+      <c r="L22" s="23">
+        <v>64.25</v>
+      </c>
+      <c r="M22" s="23">
+        <v>61.75</v>
+      </c>
+      <c r="N22" s="23">
+        <v>61.75</v>
+      </c>
+      <c r="O22" s="23">
+        <v>59</v>
+      </c>
+      <c r="P22" s="23">
+        <v>59.875</v>
+      </c>
+      <c r="Q22" s="23">
+        <v>59.5</v>
+      </c>
+      <c r="R22" s="23">
+        <v>59.125</v>
+      </c>
+      <c r="S22" s="23">
+        <v>58.625</v>
+      </c>
+      <c r="T22" s="23">
+        <v>58.75</v>
+      </c>
+      <c r="U22" s="23">
+        <v>60.375</v>
+      </c>
+      <c r="V22" s="23">
+        <v>60.25</v>
+      </c>
+      <c r="W22" s="23">
+        <v>58.375</v>
+      </c>
+      <c r="X22" s="23">
+        <v>58.375</v>
+      </c>
+      <c r="Y22" s="23">
+        <v>60.25</v>
+      </c>
+      <c r="Z22" s="23">
+        <v>58.125</v>
+      </c>
+      <c r="AA22" s="23">
+        <v>57.875</v>
+      </c>
+      <c r="AB22" s="23">
+        <v>57.125</v>
+      </c>
+      <c r="AC22" s="23">
+        <v>55.625</v>
+      </c>
+      <c r="AD22" s="23">
+        <v>58.125</v>
+      </c>
+      <c r="AE22" s="23">
+        <v>57</v>
+      </c>
+      <c r="AF22" s="23">
+        <v>58.625</v>
+      </c>
+      <c r="AG22" s="23">
+        <v>60.625</v>
+      </c>
+      <c r="AH22" s="23">
+        <v>60.375</v>
+      </c>
+      <c r="AI22" s="23">
+        <v>59.25</v>
+      </c>
+      <c r="AJ22" s="23">
+        <v>60.875</v>
+      </c>
+      <c r="AK22" s="23">
+        <v>57.375</v>
+      </c>
+      <c r="AL22" s="23">
+        <v>56.75</v>
+      </c>
+      <c r="AM22" s="23">
+        <v>55.625</v>
+      </c>
+      <c r="AN22" s="23">
+        <v>56</v>
+      </c>
+      <c r="AO22" s="23">
+        <v>56</v>
+      </c>
+      <c r="AP22" s="23">
+        <v>54</v>
+      </c>
+      <c r="AQ22" s="23">
+        <v>54.5</v>
+      </c>
+      <c r="AR22" s="23">
+        <v>54.5</v>
+      </c>
+      <c r="AS22" s="23">
+        <v>53.875</v>
+      </c>
+      <c r="AT22" s="23">
+        <v>52</v>
+      </c>
+      <c r="AU22" s="23">
+        <v>52.5</v>
+      </c>
+      <c r="AV22" s="23">
+        <v>53</v>
+      </c>
+      <c r="AW22" s="23">
+        <v>53.75</v>
+      </c>
+      <c r="AX22" s="23">
+        <v>51.75</v>
+      </c>
+      <c r="AY22" s="23">
+        <v>52.375</v>
+      </c>
+      <c r="AZ22" s="23">
+        <v>51.25</v>
+      </c>
+      <c r="BA22" s="23">
+        <v>52.25</v>
+      </c>
+      <c r="BB22" s="23">
+        <f>MAX(B22:BA22)</f>
+        <v>64.25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:103">
+      <c r="A23" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" s="23">
+        <v>67.375</v>
+      </c>
+      <c r="C23" s="23">
+        <v>68.75</v>
+      </c>
+      <c r="D23" s="23">
+        <v>70.75</v>
+      </c>
+      <c r="E23" s="23">
+        <v>71.125</v>
+      </c>
+      <c r="F23" s="23">
+        <v>69.125</v>
+      </c>
+      <c r="G23" s="23">
+        <v>68.75</v>
+      </c>
+      <c r="H23" s="23">
+        <v>70.625</v>
+      </c>
+      <c r="I23" s="23">
+        <v>69.5</v>
+      </c>
+      <c r="J23" s="23">
+        <v>68.875</v>
+      </c>
+      <c r="K23" s="23">
+        <v>72.5</v>
+      </c>
+      <c r="L23" s="23">
+        <v>71.5</v>
+      </c>
+      <c r="M23" s="23">
+        <v>73.125</v>
+      </c>
+      <c r="N23" s="23">
+        <v>72.375</v>
+      </c>
+      <c r="O23" s="23">
+        <v>71.125</v>
+      </c>
+      <c r="P23" s="23">
+        <v>70.25</v>
+      </c>
+      <c r="Q23" s="23">
+        <v>70</v>
+      </c>
+      <c r="R23" s="23">
+        <v>69.625</v>
+      </c>
+      <c r="S23" s="23">
+        <v>68.125</v>
+      </c>
+      <c r="T23" s="23">
+        <v>71.875</v>
+      </c>
+      <c r="U23" s="23">
+        <v>71.5</v>
+      </c>
+      <c r="V23" s="23">
+        <v>71.75</v>
+      </c>
+      <c r="W23" s="23">
+        <v>71.125</v>
+      </c>
+      <c r="X23" s="23">
+        <v>74.5</v>
+      </c>
+      <c r="Y23" s="23">
+        <v>72.875</v>
+      </c>
+      <c r="Z23" s="23">
+        <v>71.875</v>
+      </c>
+      <c r="AA23" s="23">
+        <v>73.25</v>
+      </c>
+      <c r="AB23" s="23">
+        <v>73.625</v>
+      </c>
+      <c r="AC23" s="23">
+        <v>75.375</v>
+      </c>
+      <c r="AD23" s="23">
+        <v>74.125</v>
+      </c>
+      <c r="AE23" s="23">
+        <v>72.5</v>
+      </c>
+      <c r="AF23" s="23">
+        <v>74.375</v>
+      </c>
+      <c r="AG23" s="23">
+        <v>73.5</v>
+      </c>
+      <c r="AH23" s="23">
+        <v>72.125</v>
+      </c>
+      <c r="AI23" s="23">
+        <v>71.25</v>
+      </c>
+      <c r="AJ23" s="23">
+        <v>71.75</v>
+      </c>
+      <c r="AK23" s="23">
+        <v>70.25</v>
+      </c>
+      <c r="AL23" s="23">
+        <v>70.75</v>
+      </c>
+      <c r="AM23" s="23">
+        <v>70.375</v>
+      </c>
+      <c r="AN23" s="23">
+        <v>70.875</v>
+      </c>
+      <c r="AO23" s="23">
+        <v>75.875</v>
+      </c>
+      <c r="AP23" s="23">
+        <v>75.625</v>
+      </c>
+      <c r="AQ23" s="23">
+        <v>74.125</v>
+      </c>
+      <c r="AR23" s="23">
+        <v>73.75</v>
+      </c>
+      <c r="AS23" s="23">
+        <v>74</v>
+      </c>
+      <c r="AT23" s="23">
+        <v>73.625</v>
+      </c>
+      <c r="AU23" s="23">
+        <v>74</v>
+      </c>
+      <c r="AV23" s="23">
+        <v>72.625</v>
+      </c>
+      <c r="AW23" s="23">
+        <v>72.5</v>
+      </c>
+      <c r="AX23" s="23">
+        <v>74</v>
+      </c>
+      <c r="AY23" s="23">
+        <v>75.75</v>
+      </c>
+      <c r="AZ23" s="23">
+        <v>75.75</v>
+      </c>
+      <c r="BA23" s="23">
+        <v>78.125</v>
+      </c>
+      <c r="BB23" s="23">
+        <f t="shared" ref="BB23:BB24" si="1">MAX(B23:BA23)</f>
+        <v>78.125</v>
+      </c>
+    </row>
+    <row r="24" spans="1:103">
+      <c r="A24" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="23">
+        <v>68</v>
+      </c>
+      <c r="C24" s="23">
+        <v>70.5</v>
+      </c>
+      <c r="D24" s="23">
+        <v>71.25</v>
+      </c>
+      <c r="E24" s="23">
+        <v>70.75</v>
+      </c>
+      <c r="F24" s="23">
+        <v>70</v>
+      </c>
+      <c r="G24" s="23">
+        <v>69.75</v>
+      </c>
+      <c r="H24" s="23">
+        <v>71.25</v>
+      </c>
+      <c r="I24" s="23">
+        <v>71.5</v>
+      </c>
+      <c r="J24" s="23">
+        <v>72.125</v>
+      </c>
+      <c r="K24" s="23">
+        <v>71.5</v>
+      </c>
+      <c r="L24" s="23">
+        <v>70.25</v>
+      </c>
+      <c r="M24" s="23">
+        <v>72</v>
+      </c>
+      <c r="N24" s="23">
+        <v>72</v>
+      </c>
+      <c r="O24" s="23">
+        <v>70</v>
+      </c>
+      <c r="P24" s="23">
+        <v>71.875</v>
+      </c>
+      <c r="Q24" s="23">
+        <v>70.75</v>
+      </c>
+      <c r="R24" s="23">
+        <v>73.5</v>
+      </c>
+      <c r="S24" s="23">
+        <v>74.625</v>
+      </c>
+      <c r="T24" s="23">
+        <v>75.25</v>
+      </c>
+      <c r="U24" s="23">
+        <v>76.125</v>
+      </c>
+      <c r="V24" s="23">
+        <v>76.625</v>
+      </c>
+      <c r="W24" s="23">
+        <v>74.25</v>
+      </c>
+      <c r="X24" s="23">
+        <v>75.875</v>
+      </c>
+      <c r="Y24" s="23">
+        <v>74.625</v>
+      </c>
+      <c r="Z24" s="23">
+        <v>73.625</v>
+      </c>
+      <c r="AA24" s="23">
+        <v>72.25</v>
+      </c>
+      <c r="AB24" s="23">
+        <v>72.375</v>
+      </c>
+      <c r="AC24" s="23">
+        <v>72.75</v>
+      </c>
+      <c r="AD24" s="23">
+        <v>73.25</v>
+      </c>
+      <c r="AE24" s="23">
+        <v>71.75</v>
+      </c>
+      <c r="AF24" s="23">
+        <v>71.25</v>
+      </c>
+      <c r="AG24" s="23">
+        <v>70</v>
+      </c>
+      <c r="AH24" s="23">
+        <v>72.375</v>
+      </c>
+      <c r="AI24" s="23">
+        <v>71.875</v>
+      </c>
+      <c r="AJ24" s="23">
+        <v>71.875</v>
+      </c>
+      <c r="AK24" s="23">
+        <v>67.5</v>
+      </c>
+      <c r="AL24" s="23">
+        <v>69.875</v>
+      </c>
+      <c r="AM24" s="23">
+        <v>70</v>
+      </c>
+      <c r="AN24" s="23">
+        <v>69.375</v>
+      </c>
+      <c r="AO24" s="23">
+        <v>67.375</v>
+      </c>
+      <c r="AP24" s="23">
+        <v>67.25</v>
+      </c>
+      <c r="AQ24" s="23">
+        <v>67.625</v>
+      </c>
+      <c r="AR24" s="23">
+        <v>65.625</v>
+      </c>
+      <c r="AS24" s="23">
+        <v>69.5</v>
+      </c>
+      <c r="AT24" s="23">
+        <v>69.875</v>
+      </c>
+      <c r="AU24" s="23">
+        <v>68.75</v>
+      </c>
+      <c r="AV24" s="23">
+        <v>69.5</v>
+      </c>
+      <c r="AW24" s="23">
+        <v>68.75</v>
+      </c>
+      <c r="AX24" s="23">
+        <v>67.125</v>
+      </c>
+      <c r="AY24" s="23">
+        <v>69.125</v>
+      </c>
+      <c r="AZ24" s="23">
+        <v>68.375</v>
+      </c>
+      <c r="BA24" s="23">
+        <v>68.625</v>
+      </c>
+      <c r="BB24" s="23">
+        <f t="shared" si="1"/>
+        <v>76.625</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A7:E7"/>
     <mergeCell ref="A13:E13"/>
+    <mergeCell ref="A20:E20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Adding the results of the tests of the random classification.
</commit_message>
<xml_diff>
--- a/MasterThesis/experiments/neural.xlsx
+++ b/MasterThesis/experiments/neural.xlsx
@@ -9,14 +9,15 @@
   <sheets>
     <sheet name="класификация" sheetId="1" r:id="rId1"/>
     <sheet name="разпознаване" sheetId="2" r:id="rId2"/>
-    <sheet name="Лист1" sheetId="3" r:id="rId3"/>
+    <sheet name="експерименти" sheetId="3" r:id="rId3"/>
+    <sheet name="Лист1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="32">
   <si>
     <t>Backpropagation, 6 експеримента, 82 обучаващи, 20 верифициращи, 10000 итерации в мрежата</t>
   </si>
@@ -103,6 +104,15 @@
   </si>
   <si>
     <t>rand</t>
+  </si>
+  <si>
+    <t>Учител \ Компоненти</t>
+  </si>
+  <si>
+    <t>А</t>
+  </si>
+  <si>
+    <t>Б</t>
   </si>
 </sst>
 </file>
@@ -439,7 +449,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -723,6 +733,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -768,7 +791,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -828,6 +851,8 @@
     <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Акцент1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -1242,8 +1267,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O27"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1387,16 +1412,16 @@
       </c>
     </row>
     <row r="7" spans="1:15" ht="15.75" thickBot="1">
-      <c r="H7" s="20" t="s">
+      <c r="H7" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="I7" s="3">
+      <c r="I7" s="38">
         <v>23</v>
       </c>
-      <c r="J7" s="3">
+      <c r="J7" s="38">
         <v>79</v>
       </c>
-      <c r="K7" s="8">
+      <c r="K7" s="5">
         <v>0.77449999999999997</v>
       </c>
     </row>
@@ -1408,6 +1433,18 @@
       <c r="C8" s="33"/>
       <c r="D8" s="33"/>
       <c r="E8" s="34"/>
+      <c r="H8" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="I8" s="3">
+        <v>45</v>
+      </c>
+      <c r="J8" s="3">
+        <v>57</v>
+      </c>
+      <c r="K8" s="8">
+        <v>0.55879999999999996</v>
+      </c>
     </row>
     <row r="9" spans="1:15" ht="15.75" thickBot="1">
       <c r="A9" s="4" t="s">
@@ -1652,7 +1689,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="A2" sqref="A2:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1788,10 +1825,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:CY27"/>
+  <dimension ref="A1:CY28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39:XFD49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7001,7 +7038,7 @@
         <v>78.125</v>
       </c>
       <c r="BB26" s="23">
-        <f t="shared" ref="BB26:BB27" si="1">MAX(B26:BA26)</f>
+        <f t="shared" ref="BB26:BB28" si="1">MAX(B26:BA26)</f>
         <v>78.125</v>
       </c>
     </row>
@@ -7168,6 +7205,171 @@
       <c r="BB27" s="23">
         <f t="shared" si="1"/>
         <v>76.625</v>
+      </c>
+    </row>
+    <row r="28" spans="1:103">
+      <c r="A28" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" s="23">
+        <v>51.875</v>
+      </c>
+      <c r="C28" s="23">
+        <v>47.375</v>
+      </c>
+      <c r="D28" s="23">
+        <v>45.375</v>
+      </c>
+      <c r="E28" s="23">
+        <v>48.875</v>
+      </c>
+      <c r="F28" s="23">
+        <v>52.5</v>
+      </c>
+      <c r="G28" s="23">
+        <v>53.875</v>
+      </c>
+      <c r="H28" s="23">
+        <v>52</v>
+      </c>
+      <c r="I28" s="23">
+        <v>49.75</v>
+      </c>
+      <c r="J28" s="23">
+        <v>49.125</v>
+      </c>
+      <c r="K28" s="23">
+        <v>49.875</v>
+      </c>
+      <c r="L28" s="23">
+        <v>48.75</v>
+      </c>
+      <c r="M28" s="23">
+        <v>49.875</v>
+      </c>
+      <c r="N28" s="23">
+        <v>48.375</v>
+      </c>
+      <c r="O28" s="23">
+        <v>50.75</v>
+      </c>
+      <c r="P28" s="23">
+        <v>48</v>
+      </c>
+      <c r="Q28" s="23">
+        <v>45.375</v>
+      </c>
+      <c r="R28" s="23">
+        <v>45.75</v>
+      </c>
+      <c r="S28" s="23">
+        <v>48.125</v>
+      </c>
+      <c r="T28" s="23">
+        <v>45.625</v>
+      </c>
+      <c r="U28" s="23">
+        <v>46</v>
+      </c>
+      <c r="V28" s="23">
+        <v>45.375</v>
+      </c>
+      <c r="W28" s="23">
+        <v>48</v>
+      </c>
+      <c r="X28" s="23">
+        <v>44.125</v>
+      </c>
+      <c r="Y28" s="23">
+        <v>47.75</v>
+      </c>
+      <c r="Z28" s="23">
+        <v>43.75</v>
+      </c>
+      <c r="AA28" s="23">
+        <v>47.875</v>
+      </c>
+      <c r="AB28" s="23">
+        <v>47</v>
+      </c>
+      <c r="AC28" s="23">
+        <v>51.125</v>
+      </c>
+      <c r="AD28" s="23">
+        <v>48.625</v>
+      </c>
+      <c r="AE28" s="23">
+        <v>49.375</v>
+      </c>
+      <c r="AF28" s="23">
+        <v>48.5</v>
+      </c>
+      <c r="AG28" s="23">
+        <v>50.375</v>
+      </c>
+      <c r="AH28" s="23">
+        <v>48.875</v>
+      </c>
+      <c r="AI28" s="23">
+        <v>47</v>
+      </c>
+      <c r="AJ28" s="23">
+        <v>47.125</v>
+      </c>
+      <c r="AK28" s="23">
+        <v>44.75</v>
+      </c>
+      <c r="AL28" s="23">
+        <v>45.5</v>
+      </c>
+      <c r="AM28" s="23">
+        <v>46.5</v>
+      </c>
+      <c r="AN28" s="23">
+        <v>44.75</v>
+      </c>
+      <c r="AO28" s="23">
+        <v>44.375</v>
+      </c>
+      <c r="AP28" s="23">
+        <v>45.25</v>
+      </c>
+      <c r="AQ28" s="23">
+        <v>45.375</v>
+      </c>
+      <c r="AR28" s="23">
+        <v>46</v>
+      </c>
+      <c r="AS28" s="23">
+        <v>42.25</v>
+      </c>
+      <c r="AT28" s="23">
+        <v>40.75</v>
+      </c>
+      <c r="AU28" s="23">
+        <v>42.625</v>
+      </c>
+      <c r="AV28" s="23">
+        <v>42.625</v>
+      </c>
+      <c r="AW28" s="23">
+        <v>39.625</v>
+      </c>
+      <c r="AX28" s="23">
+        <v>42</v>
+      </c>
+      <c r="AY28" s="23">
+        <v>40.125</v>
+      </c>
+      <c r="AZ28" s="23">
+        <v>39.75</v>
+      </c>
+      <c r="BA28" s="23">
+        <v>40.625</v>
+      </c>
+      <c r="BB28" s="23">
+        <f t="shared" si="1"/>
+        <v>53.875</v>
       </c>
     </row>
   </sheetData>
@@ -7179,4 +7381,120 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J3" sqref="A1:J3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="25">
+        <v>5</v>
+      </c>
+      <c r="C1" s="25">
+        <v>10</v>
+      </c>
+      <c r="D1" s="25">
+        <v>11</v>
+      </c>
+      <c r="E1" s="25">
+        <v>20</v>
+      </c>
+      <c r="F1" s="25">
+        <v>30</v>
+      </c>
+      <c r="G1" s="25">
+        <v>40</v>
+      </c>
+      <c r="H1" s="25">
+        <v>50</v>
+      </c>
+      <c r="I1" s="25">
+        <v>60</v>
+      </c>
+      <c r="J1" s="28" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="23">
+        <v>54.88</v>
+      </c>
+      <c r="C2" s="23">
+        <v>63.38</v>
+      </c>
+      <c r="D2" s="23">
+        <v>64.25</v>
+      </c>
+      <c r="E2" s="23">
+        <v>61.75</v>
+      </c>
+      <c r="F2" s="23">
+        <v>58.38</v>
+      </c>
+      <c r="G2" s="23">
+        <v>60.66</v>
+      </c>
+      <c r="H2" s="23">
+        <v>54.5</v>
+      </c>
+      <c r="I2" s="23">
+        <v>52.25</v>
+      </c>
+      <c r="J2" s="23">
+        <f>MAX(B2:I2)</f>
+        <v>64.25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="23">
+        <v>69.13</v>
+      </c>
+      <c r="C3" s="23">
+        <v>72.5</v>
+      </c>
+      <c r="D3" s="23">
+        <v>71.5</v>
+      </c>
+      <c r="E3" s="23">
+        <v>73.13</v>
+      </c>
+      <c r="F3" s="23">
+        <v>71.16</v>
+      </c>
+      <c r="G3" s="23">
+        <v>73.5</v>
+      </c>
+      <c r="H3" s="23">
+        <v>74.16</v>
+      </c>
+      <c r="I3" s="23">
+        <v>78.16</v>
+      </c>
+      <c r="J3" s="23">
+        <f>MAX(B3:I3)</f>
+        <v>78.16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adding the naive baies classifier.
</commit_message>
<xml_diff>
--- a/MasterThesis/experiments/neural.xlsx
+++ b/MasterThesis/experiments/neural.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="47">
   <si>
     <t>Backpropagation, 6 експеримента, 82 обучаващи, 20 верифициращи, 10000 итерации в мрежата</t>
   </si>
@@ -106,13 +106,58 @@
     <t>rand</t>
   </si>
   <si>
-    <t>Учител \ Компоненти</t>
+    <t>Алгоритъм \ Компоненти</t>
   </si>
   <si>
-    <t>А</t>
+    <t>wNN</t>
   </si>
   <si>
-    <t>Б</t>
+    <t>neural net</t>
+  </si>
+  <si>
+    <t>Задача \ параметри</t>
+  </si>
+  <si>
+    <t>Клас 1</t>
+  </si>
+  <si>
+    <t>Клас 2</t>
+  </si>
+  <si>
+    <t>Разпознаване на пол</t>
+  </si>
+  <si>
+    <t>Красота според А</t>
+  </si>
+  <si>
+    <t>Красота според Б</t>
+  </si>
+  <si>
+    <t>Произволно определяне</t>
+  </si>
+  <si>
+    <t>Наивен класификатор</t>
+  </si>
+  <si>
+    <t>Разпознаване на зашумено изображение</t>
+  </si>
+  <si>
+    <t>n \ a</t>
+  </si>
+  <si>
+    <t>Classifier: Naive baies</t>
+  </si>
+  <si>
+    <t>beauty A</t>
+  </si>
+  <si>
+    <t>beauty B</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>random</t>
   </si>
 </sst>
 </file>
@@ -276,7 +321,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -448,8 +493,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="24">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -746,6 +797,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -791,7 +864,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -827,6 +900,13 @@
     <xf numFmtId="0" fontId="0" fillId="32" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="33" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="28" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -851,8 +931,6 @@
     <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Акцент1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -1268,7 +1346,7 @@
   <dimension ref="A1:O27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="H4" sqref="H4:K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1281,13 +1359,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="34"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="41"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -1332,12 +1410,12 @@
       <c r="E3" s="5">
         <v>0.75829999999999997</v>
       </c>
-      <c r="H3" s="32" t="s">
+      <c r="H3" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="33"/>
-      <c r="J3" s="33"/>
-      <c r="K3" s="34"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="40"/>
+      <c r="K3" s="41"/>
     </row>
     <row r="4" spans="1:15" ht="15.75" thickBot="1">
       <c r="A4" s="20" t="s">
@@ -1412,13 +1490,13 @@
       </c>
     </row>
     <row r="7" spans="1:15" ht="15.75" thickBot="1">
-      <c r="H7" s="37" t="s">
+      <c r="H7" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="I7" s="38">
+      <c r="I7" s="30">
         <v>23</v>
       </c>
-      <c r="J7" s="38">
+      <c r="J7" s="30">
         <v>79</v>
       </c>
       <c r="K7" s="5">
@@ -1426,13 +1504,13 @@
       </c>
     </row>
     <row r="8" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="33"/>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="34"/>
+      <c r="B8" s="40"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="41"/>
       <c r="H8" s="20" t="s">
         <v>28</v>
       </c>
@@ -1516,13 +1594,13 @@
     </row>
     <row r="14" spans="1:15" ht="15.75" thickBot="1"/>
     <row r="15" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A15" s="32" t="s">
+      <c r="A15" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="33"/>
-      <c r="C15" s="33"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="34"/>
+      <c r="B15" s="40"/>
+      <c r="C15" s="40"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="41"/>
     </row>
     <row r="16" spans="1:15" ht="15.75" thickBot="1">
       <c r="A16" s="4" t="s">
@@ -1594,13 +1672,13 @@
     </row>
     <row r="22" spans="1:5" ht="15.75" thickBot="1"/>
     <row r="23" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A23" s="29" t="s">
+      <c r="A23" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="30"/>
-      <c r="C23" s="30"/>
-      <c r="D23" s="30"/>
-      <c r="E23" s="31"/>
+      <c r="B23" s="37"/>
+      <c r="C23" s="37"/>
+      <c r="D23" s="37"/>
+      <c r="E23" s="38"/>
     </row>
     <row r="24" spans="1:5" ht="15.75" thickBot="1">
       <c r="A24" s="4" t="s">
@@ -1825,22 +1903,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:CY28"/>
+  <dimension ref="A1:CY37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+      <selection activeCell="A3" sqref="A3:A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:103">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
     </row>
     <row r="2" spans="1:103">
       <c r="A2" s="25" t="s">
@@ -2155,7 +2233,7 @@
     </row>
     <row r="3" spans="1:103">
       <c r="A3" s="20" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="B3" s="23">
         <v>54.333300000000001</v>
@@ -2467,7 +2545,7 @@
     </row>
     <row r="4" spans="1:103">
       <c r="A4" s="20" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="B4" s="23">
         <v>79.666700000000006</v>
@@ -2779,7 +2857,7 @@
     </row>
     <row r="5" spans="1:103">
       <c r="A5" s="20" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="B5" s="23">
         <v>72.333299999999994</v>
@@ -3091,7 +3169,7 @@
     </row>
     <row r="6" spans="1:103">
       <c r="A6" s="20" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="B6" s="23">
         <v>43.625</v>
@@ -3403,13 +3481,13 @@
       <c r="CY7" s="27"/>
     </row>
     <row r="8" spans="1:103">
-      <c r="A8" s="36" t="s">
+      <c r="A8" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="36"/>
-      <c r="C8" s="36"/>
-      <c r="D8" s="36"/>
-      <c r="E8" s="36"/>
+      <c r="B8" s="43"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="43"/>
       <c r="CY8" s="27"/>
     </row>
     <row r="9" spans="1:103">
@@ -3725,7 +3803,7 @@
     </row>
     <row r="10" spans="1:103">
       <c r="A10" s="20" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="B10" s="23">
         <v>56.083300000000001</v>
@@ -4037,7 +4115,7 @@
     </row>
     <row r="11" spans="1:103">
       <c r="A11" s="20" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="B11" s="23">
         <v>76.583299999999994</v>
@@ -4349,7 +4427,7 @@
     </row>
     <row r="12" spans="1:103">
       <c r="A12" s="20" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="B12" s="23">
         <v>68.5</v>
@@ -4661,7 +4739,7 @@
     </row>
     <row r="13" spans="1:103">
       <c r="A13" s="20" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="B13" s="23">
         <v>43.625</v>
@@ -4973,13 +5051,13 @@
       <c r="CY14" s="27"/>
     </row>
     <row r="15" spans="1:103">
-      <c r="A15" s="36" t="s">
+      <c r="A15" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="36"/>
-      <c r="C15" s="36"/>
-      <c r="D15" s="36"/>
-      <c r="E15" s="36"/>
+      <c r="B15" s="43"/>
+      <c r="C15" s="43"/>
+      <c r="D15" s="43"/>
+      <c r="E15" s="43"/>
       <c r="CY15" s="27"/>
     </row>
     <row r="16" spans="1:103">
@@ -5295,7 +5373,7 @@
     </row>
     <row r="17" spans="1:103">
       <c r="A17" s="20" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="B17" s="23">
         <v>48</v>
@@ -5607,7 +5685,7 @@
     </row>
     <row r="18" spans="1:103">
       <c r="A18" s="20" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="B18" s="23">
         <v>65.75</v>
@@ -5919,7 +5997,7 @@
     </row>
     <row r="19" spans="1:103">
       <c r="A19" s="20" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="B19" s="23">
         <v>49.916699999999999</v>
@@ -6231,7 +6309,7 @@
     </row>
     <row r="20" spans="1:103">
       <c r="A20" s="20" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="B20" s="23">
         <v>50</v>
@@ -6540,13 +6618,13 @@
       </c>
     </row>
     <row r="23" spans="1:103">
-      <c r="A23" s="36" t="s">
+      <c r="A23" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="36"/>
-      <c r="C23" s="36"/>
-      <c r="D23" s="36"/>
-      <c r="E23" s="36"/>
+      <c r="B23" s="43"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="43"/>
+      <c r="E23" s="43"/>
     </row>
     <row r="24" spans="1:103">
       <c r="A24" s="25" t="s">
@@ -6714,7 +6792,7 @@
     </row>
     <row r="25" spans="1:103">
       <c r="A25" s="20" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="B25" s="23">
         <v>58</v>
@@ -6879,7 +6957,7 @@
     </row>
     <row r="26" spans="1:103">
       <c r="A26" s="20" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="B26" s="23">
         <v>67.375</v>
@@ -7044,7 +7122,7 @@
     </row>
     <row r="27" spans="1:103">
       <c r="A27" s="20" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="B27" s="23">
         <v>68</v>
@@ -7209,7 +7287,7 @@
     </row>
     <row r="28" spans="1:103">
       <c r="A28" s="20" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="B28" s="23">
         <v>51.875</v>
@@ -7372,12 +7450,1566 @@
         <v>53.875</v>
       </c>
     </row>
+    <row r="32" spans="1:103">
+      <c r="A32" s="43" t="s">
+        <v>42</v>
+      </c>
+      <c r="B32" s="43"/>
+      <c r="C32" s="43"/>
+      <c r="D32" s="43"/>
+      <c r="E32" s="43"/>
+    </row>
+    <row r="33" spans="1:102">
+      <c r="A33" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="B33" s="25">
+        <v>1</v>
+      </c>
+      <c r="C33" s="25">
+        <v>2</v>
+      </c>
+      <c r="D33" s="25">
+        <v>3</v>
+      </c>
+      <c r="E33" s="25">
+        <v>4</v>
+      </c>
+      <c r="F33" s="25">
+        <v>5</v>
+      </c>
+      <c r="G33" s="25">
+        <v>6</v>
+      </c>
+      <c r="H33" s="25">
+        <v>7</v>
+      </c>
+      <c r="I33" s="25">
+        <v>8</v>
+      </c>
+      <c r="J33" s="25">
+        <v>9</v>
+      </c>
+      <c r="K33" s="25">
+        <v>10</v>
+      </c>
+      <c r="L33" s="25">
+        <v>11</v>
+      </c>
+      <c r="M33" s="25">
+        <v>12</v>
+      </c>
+      <c r="N33" s="25">
+        <v>13</v>
+      </c>
+      <c r="O33" s="25">
+        <v>14</v>
+      </c>
+      <c r="P33" s="25">
+        <v>15</v>
+      </c>
+      <c r="Q33" s="25">
+        <v>16</v>
+      </c>
+      <c r="R33" s="25">
+        <v>17</v>
+      </c>
+      <c r="S33" s="25">
+        <v>18</v>
+      </c>
+      <c r="T33" s="25">
+        <v>19</v>
+      </c>
+      <c r="U33" s="25">
+        <v>20</v>
+      </c>
+      <c r="V33" s="25">
+        <v>21</v>
+      </c>
+      <c r="W33" s="25">
+        <v>22</v>
+      </c>
+      <c r="X33" s="25">
+        <v>23</v>
+      </c>
+      <c r="Y33" s="25">
+        <v>24</v>
+      </c>
+      <c r="Z33" s="25">
+        <v>25</v>
+      </c>
+      <c r="AA33" s="25">
+        <v>26</v>
+      </c>
+      <c r="AB33" s="25">
+        <v>27</v>
+      </c>
+      <c r="AC33" s="25">
+        <v>28</v>
+      </c>
+      <c r="AD33" s="25">
+        <v>29</v>
+      </c>
+      <c r="AE33" s="25">
+        <v>30</v>
+      </c>
+      <c r="AF33" s="25">
+        <v>31</v>
+      </c>
+      <c r="AG33" s="25">
+        <v>32</v>
+      </c>
+      <c r="AH33" s="25">
+        <v>33</v>
+      </c>
+      <c r="AI33" s="25">
+        <v>34</v>
+      </c>
+      <c r="AJ33" s="25">
+        <v>35</v>
+      </c>
+      <c r="AK33" s="25">
+        <v>36</v>
+      </c>
+      <c r="AL33" s="25">
+        <v>37</v>
+      </c>
+      <c r="AM33" s="25">
+        <v>38</v>
+      </c>
+      <c r="AN33" s="25">
+        <v>39</v>
+      </c>
+      <c r="AO33" s="25">
+        <v>40</v>
+      </c>
+      <c r="AP33" s="25">
+        <v>41</v>
+      </c>
+      <c r="AQ33" s="25">
+        <v>42</v>
+      </c>
+      <c r="AR33" s="25">
+        <v>43</v>
+      </c>
+      <c r="AS33" s="25">
+        <v>44</v>
+      </c>
+      <c r="AT33" s="25">
+        <v>45</v>
+      </c>
+      <c r="AU33" s="25">
+        <v>46</v>
+      </c>
+      <c r="AV33" s="25">
+        <v>47</v>
+      </c>
+      <c r="AW33" s="25">
+        <v>48</v>
+      </c>
+      <c r="AX33" s="25">
+        <v>49</v>
+      </c>
+      <c r="AY33" s="25">
+        <v>50</v>
+      </c>
+      <c r="AZ33" s="25">
+        <v>51</v>
+      </c>
+      <c r="BA33" s="25">
+        <v>52</v>
+      </c>
+      <c r="BB33" s="25">
+        <v>53</v>
+      </c>
+      <c r="BC33" s="25">
+        <v>54</v>
+      </c>
+      <c r="BD33" s="25">
+        <v>55</v>
+      </c>
+      <c r="BE33" s="25">
+        <v>56</v>
+      </c>
+      <c r="BF33" s="25">
+        <v>57</v>
+      </c>
+      <c r="BG33" s="25">
+        <v>58</v>
+      </c>
+      <c r="BH33" s="25">
+        <v>59</v>
+      </c>
+      <c r="BI33" s="25">
+        <v>60</v>
+      </c>
+      <c r="BJ33" s="25">
+        <v>61</v>
+      </c>
+      <c r="BK33" s="25">
+        <v>62</v>
+      </c>
+      <c r="BL33" s="25">
+        <v>63</v>
+      </c>
+      <c r="BM33" s="25">
+        <v>64</v>
+      </c>
+      <c r="BN33" s="25">
+        <v>65</v>
+      </c>
+      <c r="BO33" s="25">
+        <v>66</v>
+      </c>
+      <c r="BP33" s="25">
+        <v>67</v>
+      </c>
+      <c r="BQ33" s="25">
+        <v>68</v>
+      </c>
+      <c r="BR33" s="25">
+        <v>69</v>
+      </c>
+      <c r="BS33" s="25">
+        <v>70</v>
+      </c>
+      <c r="BT33" s="25">
+        <v>71</v>
+      </c>
+      <c r="BU33" s="25">
+        <v>72</v>
+      </c>
+      <c r="BV33" s="25">
+        <v>73</v>
+      </c>
+      <c r="BW33" s="25">
+        <v>74</v>
+      </c>
+      <c r="BX33" s="25">
+        <v>75</v>
+      </c>
+      <c r="BY33" s="25">
+        <v>76</v>
+      </c>
+      <c r="BZ33" s="25">
+        <v>77</v>
+      </c>
+      <c r="CA33" s="25">
+        <v>78</v>
+      </c>
+      <c r="CB33" s="25">
+        <v>79</v>
+      </c>
+      <c r="CC33" s="25">
+        <v>80</v>
+      </c>
+      <c r="CD33" s="25">
+        <v>81</v>
+      </c>
+      <c r="CE33" s="25">
+        <v>82</v>
+      </c>
+      <c r="CF33" s="25">
+        <v>83</v>
+      </c>
+      <c r="CG33" s="25">
+        <v>84</v>
+      </c>
+      <c r="CH33" s="25">
+        <v>85</v>
+      </c>
+      <c r="CI33" s="25">
+        <v>86</v>
+      </c>
+      <c r="CJ33" s="25">
+        <v>87</v>
+      </c>
+      <c r="CK33" s="25">
+        <v>88</v>
+      </c>
+      <c r="CL33" s="25">
+        <v>89</v>
+      </c>
+      <c r="CM33" s="25">
+        <v>90</v>
+      </c>
+      <c r="CN33" s="25">
+        <v>91</v>
+      </c>
+      <c r="CO33" s="25">
+        <v>92</v>
+      </c>
+      <c r="CP33" s="25">
+        <v>93</v>
+      </c>
+      <c r="CQ33" s="25">
+        <v>94</v>
+      </c>
+      <c r="CR33" s="25">
+        <v>95</v>
+      </c>
+      <c r="CS33" s="25">
+        <v>96</v>
+      </c>
+      <c r="CT33" s="25">
+        <v>97</v>
+      </c>
+      <c r="CU33" s="25">
+        <v>98</v>
+      </c>
+      <c r="CV33" s="25">
+        <v>99</v>
+      </c>
+      <c r="CW33" s="25">
+        <v>100</v>
+      </c>
+      <c r="CX33" s="26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="34" spans="1:102">
+      <c r="A34" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="B34" s="23">
+        <v>58.25</v>
+      </c>
+      <c r="C34" s="23">
+        <v>56.875</v>
+      </c>
+      <c r="D34" s="23">
+        <v>54.625</v>
+      </c>
+      <c r="E34" s="23">
+        <v>56.5</v>
+      </c>
+      <c r="F34" s="23">
+        <v>57.25</v>
+      </c>
+      <c r="G34" s="23">
+        <v>58.25</v>
+      </c>
+      <c r="H34" s="23">
+        <v>59.875</v>
+      </c>
+      <c r="I34" s="23">
+        <v>60.875</v>
+      </c>
+      <c r="J34" s="23">
+        <v>61.75</v>
+      </c>
+      <c r="K34" s="23">
+        <v>61.125</v>
+      </c>
+      <c r="L34" s="23">
+        <v>59.625</v>
+      </c>
+      <c r="M34" s="23">
+        <v>59.75</v>
+      </c>
+      <c r="N34" s="23">
+        <v>59.125</v>
+      </c>
+      <c r="O34" s="23">
+        <v>59.25</v>
+      </c>
+      <c r="P34" s="23">
+        <v>59</v>
+      </c>
+      <c r="Q34" s="23">
+        <v>59.875</v>
+      </c>
+      <c r="R34" s="23">
+        <v>59.75</v>
+      </c>
+      <c r="S34" s="23">
+        <v>59.75</v>
+      </c>
+      <c r="T34" s="23">
+        <v>59.5</v>
+      </c>
+      <c r="U34" s="23">
+        <v>59.25</v>
+      </c>
+      <c r="V34" s="23">
+        <v>59.25</v>
+      </c>
+      <c r="W34" s="23">
+        <v>58.625</v>
+      </c>
+      <c r="X34" s="23">
+        <v>59</v>
+      </c>
+      <c r="Y34" s="23">
+        <v>59.125</v>
+      </c>
+      <c r="Z34" s="23">
+        <v>58.875</v>
+      </c>
+      <c r="AA34" s="23">
+        <v>59.25</v>
+      </c>
+      <c r="AB34" s="23">
+        <v>59.25</v>
+      </c>
+      <c r="AC34" s="23">
+        <v>59.125</v>
+      </c>
+      <c r="AD34" s="23">
+        <v>59.125</v>
+      </c>
+      <c r="AE34" s="23">
+        <v>59.125</v>
+      </c>
+      <c r="AF34" s="23">
+        <v>58.875</v>
+      </c>
+      <c r="AG34" s="23">
+        <v>59.125</v>
+      </c>
+      <c r="AH34" s="23">
+        <v>59</v>
+      </c>
+      <c r="AI34" s="23">
+        <v>58.875</v>
+      </c>
+      <c r="AJ34" s="23">
+        <v>58.875</v>
+      </c>
+      <c r="AK34" s="23">
+        <v>58.5</v>
+      </c>
+      <c r="AL34" s="23">
+        <v>59.125</v>
+      </c>
+      <c r="AM34" s="23">
+        <v>58.875</v>
+      </c>
+      <c r="AN34" s="23">
+        <v>58.875</v>
+      </c>
+      <c r="AO34" s="23">
+        <v>59</v>
+      </c>
+      <c r="AP34" s="23">
+        <v>59.25</v>
+      </c>
+      <c r="AQ34" s="23">
+        <v>59.125</v>
+      </c>
+      <c r="AR34" s="23">
+        <v>59.125</v>
+      </c>
+      <c r="AS34" s="23">
+        <v>59.25</v>
+      </c>
+      <c r="AT34" s="23">
+        <v>59.25</v>
+      </c>
+      <c r="AU34" s="23">
+        <v>59.25</v>
+      </c>
+      <c r="AV34" s="23">
+        <v>59.125</v>
+      </c>
+      <c r="AW34" s="23">
+        <v>59.125</v>
+      </c>
+      <c r="AX34" s="23">
+        <v>59</v>
+      </c>
+      <c r="AY34" s="23">
+        <v>59.125</v>
+      </c>
+      <c r="AZ34" s="23">
+        <v>59.25</v>
+      </c>
+      <c r="BA34" s="23">
+        <v>59.125</v>
+      </c>
+      <c r="BB34" s="23">
+        <v>59.25</v>
+      </c>
+      <c r="BC34" s="23">
+        <v>59.25</v>
+      </c>
+      <c r="BD34" s="23">
+        <v>59.125</v>
+      </c>
+      <c r="BE34" s="23">
+        <v>59.125</v>
+      </c>
+      <c r="BF34" s="23">
+        <v>59.125</v>
+      </c>
+      <c r="BG34" s="23">
+        <v>59.125</v>
+      </c>
+      <c r="BH34" s="23">
+        <v>59</v>
+      </c>
+      <c r="BI34" s="23">
+        <v>59</v>
+      </c>
+      <c r="BJ34" s="23">
+        <v>58.875</v>
+      </c>
+      <c r="BK34" s="23">
+        <v>58.875</v>
+      </c>
+      <c r="BL34" s="23">
+        <v>59</v>
+      </c>
+      <c r="BM34" s="23">
+        <v>58.875</v>
+      </c>
+      <c r="BN34" s="23">
+        <v>58.875</v>
+      </c>
+      <c r="BO34" s="23">
+        <v>58.875</v>
+      </c>
+      <c r="BP34" s="23">
+        <v>58.875</v>
+      </c>
+      <c r="BQ34" s="23">
+        <v>59.125</v>
+      </c>
+      <c r="BR34" s="23">
+        <v>59.125</v>
+      </c>
+      <c r="BS34" s="23">
+        <v>59.125</v>
+      </c>
+      <c r="BT34" s="23">
+        <v>59.125</v>
+      </c>
+      <c r="BU34" s="23">
+        <v>59.125</v>
+      </c>
+      <c r="BV34" s="23">
+        <v>59.125</v>
+      </c>
+      <c r="BW34" s="23">
+        <v>59.125</v>
+      </c>
+      <c r="BX34" s="23">
+        <v>59.375</v>
+      </c>
+      <c r="BY34" s="23">
+        <v>59.25</v>
+      </c>
+      <c r="BZ34" s="23">
+        <v>59.5</v>
+      </c>
+      <c r="CA34" s="23">
+        <v>59.375</v>
+      </c>
+      <c r="CB34" s="23">
+        <v>59.25</v>
+      </c>
+      <c r="CC34" s="23">
+        <v>59.25</v>
+      </c>
+      <c r="CD34" s="23">
+        <v>59.375</v>
+      </c>
+      <c r="CE34" s="23">
+        <v>59.25</v>
+      </c>
+      <c r="CF34" s="23">
+        <v>59.375</v>
+      </c>
+      <c r="CG34" s="23">
+        <v>59.375</v>
+      </c>
+      <c r="CH34" s="23">
+        <v>59.25</v>
+      </c>
+      <c r="CI34" s="23">
+        <v>59.125</v>
+      </c>
+      <c r="CJ34" s="23">
+        <v>59.375</v>
+      </c>
+      <c r="CK34" s="23">
+        <v>59.125</v>
+      </c>
+      <c r="CL34" s="23">
+        <v>59.125</v>
+      </c>
+      <c r="CM34" s="23">
+        <v>59.5</v>
+      </c>
+      <c r="CN34" s="23">
+        <v>59.375</v>
+      </c>
+      <c r="CO34" s="23">
+        <v>59.5</v>
+      </c>
+      <c r="CP34" s="23">
+        <v>59.375</v>
+      </c>
+      <c r="CQ34" s="23">
+        <v>59.25</v>
+      </c>
+      <c r="CR34" s="23">
+        <v>59.25</v>
+      </c>
+      <c r="CS34" s="23">
+        <v>59.25</v>
+      </c>
+      <c r="CT34" s="23">
+        <v>59.375</v>
+      </c>
+      <c r="CU34" s="23">
+        <v>59.375</v>
+      </c>
+      <c r="CV34" s="23">
+        <v>59.25</v>
+      </c>
+      <c r="CW34" s="23">
+        <v>59.25</v>
+      </c>
+      <c r="CX34" s="23">
+        <f t="shared" ref="CX34:CX37" si="2">MAX(A34:CW34)</f>
+        <v>61.75</v>
+      </c>
+    </row>
+    <row r="35" spans="1:102">
+      <c r="A35" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B35" s="23">
+        <v>77.375</v>
+      </c>
+      <c r="C35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="D35" s="23">
+        <v>78.25</v>
+      </c>
+      <c r="E35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="F35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="G35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="H35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="I35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="J35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="K35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="L35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="M35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="N35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="O35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="P35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="Q35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="R35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="S35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="T35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="U35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="V35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="W35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="X35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="Y35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="Z35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="AA35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="AB35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="AC35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="AD35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="AE35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="AF35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="AG35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="AH35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="AI35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="AJ35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="AK35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="AL35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="AM35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="AN35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="AO35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="AP35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="AQ35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="AR35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="AS35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="AT35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="AU35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="AV35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="AW35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="AX35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="AY35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="AZ35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="BA35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="BB35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="BC35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="BD35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="BE35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="BF35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="BG35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="BH35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="BI35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="BJ35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="BK35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="BL35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="BM35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="BN35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="BO35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="BP35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="BQ35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="BR35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="BS35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="BT35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="BU35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="BV35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="BW35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="BX35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="BY35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="BZ35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="CA35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="CB35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="CC35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="CD35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="CE35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="CF35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="CG35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="CH35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="CI35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="CJ35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="CK35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="CL35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="CM35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="CN35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="CO35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="CP35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="CQ35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="CR35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="CS35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="CT35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="CU35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="CV35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="CW35" s="23">
+        <v>78.375</v>
+      </c>
+      <c r="CX35" s="23">
+        <f t="shared" si="2"/>
+        <v>78.375</v>
+      </c>
+    </row>
+    <row r="36" spans="1:102">
+      <c r="A36" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="B36" s="23">
+        <v>72.125</v>
+      </c>
+      <c r="C36" s="23">
+        <v>73.125</v>
+      </c>
+      <c r="D36" s="23">
+        <v>75.625</v>
+      </c>
+      <c r="E36" s="23">
+        <v>77.875</v>
+      </c>
+      <c r="F36" s="23">
+        <v>77.625</v>
+      </c>
+      <c r="G36" s="23">
+        <v>75.125</v>
+      </c>
+      <c r="H36" s="23">
+        <v>73.75</v>
+      </c>
+      <c r="I36" s="23">
+        <v>73.125</v>
+      </c>
+      <c r="J36" s="23">
+        <v>72.5</v>
+      </c>
+      <c r="K36" s="23">
+        <v>69.875</v>
+      </c>
+      <c r="L36" s="23">
+        <v>69.5</v>
+      </c>
+      <c r="M36" s="23">
+        <v>69.125</v>
+      </c>
+      <c r="N36" s="23">
+        <v>68.625</v>
+      </c>
+      <c r="O36" s="23">
+        <v>68.25</v>
+      </c>
+      <c r="P36" s="23">
+        <v>67.875</v>
+      </c>
+      <c r="Q36" s="23">
+        <v>66</v>
+      </c>
+      <c r="R36" s="23">
+        <v>65.625</v>
+      </c>
+      <c r="S36" s="23">
+        <v>64.875</v>
+      </c>
+      <c r="T36" s="23">
+        <v>64.375</v>
+      </c>
+      <c r="U36" s="23">
+        <v>63.375</v>
+      </c>
+      <c r="V36" s="23">
+        <v>63.375</v>
+      </c>
+      <c r="W36" s="23">
+        <v>62.625</v>
+      </c>
+      <c r="X36" s="23">
+        <v>61.75</v>
+      </c>
+      <c r="Y36" s="23">
+        <v>62.125</v>
+      </c>
+      <c r="Z36" s="23">
+        <v>62</v>
+      </c>
+      <c r="AA36" s="23">
+        <v>61.625</v>
+      </c>
+      <c r="AB36" s="23">
+        <v>62.125</v>
+      </c>
+      <c r="AC36" s="23">
+        <v>61.875</v>
+      </c>
+      <c r="AD36" s="23">
+        <v>60.25</v>
+      </c>
+      <c r="AE36" s="23">
+        <v>60</v>
+      </c>
+      <c r="AF36" s="23">
+        <v>59.75</v>
+      </c>
+      <c r="AG36" s="23">
+        <v>59.375</v>
+      </c>
+      <c r="AH36" s="23">
+        <v>59.375</v>
+      </c>
+      <c r="AI36" s="23">
+        <v>59</v>
+      </c>
+      <c r="AJ36" s="23">
+        <v>59.125</v>
+      </c>
+      <c r="AK36" s="23">
+        <v>58.875</v>
+      </c>
+      <c r="AL36" s="23">
+        <v>59.125</v>
+      </c>
+      <c r="AM36" s="23">
+        <v>59.125</v>
+      </c>
+      <c r="AN36" s="23">
+        <v>58.75</v>
+      </c>
+      <c r="AO36" s="23">
+        <v>58.5</v>
+      </c>
+      <c r="AP36" s="23">
+        <v>58.75</v>
+      </c>
+      <c r="AQ36" s="23">
+        <v>58.5</v>
+      </c>
+      <c r="AR36" s="23">
+        <v>58.5</v>
+      </c>
+      <c r="AS36" s="23">
+        <v>58.5</v>
+      </c>
+      <c r="AT36" s="23">
+        <v>58.125</v>
+      </c>
+      <c r="AU36" s="23">
+        <v>58.25</v>
+      </c>
+      <c r="AV36" s="23">
+        <v>58.25</v>
+      </c>
+      <c r="AW36" s="23">
+        <v>58.75</v>
+      </c>
+      <c r="AX36" s="23">
+        <v>58.625</v>
+      </c>
+      <c r="AY36" s="23">
+        <v>58.625</v>
+      </c>
+      <c r="AZ36" s="23">
+        <v>58.625</v>
+      </c>
+      <c r="BA36" s="23">
+        <v>58.75</v>
+      </c>
+      <c r="BB36" s="23">
+        <v>58.875</v>
+      </c>
+      <c r="BC36" s="23">
+        <v>58.75</v>
+      </c>
+      <c r="BD36" s="23">
+        <v>58.625</v>
+      </c>
+      <c r="BE36" s="23">
+        <v>58.875</v>
+      </c>
+      <c r="BF36" s="23">
+        <v>59</v>
+      </c>
+      <c r="BG36" s="23">
+        <v>58.75</v>
+      </c>
+      <c r="BH36" s="23">
+        <v>58.875</v>
+      </c>
+      <c r="BI36" s="23">
+        <v>58.75</v>
+      </c>
+      <c r="BJ36" s="23">
+        <v>59</v>
+      </c>
+      <c r="BK36" s="23">
+        <v>58.875</v>
+      </c>
+      <c r="BL36" s="23">
+        <v>58.875</v>
+      </c>
+      <c r="BM36" s="23">
+        <v>59</v>
+      </c>
+      <c r="BN36" s="23">
+        <v>59</v>
+      </c>
+      <c r="BO36" s="23">
+        <v>59</v>
+      </c>
+      <c r="BP36" s="23">
+        <v>58.75</v>
+      </c>
+      <c r="BQ36" s="23">
+        <v>58.875</v>
+      </c>
+      <c r="BR36" s="23">
+        <v>58.875</v>
+      </c>
+      <c r="BS36" s="23">
+        <v>58.875</v>
+      </c>
+      <c r="BT36" s="23">
+        <v>58.875</v>
+      </c>
+      <c r="BU36" s="23">
+        <v>58.875</v>
+      </c>
+      <c r="BV36" s="23">
+        <v>58.875</v>
+      </c>
+      <c r="BW36" s="23">
+        <v>58.875</v>
+      </c>
+      <c r="BX36" s="23">
+        <v>58.875</v>
+      </c>
+      <c r="BY36" s="23">
+        <v>59</v>
+      </c>
+      <c r="BZ36" s="23">
+        <v>58.875</v>
+      </c>
+      <c r="CA36" s="23">
+        <v>59</v>
+      </c>
+      <c r="CB36" s="23">
+        <v>58.875</v>
+      </c>
+      <c r="CC36" s="23">
+        <v>58.875</v>
+      </c>
+      <c r="CD36" s="23">
+        <v>59.125</v>
+      </c>
+      <c r="CE36" s="23">
+        <v>59</v>
+      </c>
+      <c r="CF36" s="23">
+        <v>59</v>
+      </c>
+      <c r="CG36" s="23">
+        <v>58.875</v>
+      </c>
+      <c r="CH36" s="23">
+        <v>58.75</v>
+      </c>
+      <c r="CI36" s="23">
+        <v>59.125</v>
+      </c>
+      <c r="CJ36" s="23">
+        <v>59</v>
+      </c>
+      <c r="CK36" s="23">
+        <v>59</v>
+      </c>
+      <c r="CL36" s="23">
+        <v>59.25</v>
+      </c>
+      <c r="CM36" s="23">
+        <v>59.25</v>
+      </c>
+      <c r="CN36" s="23">
+        <v>59</v>
+      </c>
+      <c r="CO36" s="23">
+        <v>59.125</v>
+      </c>
+      <c r="CP36" s="23">
+        <v>58.75</v>
+      </c>
+      <c r="CQ36" s="23">
+        <v>58.75</v>
+      </c>
+      <c r="CR36" s="23">
+        <v>58.875</v>
+      </c>
+      <c r="CS36" s="23">
+        <v>58.75</v>
+      </c>
+      <c r="CT36" s="23">
+        <v>58.75</v>
+      </c>
+      <c r="CU36" s="23">
+        <v>58.875</v>
+      </c>
+      <c r="CV36" s="23">
+        <v>58.875</v>
+      </c>
+      <c r="CW36" s="23">
+        <v>59</v>
+      </c>
+      <c r="CX36" s="23">
+        <f t="shared" si="2"/>
+        <v>77.875</v>
+      </c>
+    </row>
+    <row r="37" spans="1:102">
+      <c r="A37" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B37" s="23">
+        <v>50.375</v>
+      </c>
+      <c r="C37" s="23">
+        <v>48.75</v>
+      </c>
+      <c r="D37" s="23">
+        <v>49.375</v>
+      </c>
+      <c r="E37" s="23">
+        <v>55.375</v>
+      </c>
+      <c r="F37" s="23">
+        <v>53.75</v>
+      </c>
+      <c r="G37" s="23">
+        <v>53.5</v>
+      </c>
+      <c r="H37" s="23">
+        <v>53.125</v>
+      </c>
+      <c r="I37" s="23">
+        <v>53.875</v>
+      </c>
+      <c r="J37" s="23">
+        <v>54.25</v>
+      </c>
+      <c r="K37" s="23">
+        <v>54</v>
+      </c>
+      <c r="L37" s="23">
+        <v>54.625</v>
+      </c>
+      <c r="M37" s="23">
+        <v>54.25</v>
+      </c>
+      <c r="N37" s="23">
+        <v>54.625</v>
+      </c>
+      <c r="O37" s="23">
+        <v>54.375</v>
+      </c>
+      <c r="P37" s="23">
+        <v>53.625</v>
+      </c>
+      <c r="Q37" s="23">
+        <v>55</v>
+      </c>
+      <c r="R37" s="23">
+        <v>53.75</v>
+      </c>
+      <c r="S37" s="23">
+        <v>53.75</v>
+      </c>
+      <c r="T37" s="23">
+        <v>54</v>
+      </c>
+      <c r="U37" s="23">
+        <v>54.5</v>
+      </c>
+      <c r="V37" s="23">
+        <v>54.125</v>
+      </c>
+      <c r="W37" s="23">
+        <v>54.375</v>
+      </c>
+      <c r="X37" s="23">
+        <v>54.875</v>
+      </c>
+      <c r="Y37" s="23">
+        <v>54.375</v>
+      </c>
+      <c r="Z37" s="23">
+        <v>54.625</v>
+      </c>
+      <c r="AA37" s="23">
+        <v>54.125</v>
+      </c>
+      <c r="AB37" s="23">
+        <v>54</v>
+      </c>
+      <c r="AC37" s="23">
+        <v>54.25</v>
+      </c>
+      <c r="AD37" s="23">
+        <v>54.125</v>
+      </c>
+      <c r="AE37" s="23">
+        <v>54.375</v>
+      </c>
+      <c r="AF37" s="23">
+        <v>54.25</v>
+      </c>
+      <c r="AG37" s="23">
+        <v>54.5</v>
+      </c>
+      <c r="AH37" s="23">
+        <v>54.75</v>
+      </c>
+      <c r="AI37" s="23">
+        <v>54.75</v>
+      </c>
+      <c r="AJ37" s="23">
+        <v>54.75</v>
+      </c>
+      <c r="AK37" s="23">
+        <v>54.75</v>
+      </c>
+      <c r="AL37" s="23">
+        <v>54.875</v>
+      </c>
+      <c r="AM37" s="23">
+        <v>55.25</v>
+      </c>
+      <c r="AN37" s="23">
+        <v>55.25</v>
+      </c>
+      <c r="AO37" s="23">
+        <v>55.25</v>
+      </c>
+      <c r="AP37" s="23">
+        <v>55.625</v>
+      </c>
+      <c r="AQ37" s="23">
+        <v>55.625</v>
+      </c>
+      <c r="AR37" s="23">
+        <v>55.75</v>
+      </c>
+      <c r="AS37" s="23">
+        <v>55.875</v>
+      </c>
+      <c r="AT37" s="23">
+        <v>56</v>
+      </c>
+      <c r="AU37" s="23">
+        <v>56.125</v>
+      </c>
+      <c r="AV37" s="23">
+        <v>56</v>
+      </c>
+      <c r="AW37" s="23">
+        <v>56.25</v>
+      </c>
+      <c r="AX37" s="23">
+        <v>56.125</v>
+      </c>
+      <c r="AY37" s="23">
+        <v>56.125</v>
+      </c>
+      <c r="AZ37" s="23">
+        <v>56.125</v>
+      </c>
+      <c r="BA37" s="23">
+        <v>56.125</v>
+      </c>
+      <c r="BB37" s="23">
+        <v>56.125</v>
+      </c>
+      <c r="BC37" s="23">
+        <v>56.125</v>
+      </c>
+      <c r="BD37" s="23">
+        <v>56.125</v>
+      </c>
+      <c r="BE37" s="23">
+        <v>56</v>
+      </c>
+      <c r="BF37" s="23">
+        <v>55.875</v>
+      </c>
+      <c r="BG37" s="23">
+        <v>56</v>
+      </c>
+      <c r="BH37" s="23">
+        <v>56</v>
+      </c>
+      <c r="BI37" s="23">
+        <v>55.75</v>
+      </c>
+      <c r="BJ37" s="23">
+        <v>55.875</v>
+      </c>
+      <c r="BK37" s="23">
+        <v>55.75</v>
+      </c>
+      <c r="BL37" s="23">
+        <v>55.75</v>
+      </c>
+      <c r="BM37" s="23">
+        <v>55.75</v>
+      </c>
+      <c r="BN37" s="23">
+        <v>55.625</v>
+      </c>
+      <c r="BO37" s="23">
+        <v>55.5</v>
+      </c>
+      <c r="BP37" s="23">
+        <v>55.875</v>
+      </c>
+      <c r="BQ37" s="23">
+        <v>55.625</v>
+      </c>
+      <c r="BR37" s="23">
+        <v>55.625</v>
+      </c>
+      <c r="BS37" s="23">
+        <v>55.875</v>
+      </c>
+      <c r="BT37" s="23">
+        <v>55.75</v>
+      </c>
+      <c r="BU37" s="23">
+        <v>56</v>
+      </c>
+      <c r="BV37" s="23">
+        <v>56.125</v>
+      </c>
+      <c r="BW37" s="23">
+        <v>56.125</v>
+      </c>
+      <c r="BX37" s="23">
+        <v>56.125</v>
+      </c>
+      <c r="BY37" s="23">
+        <v>56.25</v>
+      </c>
+      <c r="BZ37" s="23">
+        <v>56.25</v>
+      </c>
+      <c r="CA37" s="23">
+        <v>56.125</v>
+      </c>
+      <c r="CB37" s="23">
+        <v>56.125</v>
+      </c>
+      <c r="CC37" s="23">
+        <v>56.25</v>
+      </c>
+      <c r="CD37" s="23">
+        <v>56.125</v>
+      </c>
+      <c r="CE37" s="23">
+        <v>56.125</v>
+      </c>
+      <c r="CF37" s="23">
+        <v>56.25</v>
+      </c>
+      <c r="CG37" s="23">
+        <v>56.25</v>
+      </c>
+      <c r="CH37" s="23">
+        <v>55.875</v>
+      </c>
+      <c r="CI37" s="23">
+        <v>55.75</v>
+      </c>
+      <c r="CJ37" s="23">
+        <v>55.875</v>
+      </c>
+      <c r="CK37" s="23">
+        <v>56</v>
+      </c>
+      <c r="CL37" s="23">
+        <v>56</v>
+      </c>
+      <c r="CM37" s="23">
+        <v>56</v>
+      </c>
+      <c r="CN37" s="23">
+        <v>56</v>
+      </c>
+      <c r="CO37" s="23">
+        <v>56</v>
+      </c>
+      <c r="CP37" s="23">
+        <v>56</v>
+      </c>
+      <c r="CQ37" s="23">
+        <v>56</v>
+      </c>
+      <c r="CR37" s="23">
+        <v>56</v>
+      </c>
+      <c r="CS37" s="23">
+        <v>56</v>
+      </c>
+      <c r="CT37" s="23">
+        <v>56</v>
+      </c>
+      <c r="CU37" s="23">
+        <v>56</v>
+      </c>
+      <c r="CV37" s="23">
+        <v>56</v>
+      </c>
+      <c r="CW37" s="23">
+        <v>56</v>
+      </c>
+      <c r="CX37" s="23">
+        <f t="shared" si="2"/>
+        <v>56.25</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A8:E8"/>
     <mergeCell ref="A15:E15"/>
     <mergeCell ref="A23:E23"/>
+    <mergeCell ref="A32:E32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7385,10 +9017,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:BB21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J3" sqref="A1:J3"/>
+      <selection sqref="A1:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7396,105 +9028,528 @@
     <col min="1" max="1" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A2" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" s="34">
+        <v>0.01</v>
+      </c>
+      <c r="E2" s="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="2">
+        <v>57</v>
+      </c>
+      <c r="C3" s="2">
+        <v>45</v>
+      </c>
+      <c r="D3" s="5">
+        <v>0.55879999999999996</v>
+      </c>
+      <c r="E3" s="31">
+        <v>0.85750000000000004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="2">
+        <v>44</v>
+      </c>
+      <c r="C4" s="2">
+        <v>58</v>
+      </c>
+      <c r="D4" s="5">
+        <v>0.56859999999999999</v>
+      </c>
+      <c r="E4" s="5">
+        <v>0.64249999999999996</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="30">
+        <v>23</v>
+      </c>
+      <c r="C5" s="30">
+        <v>79</v>
+      </c>
+      <c r="D5" s="5">
+        <v>0.77449999999999997</v>
+      </c>
+      <c r="E5" s="5">
+        <v>0.83750000000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="3">
+        <v>45</v>
+      </c>
+      <c r="C6" s="3">
+        <v>57</v>
+      </c>
+      <c r="D6" s="8">
+        <v>0.55879999999999996</v>
+      </c>
+      <c r="E6" s="8">
+        <v>0.53879999999999995</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="25">
+      <c r="B9" s="25">
+        <v>1</v>
+      </c>
+      <c r="C9" s="25">
+        <v>4</v>
+      </c>
+      <c r="D9" s="25">
+        <v>6</v>
+      </c>
+      <c r="E9" s="25">
+        <v>10</v>
+      </c>
+      <c r="F9" s="25">
+        <v>20</v>
+      </c>
+      <c r="G9" s="25">
+        <v>40</v>
+      </c>
+      <c r="H9" s="25">
+        <v>60</v>
+      </c>
+      <c r="I9" s="26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="23">
+        <v>43.625</v>
+      </c>
+      <c r="C10" s="23">
+        <v>49.75</v>
+      </c>
+      <c r="D10" s="23">
+        <v>48.375</v>
+      </c>
+      <c r="E10" s="23">
+        <v>48.875</v>
+      </c>
+      <c r="F10" s="23">
+        <v>47.75</v>
+      </c>
+      <c r="G10" s="23">
+        <v>47.25</v>
+      </c>
+      <c r="H10" s="23">
+        <v>47.375</v>
+      </c>
+      <c r="I10" s="23">
+        <f>MAX(B10:H10)</f>
+        <v>49.75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="23">
+        <v>51.875</v>
+      </c>
+      <c r="C11" s="23">
+        <v>48.875</v>
+      </c>
+      <c r="D11" s="23">
+        <v>53.875</v>
+      </c>
+      <c r="E11" s="23">
+        <v>49.875</v>
+      </c>
+      <c r="F11" s="23">
+        <v>49.875</v>
+      </c>
+      <c r="G11" s="23">
+        <v>50.375</v>
+      </c>
+      <c r="H11" s="23">
+        <v>40.625</v>
+      </c>
+      <c r="I11" s="23">
+        <f>MAX(B11:H11)</f>
+        <v>53.875</v>
+      </c>
+    </row>
+    <row r="20" spans="1:54">
+      <c r="A20" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="25">
+        <v>1</v>
+      </c>
+      <c r="C20" s="25">
+        <v>2</v>
+      </c>
+      <c r="D20" s="25">
+        <v>3</v>
+      </c>
+      <c r="E20" s="25">
+        <v>4</v>
+      </c>
+      <c r="F20" s="25">
         <v>5</v>
       </c>
-      <c r="C1" s="25">
+      <c r="G20" s="25">
+        <v>6</v>
+      </c>
+      <c r="H20" s="25">
+        <v>7</v>
+      </c>
+      <c r="I20" s="25">
+        <v>8</v>
+      </c>
+      <c r="J20" s="25">
+        <v>9</v>
+      </c>
+      <c r="K20" s="25">
         <v>10</v>
       </c>
-      <c r="D1" s="25">
+      <c r="L20" s="25">
         <v>11</v>
       </c>
-      <c r="E1" s="25">
+      <c r="M20" s="25">
         <v>20</v>
       </c>
-      <c r="F1" s="25">
+      <c r="N20" s="25">
+        <v>21</v>
+      </c>
+      <c r="O20" s="25">
+        <v>22</v>
+      </c>
+      <c r="P20" s="25">
+        <v>23</v>
+      </c>
+      <c r="Q20" s="25">
+        <v>24</v>
+      </c>
+      <c r="R20" s="25">
+        <v>25</v>
+      </c>
+      <c r="S20" s="25">
+        <v>26</v>
+      </c>
+      <c r="T20" s="25">
+        <v>27</v>
+      </c>
+      <c r="U20" s="25">
+        <v>28</v>
+      </c>
+      <c r="V20" s="25">
+        <v>29</v>
+      </c>
+      <c r="W20" s="25">
         <v>30</v>
       </c>
-      <c r="G1" s="25">
+      <c r="X20" s="25">
+        <v>31</v>
+      </c>
+      <c r="Y20" s="25">
+        <v>32</v>
+      </c>
+      <c r="Z20" s="25">
+        <v>33</v>
+      </c>
+      <c r="AA20" s="25">
+        <v>34</v>
+      </c>
+      <c r="AB20" s="25">
+        <v>35</v>
+      </c>
+      <c r="AC20" s="25">
+        <v>36</v>
+      </c>
+      <c r="AD20" s="25">
+        <v>37</v>
+      </c>
+      <c r="AE20" s="25">
+        <v>38</v>
+      </c>
+      <c r="AF20" s="25">
+        <v>39</v>
+      </c>
+      <c r="AG20" s="25">
         <v>40</v>
       </c>
-      <c r="H1" s="25">
+      <c r="AH20" s="25">
+        <v>41</v>
+      </c>
+      <c r="AI20" s="25">
+        <v>42</v>
+      </c>
+      <c r="AJ20" s="25">
+        <v>43</v>
+      </c>
+      <c r="AK20" s="25">
+        <v>44</v>
+      </c>
+      <c r="AL20" s="25">
+        <v>45</v>
+      </c>
+      <c r="AM20" s="25">
+        <v>46</v>
+      </c>
+      <c r="AN20" s="25">
+        <v>47</v>
+      </c>
+      <c r="AO20" s="25">
+        <v>48</v>
+      </c>
+      <c r="AP20" s="25">
+        <v>49</v>
+      </c>
+      <c r="AQ20" s="25">
         <v>50</v>
       </c>
-      <c r="I1" s="25">
+      <c r="AR20" s="25">
+        <v>51</v>
+      </c>
+      <c r="AS20" s="25">
+        <v>52</v>
+      </c>
+      <c r="AT20" s="25">
+        <v>53</v>
+      </c>
+      <c r="AU20" s="25">
+        <v>54</v>
+      </c>
+      <c r="AV20" s="25">
+        <v>55</v>
+      </c>
+      <c r="AW20" s="25">
+        <v>56</v>
+      </c>
+      <c r="AX20" s="25">
+        <v>57</v>
+      </c>
+      <c r="AY20" s="25">
+        <v>58</v>
+      </c>
+      <c r="AZ20" s="25">
+        <v>59</v>
+      </c>
+      <c r="BA20" s="25">
         <v>60</v>
       </c>
-      <c r="J1" s="28" t="s">
+      <c r="BB20" s="28" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" s="23">
-        <v>54.88</v>
-      </c>
-      <c r="C2" s="23">
-        <v>63.38</v>
-      </c>
-      <c r="D2" s="23">
-        <v>64.25</v>
-      </c>
-      <c r="E2" s="23">
-        <v>61.75</v>
-      </c>
-      <c r="F2" s="23">
-        <v>58.38</v>
-      </c>
-      <c r="G2" s="23">
-        <v>60.66</v>
-      </c>
-      <c r="H2" s="23">
-        <v>54.5</v>
-      </c>
-      <c r="I2" s="23">
-        <v>52.25</v>
-      </c>
-      <c r="J2" s="23">
-        <f>MAX(B2:I2)</f>
-        <v>64.25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" s="23">
-        <v>69.13</v>
-      </c>
-      <c r="C3" s="23">
-        <v>72.5</v>
-      </c>
-      <c r="D3" s="23">
-        <v>71.5</v>
-      </c>
-      <c r="E3" s="23">
-        <v>73.13</v>
-      </c>
-      <c r="F3" s="23">
-        <v>71.16</v>
-      </c>
-      <c r="G3" s="23">
-        <v>73.5</v>
-      </c>
-      <c r="H3" s="23">
-        <v>74.16</v>
-      </c>
-      <c r="I3" s="23">
-        <v>78.16</v>
-      </c>
-      <c r="J3" s="23">
-        <f>MAX(B3:I3)</f>
-        <v>78.16</v>
+    <row r="21" spans="1:54">
+      <c r="A21" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="23">
+        <v>51.875</v>
+      </c>
+      <c r="C21" s="23">
+        <v>47.375</v>
+      </c>
+      <c r="D21" s="23">
+        <v>45.375</v>
+      </c>
+      <c r="E21" s="23">
+        <v>48.875</v>
+      </c>
+      <c r="F21" s="23">
+        <v>52.5</v>
+      </c>
+      <c r="G21" s="23">
+        <v>53.875</v>
+      </c>
+      <c r="H21" s="23">
+        <v>52</v>
+      </c>
+      <c r="I21" s="23">
+        <v>49.75</v>
+      </c>
+      <c r="J21" s="23">
+        <v>49.125</v>
+      </c>
+      <c r="K21" s="23">
+        <v>49.875</v>
+      </c>
+      <c r="L21" s="23">
+        <v>48.75</v>
+      </c>
+      <c r="M21" s="23">
+        <v>49.875</v>
+      </c>
+      <c r="N21" s="23">
+        <v>48.375</v>
+      </c>
+      <c r="O21" s="23">
+        <v>50.75</v>
+      </c>
+      <c r="P21" s="23">
+        <v>48</v>
+      </c>
+      <c r="Q21" s="23">
+        <v>45.375</v>
+      </c>
+      <c r="R21" s="23">
+        <v>45.75</v>
+      </c>
+      <c r="S21" s="23">
+        <v>48.125</v>
+      </c>
+      <c r="T21" s="23">
+        <v>45.625</v>
+      </c>
+      <c r="U21" s="23">
+        <v>46</v>
+      </c>
+      <c r="V21" s="23">
+        <v>45.375</v>
+      </c>
+      <c r="W21" s="23">
+        <v>48</v>
+      </c>
+      <c r="X21" s="23">
+        <v>44.125</v>
+      </c>
+      <c r="Y21" s="23">
+        <v>47.75</v>
+      </c>
+      <c r="Z21" s="23">
+        <v>43.75</v>
+      </c>
+      <c r="AA21" s="23">
+        <v>47.875</v>
+      </c>
+      <c r="AB21" s="23">
+        <v>47</v>
+      </c>
+      <c r="AC21" s="23">
+        <v>51.125</v>
+      </c>
+      <c r="AD21" s="23">
+        <v>48.625</v>
+      </c>
+      <c r="AE21" s="23">
+        <v>49.375</v>
+      </c>
+      <c r="AF21" s="23">
+        <v>48.5</v>
+      </c>
+      <c r="AG21" s="23">
+        <v>50.375</v>
+      </c>
+      <c r="AH21" s="23">
+        <v>48.875</v>
+      </c>
+      <c r="AI21" s="23">
+        <v>47</v>
+      </c>
+      <c r="AJ21" s="23">
+        <v>47.125</v>
+      </c>
+      <c r="AK21" s="23">
+        <v>44.75</v>
+      </c>
+      <c r="AL21" s="23">
+        <v>45.5</v>
+      </c>
+      <c r="AM21" s="23">
+        <v>46.5</v>
+      </c>
+      <c r="AN21" s="23">
+        <v>44.75</v>
+      </c>
+      <c r="AO21" s="23">
+        <v>44.375</v>
+      </c>
+      <c r="AP21" s="23">
+        <v>45.25</v>
+      </c>
+      <c r="AQ21" s="23">
+        <v>45.375</v>
+      </c>
+      <c r="AR21" s="23">
+        <v>46</v>
+      </c>
+      <c r="AS21" s="23">
+        <v>42.25</v>
+      </c>
+      <c r="AT21" s="23">
+        <v>40.75</v>
+      </c>
+      <c r="AU21" s="23">
+        <v>42.625</v>
+      </c>
+      <c r="AV21" s="23">
+        <v>42.625</v>
+      </c>
+      <c r="AW21" s="23">
+        <v>39.625</v>
+      </c>
+      <c r="AX21" s="23">
+        <v>42</v>
+      </c>
+      <c r="AY21" s="23">
+        <v>40.125</v>
+      </c>
+      <c r="AZ21" s="23">
+        <v>39.75</v>
+      </c>
+      <c r="BA21" s="23">
+        <v>40.625</v>
+      </c>
+      <c r="BB21" s="23">
+        <f t="shared" ref="BB21" si="0">MAX(B21:BA21)</f>
+        <v>53.875</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Committing improved cross validation. Adding logic for nn execution on pixel image
</commit_message>
<xml_diff>
--- a/MasterThesis/experiments/neural.xlsx
+++ b/MasterThesis/experiments/neural.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="48">
   <si>
     <t>Backpropagation, 6 експеримента, 82 обучаващи, 20 верифициращи, 10000 итерации в мрежата</t>
   </si>
@@ -158,6 +158,9 @@
   </si>
   <si>
     <t>random</t>
+  </si>
+  <si>
+    <t>Classifier: Weighted nn - new evaluation</t>
   </si>
 </sst>
 </file>
@@ -864,7 +867,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -931,6 +934,8 @@
     <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Акцент1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -1903,10 +1908,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:CY37"/>
+  <dimension ref="A1:CZ46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A6"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7459,7 +7464,7 @@
       <c r="D32" s="43"/>
       <c r="E32" s="43"/>
     </row>
-    <row r="33" spans="1:102">
+    <row r="33" spans="1:104">
       <c r="A33" s="25" t="s">
         <v>23</v>
       </c>
@@ -7767,7 +7772,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="1:102">
+    <row r="34" spans="1:104">
       <c r="A34" s="20" t="s">
         <v>43</v>
       </c>
@@ -8076,7 +8081,7 @@
         <v>61.75</v>
       </c>
     </row>
-    <row r="35" spans="1:102">
+    <row r="35" spans="1:104">
       <c r="A35" s="20" t="s">
         <v>44</v>
       </c>
@@ -8385,7 +8390,7 @@
         <v>78.375</v>
       </c>
     </row>
-    <row r="36" spans="1:102">
+    <row r="36" spans="1:104">
       <c r="A36" s="20" t="s">
         <v>45</v>
       </c>
@@ -8694,7 +8699,7 @@
         <v>77.875</v>
       </c>
     </row>
-    <row r="37" spans="1:102">
+    <row r="37" spans="1:104">
       <c r="A37" s="20" t="s">
         <v>46</v>
       </c>
@@ -9001,6 +9006,1590 @@
       <c r="CX37" s="23">
         <f t="shared" si="2"/>
         <v>56.25</v>
+      </c>
+    </row>
+    <row r="41" spans="1:104">
+      <c r="A41" s="44" t="s">
+        <v>47</v>
+      </c>
+      <c r="B41" s="44"/>
+      <c r="C41" s="44"/>
+      <c r="D41" s="45"/>
+      <c r="E41" s="45"/>
+      <c r="F41" s="45"/>
+    </row>
+    <row r="42" spans="1:104">
+      <c r="A42" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="B42" s="25">
+        <v>1</v>
+      </c>
+      <c r="C42" s="25">
+        <v>2</v>
+      </c>
+      <c r="D42" s="25">
+        <v>3</v>
+      </c>
+      <c r="E42" s="25">
+        <v>4</v>
+      </c>
+      <c r="F42" s="25">
+        <v>5</v>
+      </c>
+      <c r="G42" s="25">
+        <v>6</v>
+      </c>
+      <c r="H42" s="25">
+        <v>7</v>
+      </c>
+      <c r="I42" s="25">
+        <v>8</v>
+      </c>
+      <c r="J42" s="25">
+        <v>9</v>
+      </c>
+      <c r="K42" s="25">
+        <v>10</v>
+      </c>
+      <c r="L42" s="25">
+        <v>11</v>
+      </c>
+      <c r="M42" s="25">
+        <v>12</v>
+      </c>
+      <c r="N42" s="25">
+        <v>13</v>
+      </c>
+      <c r="O42" s="25">
+        <v>14</v>
+      </c>
+      <c r="P42" s="25">
+        <v>15</v>
+      </c>
+      <c r="Q42" s="25">
+        <v>16</v>
+      </c>
+      <c r="R42" s="25">
+        <v>17</v>
+      </c>
+      <c r="S42" s="25">
+        <v>18</v>
+      </c>
+      <c r="T42" s="25">
+        <v>19</v>
+      </c>
+      <c r="U42" s="25">
+        <v>20</v>
+      </c>
+      <c r="V42" s="25">
+        <v>21</v>
+      </c>
+      <c r="W42" s="25">
+        <v>22</v>
+      </c>
+      <c r="X42" s="25">
+        <v>23</v>
+      </c>
+      <c r="Y42" s="25">
+        <v>24</v>
+      </c>
+      <c r="Z42" s="25">
+        <v>25</v>
+      </c>
+      <c r="AA42" s="25">
+        <v>26</v>
+      </c>
+      <c r="AB42" s="25">
+        <v>27</v>
+      </c>
+      <c r="AC42" s="25">
+        <v>28</v>
+      </c>
+      <c r="AD42" s="25">
+        <v>29</v>
+      </c>
+      <c r="AE42" s="25">
+        <v>30</v>
+      </c>
+      <c r="AF42" s="25">
+        <v>31</v>
+      </c>
+      <c r="AG42" s="25">
+        <v>32</v>
+      </c>
+      <c r="AH42" s="25">
+        <v>33</v>
+      </c>
+      <c r="AI42" s="25">
+        <v>34</v>
+      </c>
+      <c r="AJ42" s="25">
+        <v>35</v>
+      </c>
+      <c r="AK42" s="25">
+        <v>36</v>
+      </c>
+      <c r="AL42" s="25">
+        <v>37</v>
+      </c>
+      <c r="AM42" s="25">
+        <v>38</v>
+      </c>
+      <c r="AN42" s="25">
+        <v>39</v>
+      </c>
+      <c r="AO42" s="25">
+        <v>40</v>
+      </c>
+      <c r="AP42" s="25">
+        <v>41</v>
+      </c>
+      <c r="AQ42" s="25">
+        <v>42</v>
+      </c>
+      <c r="AR42" s="25">
+        <v>43</v>
+      </c>
+      <c r="AS42" s="25">
+        <v>44</v>
+      </c>
+      <c r="AT42" s="25">
+        <v>45</v>
+      </c>
+      <c r="AU42" s="25">
+        <v>46</v>
+      </c>
+      <c r="AV42" s="25">
+        <v>47</v>
+      </c>
+      <c r="AW42" s="25">
+        <v>48</v>
+      </c>
+      <c r="AX42" s="25">
+        <v>49</v>
+      </c>
+      <c r="AY42" s="25">
+        <v>50</v>
+      </c>
+      <c r="AZ42" s="25">
+        <v>51</v>
+      </c>
+      <c r="BA42" s="25">
+        <v>52</v>
+      </c>
+      <c r="BB42" s="25">
+        <v>53</v>
+      </c>
+      <c r="BC42" s="25">
+        <v>54</v>
+      </c>
+      <c r="BD42" s="25">
+        <v>55</v>
+      </c>
+      <c r="BE42" s="25">
+        <v>56</v>
+      </c>
+      <c r="BF42" s="25">
+        <v>57</v>
+      </c>
+      <c r="BG42" s="25">
+        <v>58</v>
+      </c>
+      <c r="BH42" s="25">
+        <v>59</v>
+      </c>
+      <c r="BI42" s="25">
+        <v>60</v>
+      </c>
+      <c r="BJ42" s="25">
+        <v>61</v>
+      </c>
+      <c r="BK42" s="25">
+        <v>62</v>
+      </c>
+      <c r="BL42" s="25">
+        <v>63</v>
+      </c>
+      <c r="BM42" s="25">
+        <v>64</v>
+      </c>
+      <c r="BN42" s="25">
+        <v>65</v>
+      </c>
+      <c r="BO42" s="25">
+        <v>66</v>
+      </c>
+      <c r="BP42" s="25">
+        <v>67</v>
+      </c>
+      <c r="BQ42" s="25">
+        <v>68</v>
+      </c>
+      <c r="BR42" s="25">
+        <v>69</v>
+      </c>
+      <c r="BS42" s="25">
+        <v>70</v>
+      </c>
+      <c r="BT42" s="25">
+        <v>71</v>
+      </c>
+      <c r="BU42" s="25">
+        <v>72</v>
+      </c>
+      <c r="BV42" s="25">
+        <v>73</v>
+      </c>
+      <c r="BW42" s="25">
+        <v>74</v>
+      </c>
+      <c r="BX42" s="25">
+        <v>75</v>
+      </c>
+      <c r="BY42" s="25">
+        <v>76</v>
+      </c>
+      <c r="BZ42" s="25">
+        <v>77</v>
+      </c>
+      <c r="CA42" s="25">
+        <v>78</v>
+      </c>
+      <c r="CB42" s="25">
+        <v>79</v>
+      </c>
+      <c r="CC42" s="25">
+        <v>80</v>
+      </c>
+      <c r="CD42" s="25">
+        <v>81</v>
+      </c>
+      <c r="CE42" s="25">
+        <v>82</v>
+      </c>
+      <c r="CF42" s="25">
+        <v>83</v>
+      </c>
+      <c r="CG42" s="25">
+        <v>84</v>
+      </c>
+      <c r="CH42" s="25">
+        <v>85</v>
+      </c>
+      <c r="CI42" s="25">
+        <v>86</v>
+      </c>
+      <c r="CJ42" s="25">
+        <v>87</v>
+      </c>
+      <c r="CK42" s="25">
+        <v>88</v>
+      </c>
+      <c r="CL42" s="25">
+        <v>89</v>
+      </c>
+      <c r="CM42" s="25">
+        <v>90</v>
+      </c>
+      <c r="CN42" s="25">
+        <v>91</v>
+      </c>
+      <c r="CO42" s="25">
+        <v>92</v>
+      </c>
+      <c r="CP42" s="25">
+        <v>93</v>
+      </c>
+      <c r="CQ42" s="25">
+        <v>94</v>
+      </c>
+      <c r="CR42" s="25">
+        <v>95</v>
+      </c>
+      <c r="CS42" s="25">
+        <v>96</v>
+      </c>
+      <c r="CT42" s="25">
+        <v>97</v>
+      </c>
+      <c r="CU42" s="25">
+        <v>98</v>
+      </c>
+      <c r="CV42" s="25">
+        <v>99</v>
+      </c>
+      <c r="CW42" s="25">
+        <v>100</v>
+      </c>
+      <c r="CX42" s="25">
+        <v>101</v>
+      </c>
+      <c r="CY42" s="25">
+        <v>102</v>
+      </c>
+      <c r="CZ42" s="26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="43" spans="1:104">
+      <c r="A43" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="B43" s="23">
+        <v>60.833300000000001</v>
+      </c>
+      <c r="C43" s="23">
+        <v>56.416699999999999</v>
+      </c>
+      <c r="D43" s="23">
+        <v>56.666699999999999</v>
+      </c>
+      <c r="E43" s="23">
+        <v>57.083300000000001</v>
+      </c>
+      <c r="F43" s="23">
+        <v>56.583300000000001</v>
+      </c>
+      <c r="G43" s="23">
+        <v>57.416699999999999</v>
+      </c>
+      <c r="H43" s="23">
+        <v>55.583300000000001</v>
+      </c>
+      <c r="I43" s="23">
+        <v>55.583300000000001</v>
+      </c>
+      <c r="J43" s="23">
+        <v>54.75</v>
+      </c>
+      <c r="K43" s="23">
+        <v>54.5</v>
+      </c>
+      <c r="L43" s="23">
+        <v>54.666699999999999</v>
+      </c>
+      <c r="M43" s="23">
+        <v>55.416699999999999</v>
+      </c>
+      <c r="N43" s="23">
+        <v>56.083300000000001</v>
+      </c>
+      <c r="O43" s="23">
+        <v>54.75</v>
+      </c>
+      <c r="P43" s="23">
+        <v>55.666699999999999</v>
+      </c>
+      <c r="Q43" s="23">
+        <v>55.166699999999999</v>
+      </c>
+      <c r="R43" s="23">
+        <v>53.416699999999999</v>
+      </c>
+      <c r="S43" s="23">
+        <v>55.083300000000001</v>
+      </c>
+      <c r="T43" s="23">
+        <v>55.833300000000001</v>
+      </c>
+      <c r="U43" s="23">
+        <v>56.333300000000001</v>
+      </c>
+      <c r="V43" s="23">
+        <v>54.916699999999999</v>
+      </c>
+      <c r="W43" s="23">
+        <v>56.333300000000001</v>
+      </c>
+      <c r="X43" s="23">
+        <v>55.666699999999999</v>
+      </c>
+      <c r="Y43" s="23">
+        <v>54.666699999999999</v>
+      </c>
+      <c r="Z43" s="23">
+        <v>54.916699999999999</v>
+      </c>
+      <c r="AA43" s="23">
+        <v>54.416699999999999</v>
+      </c>
+      <c r="AB43" s="23">
+        <v>53.833300000000001</v>
+      </c>
+      <c r="AC43" s="23">
+        <v>55.083300000000001</v>
+      </c>
+      <c r="AD43" s="23">
+        <v>55.583300000000001</v>
+      </c>
+      <c r="AE43" s="23">
+        <v>56.25</v>
+      </c>
+      <c r="AF43" s="23">
+        <v>55.666699999999999</v>
+      </c>
+      <c r="AG43" s="23">
+        <v>54.75</v>
+      </c>
+      <c r="AH43" s="23">
+        <v>56.166699999999999</v>
+      </c>
+      <c r="AI43" s="23">
+        <v>56.166699999999999</v>
+      </c>
+      <c r="AJ43" s="23">
+        <v>55.666699999999999</v>
+      </c>
+      <c r="AK43" s="23">
+        <v>55.416699999999999</v>
+      </c>
+      <c r="AL43" s="23">
+        <v>55.25</v>
+      </c>
+      <c r="AM43" s="23">
+        <v>55.5</v>
+      </c>
+      <c r="AN43" s="23">
+        <v>56.25</v>
+      </c>
+      <c r="AO43" s="23">
+        <v>55.666699999999999</v>
+      </c>
+      <c r="AP43" s="23">
+        <v>55.333300000000001</v>
+      </c>
+      <c r="AQ43" s="23">
+        <v>55.25</v>
+      </c>
+      <c r="AR43" s="23">
+        <v>55.416699999999999</v>
+      </c>
+      <c r="AS43" s="23">
+        <v>54.75</v>
+      </c>
+      <c r="AT43" s="23">
+        <v>54.583300000000001</v>
+      </c>
+      <c r="AU43" s="23">
+        <v>55.916699999999999</v>
+      </c>
+      <c r="AV43" s="23">
+        <v>55.416699999999999</v>
+      </c>
+      <c r="AW43" s="23">
+        <v>55.916699999999999</v>
+      </c>
+      <c r="AX43" s="23">
+        <v>55.333300000000001</v>
+      </c>
+      <c r="AY43" s="23">
+        <v>55.416699999999999</v>
+      </c>
+      <c r="AZ43" s="23">
+        <v>56.166699999999999</v>
+      </c>
+      <c r="BA43" s="23">
+        <v>56.25</v>
+      </c>
+      <c r="BB43" s="23">
+        <v>55.75</v>
+      </c>
+      <c r="BC43" s="23">
+        <v>56.333300000000001</v>
+      </c>
+      <c r="BD43" s="23">
+        <v>55.916699999999999</v>
+      </c>
+      <c r="BE43" s="23">
+        <v>55.5</v>
+      </c>
+      <c r="BF43" s="23">
+        <v>55.75</v>
+      </c>
+      <c r="BG43" s="23">
+        <v>56.75</v>
+      </c>
+      <c r="BH43" s="23">
+        <v>56.166699999999999</v>
+      </c>
+      <c r="BI43" s="23">
+        <v>56.583300000000001</v>
+      </c>
+      <c r="BJ43" s="23">
+        <v>56</v>
+      </c>
+      <c r="BK43" s="23">
+        <v>55.916699999999999</v>
+      </c>
+      <c r="BL43" s="23">
+        <v>55.75</v>
+      </c>
+      <c r="BM43" s="23">
+        <v>55.5</v>
+      </c>
+      <c r="BN43" s="23">
+        <v>56.333300000000001</v>
+      </c>
+      <c r="BO43" s="23">
+        <v>55.833300000000001</v>
+      </c>
+      <c r="BP43" s="23">
+        <v>55.5</v>
+      </c>
+      <c r="BQ43" s="23">
+        <v>54.75</v>
+      </c>
+      <c r="BR43" s="23">
+        <v>55.166699999999999</v>
+      </c>
+      <c r="BS43" s="23">
+        <v>55.583300000000001</v>
+      </c>
+      <c r="BT43" s="23">
+        <v>55.416699999999999</v>
+      </c>
+      <c r="BU43" s="23">
+        <v>54.083300000000001</v>
+      </c>
+      <c r="BV43" s="23">
+        <v>54.75</v>
+      </c>
+      <c r="BW43" s="23">
+        <v>54.25</v>
+      </c>
+      <c r="BX43" s="23">
+        <v>55.25</v>
+      </c>
+      <c r="BY43" s="23">
+        <v>55.5</v>
+      </c>
+      <c r="BZ43" s="23">
+        <v>54.833300000000001</v>
+      </c>
+      <c r="CA43" s="23">
+        <v>55.083300000000001</v>
+      </c>
+      <c r="CB43" s="23">
+        <v>55.5</v>
+      </c>
+      <c r="CC43" s="23">
+        <v>55.25</v>
+      </c>
+      <c r="CD43" s="23">
+        <v>55</v>
+      </c>
+      <c r="CE43" s="23">
+        <v>54.666699999999999</v>
+      </c>
+      <c r="CF43" s="23">
+        <v>54.25</v>
+      </c>
+      <c r="CG43" s="23">
+        <v>54.75</v>
+      </c>
+      <c r="CH43" s="23">
+        <v>54.5</v>
+      </c>
+      <c r="CI43" s="23">
+        <v>54.5</v>
+      </c>
+      <c r="CJ43" s="23">
+        <v>54.833300000000001</v>
+      </c>
+      <c r="CK43" s="23">
+        <v>54.333300000000001</v>
+      </c>
+      <c r="CL43" s="23">
+        <v>54.5</v>
+      </c>
+      <c r="CM43" s="23">
+        <v>54.666699999999999</v>
+      </c>
+      <c r="CN43" s="23">
+        <v>54.5</v>
+      </c>
+      <c r="CO43" s="23">
+        <v>54.5</v>
+      </c>
+      <c r="CP43" s="23">
+        <v>54.666699999999999</v>
+      </c>
+      <c r="CQ43" s="23">
+        <v>55.166699999999999</v>
+      </c>
+      <c r="CR43" s="23">
+        <v>55.416699999999999</v>
+      </c>
+      <c r="CS43" s="23">
+        <v>54.583300000000001</v>
+      </c>
+      <c r="CT43" s="23">
+        <v>54.833300000000001</v>
+      </c>
+      <c r="CU43" s="23">
+        <v>54.416699999999999</v>
+      </c>
+      <c r="CV43" s="23">
+        <v>54.25</v>
+      </c>
+      <c r="CW43" s="23">
+        <v>54.583300000000001</v>
+      </c>
+      <c r="CX43" s="23">
+        <v>54.75</v>
+      </c>
+      <c r="CY43" s="23">
+        <v>54.75</v>
+      </c>
+      <c r="CZ43" s="23">
+        <f>MAX(B43:CY43)</f>
+        <v>60.833300000000001</v>
+      </c>
+    </row>
+    <row r="44" spans="1:104">
+      <c r="A44" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B44" s="23">
+        <v>76.416700000000006</v>
+      </c>
+      <c r="C44" s="23">
+        <v>78.583299999999994</v>
+      </c>
+      <c r="D44" s="23">
+        <v>81.5</v>
+      </c>
+      <c r="E44" s="23">
+        <v>81.833299999999994</v>
+      </c>
+      <c r="F44" s="23">
+        <v>82.666700000000006</v>
+      </c>
+      <c r="G44" s="23">
+        <v>83</v>
+      </c>
+      <c r="H44" s="23">
+        <v>82.916700000000006</v>
+      </c>
+      <c r="I44" s="23">
+        <v>82.25</v>
+      </c>
+      <c r="J44" s="23">
+        <v>82.416700000000006</v>
+      </c>
+      <c r="K44" s="23">
+        <v>82.5</v>
+      </c>
+      <c r="L44" s="23">
+        <v>82.5</v>
+      </c>
+      <c r="M44" s="23">
+        <v>82.583299999999994</v>
+      </c>
+      <c r="N44" s="23">
+        <v>82.333299999999994</v>
+      </c>
+      <c r="O44" s="23">
+        <v>82</v>
+      </c>
+      <c r="P44" s="23">
+        <v>84.166700000000006</v>
+      </c>
+      <c r="Q44" s="23">
+        <v>82.5</v>
+      </c>
+      <c r="R44" s="23">
+        <v>82.5</v>
+      </c>
+      <c r="S44" s="23">
+        <v>83.75</v>
+      </c>
+      <c r="T44" s="23">
+        <v>81.666700000000006</v>
+      </c>
+      <c r="U44" s="23">
+        <v>81.833299999999994</v>
+      </c>
+      <c r="V44" s="23">
+        <v>82.25</v>
+      </c>
+      <c r="W44" s="23">
+        <v>82.416700000000006</v>
+      </c>
+      <c r="X44" s="23">
+        <v>83.083299999999994</v>
+      </c>
+      <c r="Y44" s="23">
+        <v>82.416700000000006</v>
+      </c>
+      <c r="Z44" s="23">
+        <v>82.666700000000006</v>
+      </c>
+      <c r="AA44" s="23">
+        <v>83.25</v>
+      </c>
+      <c r="AB44" s="23">
+        <v>82.75</v>
+      </c>
+      <c r="AC44" s="23">
+        <v>83.5</v>
+      </c>
+      <c r="AD44" s="23">
+        <v>82.666700000000006</v>
+      </c>
+      <c r="AE44" s="23">
+        <v>83.75</v>
+      </c>
+      <c r="AF44" s="23">
+        <v>83.166700000000006</v>
+      </c>
+      <c r="AG44" s="23">
+        <v>83.416700000000006</v>
+      </c>
+      <c r="AH44" s="23">
+        <v>82.75</v>
+      </c>
+      <c r="AI44" s="23">
+        <v>82.25</v>
+      </c>
+      <c r="AJ44" s="23">
+        <v>81.833299999999994</v>
+      </c>
+      <c r="AK44" s="23">
+        <v>82</v>
+      </c>
+      <c r="AL44" s="23">
+        <v>83</v>
+      </c>
+      <c r="AM44" s="23">
+        <v>82</v>
+      </c>
+      <c r="AN44" s="23">
+        <v>82.083299999999994</v>
+      </c>
+      <c r="AO44" s="23">
+        <v>82.083299999999994</v>
+      </c>
+      <c r="AP44" s="23">
+        <v>82.416700000000006</v>
+      </c>
+      <c r="AQ44" s="23">
+        <v>82.416700000000006</v>
+      </c>
+      <c r="AR44" s="23">
+        <v>82.333299999999994</v>
+      </c>
+      <c r="AS44" s="23">
+        <v>82.333299999999994</v>
+      </c>
+      <c r="AT44" s="23">
+        <v>82.333299999999994</v>
+      </c>
+      <c r="AU44" s="23">
+        <v>82.583299999999994</v>
+      </c>
+      <c r="AV44" s="23">
+        <v>82.583299999999994</v>
+      </c>
+      <c r="AW44" s="23">
+        <v>82.416700000000006</v>
+      </c>
+      <c r="AX44" s="23">
+        <v>82.5</v>
+      </c>
+      <c r="AY44" s="23">
+        <v>82.166700000000006</v>
+      </c>
+      <c r="AZ44" s="23">
+        <v>81.75</v>
+      </c>
+      <c r="BA44" s="23">
+        <v>81.916700000000006</v>
+      </c>
+      <c r="BB44" s="23">
+        <v>82.416700000000006</v>
+      </c>
+      <c r="BC44" s="23">
+        <v>81.916700000000006</v>
+      </c>
+      <c r="BD44" s="23">
+        <v>82</v>
+      </c>
+      <c r="BE44" s="23">
+        <v>81.916700000000006</v>
+      </c>
+      <c r="BF44" s="23">
+        <v>81.583299999999994</v>
+      </c>
+      <c r="BG44" s="23">
+        <v>81.833299999999994</v>
+      </c>
+      <c r="BH44" s="23">
+        <v>81.416700000000006</v>
+      </c>
+      <c r="BI44" s="23">
+        <v>81.416700000000006</v>
+      </c>
+      <c r="BJ44" s="23">
+        <v>81.416700000000006</v>
+      </c>
+      <c r="BK44" s="23">
+        <v>81.5</v>
+      </c>
+      <c r="BL44" s="23">
+        <v>81.5</v>
+      </c>
+      <c r="BM44" s="23">
+        <v>81.583299999999994</v>
+      </c>
+      <c r="BN44" s="23">
+        <v>82</v>
+      </c>
+      <c r="BO44" s="23">
+        <v>81.916700000000006</v>
+      </c>
+      <c r="BP44" s="23">
+        <v>81.916700000000006</v>
+      </c>
+      <c r="BQ44" s="23">
+        <v>81.75</v>
+      </c>
+      <c r="BR44" s="23">
+        <v>82.333299999999994</v>
+      </c>
+      <c r="BS44" s="23">
+        <v>82.333299999999994</v>
+      </c>
+      <c r="BT44" s="23">
+        <v>82.25</v>
+      </c>
+      <c r="BU44" s="23">
+        <v>82.916700000000006</v>
+      </c>
+      <c r="BV44" s="23">
+        <v>82.833299999999994</v>
+      </c>
+      <c r="BW44" s="23">
+        <v>82.833299999999994</v>
+      </c>
+      <c r="BX44" s="23">
+        <v>82.583299999999994</v>
+      </c>
+      <c r="BY44" s="23">
+        <v>82.333299999999994</v>
+      </c>
+      <c r="BZ44" s="23">
+        <v>82.5</v>
+      </c>
+      <c r="CA44" s="23">
+        <v>82.416700000000006</v>
+      </c>
+      <c r="CB44" s="23">
+        <v>82.5</v>
+      </c>
+      <c r="CC44" s="23">
+        <v>82.583299999999994</v>
+      </c>
+      <c r="CD44" s="23">
+        <v>82.083299999999994</v>
+      </c>
+      <c r="CE44" s="23">
+        <v>82</v>
+      </c>
+      <c r="CF44" s="23">
+        <v>82.333299999999994</v>
+      </c>
+      <c r="CG44" s="23">
+        <v>81.916700000000006</v>
+      </c>
+      <c r="CH44" s="23">
+        <v>81.916700000000006</v>
+      </c>
+      <c r="CI44" s="23">
+        <v>81.666700000000006</v>
+      </c>
+      <c r="CJ44" s="23">
+        <v>81.25</v>
+      </c>
+      <c r="CK44" s="23">
+        <v>81.416700000000006</v>
+      </c>
+      <c r="CL44" s="23">
+        <v>81.166700000000006</v>
+      </c>
+      <c r="CM44" s="23">
+        <v>81.166700000000006</v>
+      </c>
+      <c r="CN44" s="23">
+        <v>81.083299999999994</v>
+      </c>
+      <c r="CO44" s="23">
+        <v>81.25</v>
+      </c>
+      <c r="CP44" s="23">
+        <v>81</v>
+      </c>
+      <c r="CQ44" s="23">
+        <v>81.5</v>
+      </c>
+      <c r="CR44" s="23">
+        <v>81.416700000000006</v>
+      </c>
+      <c r="CS44" s="23">
+        <v>81.5</v>
+      </c>
+      <c r="CT44" s="23">
+        <v>81.916700000000006</v>
+      </c>
+      <c r="CU44" s="23">
+        <v>82.083299999999994</v>
+      </c>
+      <c r="CV44" s="23">
+        <v>81.916700000000006</v>
+      </c>
+      <c r="CW44" s="23">
+        <v>82.25</v>
+      </c>
+      <c r="CX44" s="23">
+        <v>82.25</v>
+      </c>
+      <c r="CY44" s="23">
+        <v>82.25</v>
+      </c>
+      <c r="CZ44" s="23">
+        <f t="shared" ref="CZ44:CZ46" si="3">MAX(B44:CY44)</f>
+        <v>84.166700000000006</v>
+      </c>
+    </row>
+    <row r="45" spans="1:104">
+      <c r="A45" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="B45" s="23">
+        <v>67.583299999999994</v>
+      </c>
+      <c r="C45" s="23">
+        <v>72.5</v>
+      </c>
+      <c r="D45" s="23">
+        <v>80.083299999999994</v>
+      </c>
+      <c r="E45" s="23">
+        <v>83.666700000000006</v>
+      </c>
+      <c r="F45" s="23">
+        <v>82.916700000000006</v>
+      </c>
+      <c r="G45" s="23">
+        <v>83</v>
+      </c>
+      <c r="H45" s="23">
+        <v>83.25</v>
+      </c>
+      <c r="I45" s="23">
+        <v>82.083299999999994</v>
+      </c>
+      <c r="J45" s="23">
+        <v>83.25</v>
+      </c>
+      <c r="K45" s="23">
+        <v>83.25</v>
+      </c>
+      <c r="L45" s="23">
+        <v>83.416700000000006</v>
+      </c>
+      <c r="M45" s="23">
+        <v>83.416700000000006</v>
+      </c>
+      <c r="N45" s="23">
+        <v>83.5</v>
+      </c>
+      <c r="O45" s="23">
+        <v>83.5</v>
+      </c>
+      <c r="P45" s="23">
+        <v>83.666700000000006</v>
+      </c>
+      <c r="Q45" s="23">
+        <v>83.5</v>
+      </c>
+      <c r="R45" s="23">
+        <v>83.583299999999994</v>
+      </c>
+      <c r="S45" s="23">
+        <v>83.916700000000006</v>
+      </c>
+      <c r="T45" s="23">
+        <v>83.75</v>
+      </c>
+      <c r="U45" s="23">
+        <v>83.666700000000006</v>
+      </c>
+      <c r="V45" s="23">
+        <v>83.5</v>
+      </c>
+      <c r="W45" s="23">
+        <v>83.583299999999994</v>
+      </c>
+      <c r="X45" s="23">
+        <v>84</v>
+      </c>
+      <c r="Y45" s="23">
+        <v>83.083299999999994</v>
+      </c>
+      <c r="Z45" s="23">
+        <v>82.916700000000006</v>
+      </c>
+      <c r="AA45" s="23">
+        <v>83</v>
+      </c>
+      <c r="AB45" s="23">
+        <v>83.083299999999994</v>
+      </c>
+      <c r="AC45" s="23">
+        <v>83.75</v>
+      </c>
+      <c r="AD45" s="23">
+        <v>83.75</v>
+      </c>
+      <c r="AE45" s="23">
+        <v>83</v>
+      </c>
+      <c r="AF45" s="23">
+        <v>83</v>
+      </c>
+      <c r="AG45" s="23">
+        <v>83.666700000000006</v>
+      </c>
+      <c r="AH45" s="23">
+        <v>83.583299999999994</v>
+      </c>
+      <c r="AI45" s="23">
+        <v>83.75</v>
+      </c>
+      <c r="AJ45" s="23">
+        <v>84.083299999999994</v>
+      </c>
+      <c r="AK45" s="23">
+        <v>83.5</v>
+      </c>
+      <c r="AL45" s="23">
+        <v>83.666700000000006</v>
+      </c>
+      <c r="AM45" s="23">
+        <v>83.833299999999994</v>
+      </c>
+      <c r="AN45" s="23">
+        <v>83.75</v>
+      </c>
+      <c r="AO45" s="23">
+        <v>84</v>
+      </c>
+      <c r="AP45" s="23">
+        <v>84.833299999999994</v>
+      </c>
+      <c r="AQ45" s="23">
+        <v>84.833299999999994</v>
+      </c>
+      <c r="AR45" s="23">
+        <v>84.083299999999994</v>
+      </c>
+      <c r="AS45" s="23">
+        <v>84.416700000000006</v>
+      </c>
+      <c r="AT45" s="23">
+        <v>84.083299999999994</v>
+      </c>
+      <c r="AU45" s="23">
+        <v>84.166700000000006</v>
+      </c>
+      <c r="AV45" s="23">
+        <v>84.25</v>
+      </c>
+      <c r="AW45" s="23">
+        <v>83.833299999999994</v>
+      </c>
+      <c r="AX45" s="23">
+        <v>84</v>
+      </c>
+      <c r="AY45" s="23">
+        <v>83.916700000000006</v>
+      </c>
+      <c r="AZ45" s="23">
+        <v>83.833299999999994</v>
+      </c>
+      <c r="BA45" s="23">
+        <v>84</v>
+      </c>
+      <c r="BB45" s="23">
+        <v>83.75</v>
+      </c>
+      <c r="BC45" s="23">
+        <v>83.666700000000006</v>
+      </c>
+      <c r="BD45" s="23">
+        <v>83.75</v>
+      </c>
+      <c r="BE45" s="23">
+        <v>83.833299999999994</v>
+      </c>
+      <c r="BF45" s="23">
+        <v>83.75</v>
+      </c>
+      <c r="BG45" s="23">
+        <v>83.75</v>
+      </c>
+      <c r="BH45" s="23">
+        <v>84.083299999999994</v>
+      </c>
+      <c r="BI45" s="23">
+        <v>84.25</v>
+      </c>
+      <c r="BJ45" s="23">
+        <v>84.333299999999994</v>
+      </c>
+      <c r="BK45" s="23">
+        <v>84.083299999999994</v>
+      </c>
+      <c r="BL45" s="23">
+        <v>84.083299999999994</v>
+      </c>
+      <c r="BM45" s="23">
+        <v>83.916700000000006</v>
+      </c>
+      <c r="BN45" s="23">
+        <v>83.833299999999994</v>
+      </c>
+      <c r="BO45" s="23">
+        <v>83.75</v>
+      </c>
+      <c r="BP45" s="23">
+        <v>83.916700000000006</v>
+      </c>
+      <c r="BQ45" s="23">
+        <v>84.416700000000006</v>
+      </c>
+      <c r="BR45" s="23">
+        <v>84.416700000000006</v>
+      </c>
+      <c r="BS45" s="23">
+        <v>83.833299999999994</v>
+      </c>
+      <c r="BT45" s="23">
+        <v>83.833299999999994</v>
+      </c>
+      <c r="BU45" s="23">
+        <v>83.75</v>
+      </c>
+      <c r="BV45" s="23">
+        <v>84.25</v>
+      </c>
+      <c r="BW45" s="23">
+        <v>84.083299999999994</v>
+      </c>
+      <c r="BX45" s="23">
+        <v>83.916700000000006</v>
+      </c>
+      <c r="BY45" s="23">
+        <v>84.083299999999994</v>
+      </c>
+      <c r="BZ45" s="23">
+        <v>84.083299999999994</v>
+      </c>
+      <c r="CA45" s="23">
+        <v>83.916700000000006</v>
+      </c>
+      <c r="CB45" s="23">
+        <v>84.166700000000006</v>
+      </c>
+      <c r="CC45" s="23">
+        <v>84.083299999999994</v>
+      </c>
+      <c r="CD45" s="23">
+        <v>84.25</v>
+      </c>
+      <c r="CE45" s="23">
+        <v>84.25</v>
+      </c>
+      <c r="CF45" s="23">
+        <v>84.083299999999994</v>
+      </c>
+      <c r="CG45" s="23">
+        <v>84.083299999999994</v>
+      </c>
+      <c r="CH45" s="23">
+        <v>84</v>
+      </c>
+      <c r="CI45" s="23">
+        <v>83.75</v>
+      </c>
+      <c r="CJ45" s="23">
+        <v>84</v>
+      </c>
+      <c r="CK45" s="23">
+        <v>83.916700000000006</v>
+      </c>
+      <c r="CL45" s="23">
+        <v>84</v>
+      </c>
+      <c r="CM45" s="23">
+        <v>83.916700000000006</v>
+      </c>
+      <c r="CN45" s="23">
+        <v>84</v>
+      </c>
+      <c r="CO45" s="23">
+        <v>83.833299999999994</v>
+      </c>
+      <c r="CP45" s="23">
+        <v>83.75</v>
+      </c>
+      <c r="CQ45" s="23">
+        <v>83.75</v>
+      </c>
+      <c r="CR45" s="23">
+        <v>83.583299999999994</v>
+      </c>
+      <c r="CS45" s="23">
+        <v>83.833299999999994</v>
+      </c>
+      <c r="CT45" s="23">
+        <v>83.75</v>
+      </c>
+      <c r="CU45" s="23">
+        <v>83.75</v>
+      </c>
+      <c r="CV45" s="23">
+        <v>83.833299999999994</v>
+      </c>
+      <c r="CW45" s="23">
+        <v>83.583299999999994</v>
+      </c>
+      <c r="CX45" s="23">
+        <v>83.666700000000006</v>
+      </c>
+      <c r="CY45" s="23">
+        <v>83.666700000000006</v>
+      </c>
+      <c r="CZ45" s="23">
+        <f t="shared" si="3"/>
+        <v>84.833299999999994</v>
+      </c>
+    </row>
+    <row r="46" spans="1:104">
+      <c r="A46" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B46" s="23">
+        <v>46.5</v>
+      </c>
+      <c r="C46" s="23">
+        <v>50.166699999999999</v>
+      </c>
+      <c r="D46" s="23">
+        <v>51</v>
+      </c>
+      <c r="E46" s="23">
+        <v>49.75</v>
+      </c>
+      <c r="F46" s="23">
+        <v>48.333300000000001</v>
+      </c>
+      <c r="G46" s="23">
+        <v>49.916699999999999</v>
+      </c>
+      <c r="H46" s="23">
+        <v>48.916699999999999</v>
+      </c>
+      <c r="I46" s="23">
+        <v>50.083300000000001</v>
+      </c>
+      <c r="J46" s="23">
+        <v>49.583300000000001</v>
+      </c>
+      <c r="K46" s="23">
+        <v>48.916699999999999</v>
+      </c>
+      <c r="L46" s="23">
+        <v>49.333300000000001</v>
+      </c>
+      <c r="M46" s="23">
+        <v>49.166699999999999</v>
+      </c>
+      <c r="N46" s="23">
+        <v>49.583300000000001</v>
+      </c>
+      <c r="O46" s="23">
+        <v>49.5</v>
+      </c>
+      <c r="P46" s="23">
+        <v>49.333300000000001</v>
+      </c>
+      <c r="Q46" s="23">
+        <v>49.416699999999999</v>
+      </c>
+      <c r="R46" s="23">
+        <v>50.083300000000001</v>
+      </c>
+      <c r="S46" s="23">
+        <v>49.75</v>
+      </c>
+      <c r="T46" s="23">
+        <v>49.5</v>
+      </c>
+      <c r="U46" s="23">
+        <v>49</v>
+      </c>
+      <c r="V46" s="23">
+        <v>50.083300000000001</v>
+      </c>
+      <c r="W46" s="23">
+        <v>49.5</v>
+      </c>
+      <c r="X46" s="23">
+        <v>48.916699999999999</v>
+      </c>
+      <c r="Y46" s="23">
+        <v>48.916699999999999</v>
+      </c>
+      <c r="Z46" s="23">
+        <v>49.416699999999999</v>
+      </c>
+      <c r="AA46" s="23">
+        <v>49.5</v>
+      </c>
+      <c r="AB46" s="23">
+        <v>49.5</v>
+      </c>
+      <c r="AC46" s="23">
+        <v>50.25</v>
+      </c>
+      <c r="AD46" s="23">
+        <v>50.083300000000001</v>
+      </c>
+      <c r="AE46" s="23">
+        <v>50.75</v>
+      </c>
+      <c r="AF46" s="23">
+        <v>49.666699999999999</v>
+      </c>
+      <c r="AG46" s="23">
+        <v>49.833300000000001</v>
+      </c>
+      <c r="AH46" s="23">
+        <v>48.916699999999999</v>
+      </c>
+      <c r="AI46" s="23">
+        <v>50.833300000000001</v>
+      </c>
+      <c r="AJ46" s="23">
+        <v>50.333300000000001</v>
+      </c>
+      <c r="AK46" s="23">
+        <v>50.25</v>
+      </c>
+      <c r="AL46" s="23">
+        <v>49.5</v>
+      </c>
+      <c r="AM46" s="23">
+        <v>49.916699999999999</v>
+      </c>
+      <c r="AN46" s="23">
+        <v>49</v>
+      </c>
+      <c r="AO46" s="23">
+        <v>51.166699999999999</v>
+      </c>
+      <c r="AP46" s="23">
+        <v>50.25</v>
+      </c>
+      <c r="AQ46" s="23">
+        <v>49.75</v>
+      </c>
+      <c r="AR46" s="23">
+        <v>50.75</v>
+      </c>
+      <c r="AS46" s="23">
+        <v>50.916699999999999</v>
+      </c>
+      <c r="AT46" s="23">
+        <v>50.666699999999999</v>
+      </c>
+      <c r="AU46" s="23">
+        <v>50.5</v>
+      </c>
+      <c r="AV46" s="23">
+        <v>51.083300000000001</v>
+      </c>
+      <c r="AW46" s="23">
+        <v>50</v>
+      </c>
+      <c r="AX46" s="23">
+        <v>50.75</v>
+      </c>
+      <c r="AY46" s="23">
+        <v>50.166699999999999</v>
+      </c>
+      <c r="AZ46" s="23">
+        <v>50.25</v>
+      </c>
+      <c r="BA46" s="23">
+        <v>50.25</v>
+      </c>
+      <c r="BB46" s="23">
+        <v>49.333300000000001</v>
+      </c>
+      <c r="BC46" s="23">
+        <v>49.416699999999999</v>
+      </c>
+      <c r="BD46" s="23">
+        <v>50.166699999999999</v>
+      </c>
+      <c r="BE46" s="23">
+        <v>50</v>
+      </c>
+      <c r="BF46" s="23">
+        <v>50.333300000000001</v>
+      </c>
+      <c r="BG46" s="23">
+        <v>50.166699999999999</v>
+      </c>
+      <c r="BH46" s="23">
+        <v>50.75</v>
+      </c>
+      <c r="BI46" s="23">
+        <v>50.833300000000001</v>
+      </c>
+      <c r="BJ46" s="23">
+        <v>49.833300000000001</v>
+      </c>
+      <c r="BK46" s="23">
+        <v>49.333300000000001</v>
+      </c>
+      <c r="BL46" s="23">
+        <v>49.583300000000001</v>
+      </c>
+      <c r="BM46" s="23">
+        <v>50.166699999999999</v>
+      </c>
+      <c r="BN46" s="23">
+        <v>50</v>
+      </c>
+      <c r="BO46" s="23">
+        <v>49.916699999999999</v>
+      </c>
+      <c r="BP46" s="23">
+        <v>50</v>
+      </c>
+      <c r="BQ46" s="23">
+        <v>49.25</v>
+      </c>
+      <c r="BR46" s="23">
+        <v>49.166699999999999</v>
+      </c>
+      <c r="BS46" s="23">
+        <v>49.416699999999999</v>
+      </c>
+      <c r="BT46" s="23">
+        <v>49.583300000000001</v>
+      </c>
+      <c r="BU46" s="23">
+        <v>50.083300000000001</v>
+      </c>
+      <c r="BV46" s="23">
+        <v>50.166699999999999</v>
+      </c>
+      <c r="BW46" s="23">
+        <v>49.583300000000001</v>
+      </c>
+      <c r="BX46" s="23">
+        <v>50.333300000000001</v>
+      </c>
+      <c r="BY46" s="23">
+        <v>50.25</v>
+      </c>
+      <c r="BZ46" s="23">
+        <v>50.416699999999999</v>
+      </c>
+      <c r="CA46" s="23">
+        <v>50.25</v>
+      </c>
+      <c r="CB46" s="23">
+        <v>49.416699999999999</v>
+      </c>
+      <c r="CC46" s="23">
+        <v>50.083300000000001</v>
+      </c>
+      <c r="CD46" s="23">
+        <v>49.25</v>
+      </c>
+      <c r="CE46" s="23">
+        <v>49</v>
+      </c>
+      <c r="CF46" s="23">
+        <v>48.75</v>
+      </c>
+      <c r="CG46" s="23">
+        <v>49.75</v>
+      </c>
+      <c r="CH46" s="23">
+        <v>49.916699999999999</v>
+      </c>
+      <c r="CI46" s="23">
+        <v>49.666699999999999</v>
+      </c>
+      <c r="CJ46" s="23">
+        <v>49.583300000000001</v>
+      </c>
+      <c r="CK46" s="23">
+        <v>49.916699999999999</v>
+      </c>
+      <c r="CL46" s="23">
+        <v>49.833300000000001</v>
+      </c>
+      <c r="CM46" s="23">
+        <v>50.333300000000001</v>
+      </c>
+      <c r="CN46" s="23">
+        <v>50.333300000000001</v>
+      </c>
+      <c r="CO46" s="23">
+        <v>50.333300000000001</v>
+      </c>
+      <c r="CP46" s="23">
+        <v>50.833300000000001</v>
+      </c>
+      <c r="CQ46" s="23">
+        <v>50</v>
+      </c>
+      <c r="CR46" s="23">
+        <v>50.25</v>
+      </c>
+      <c r="CS46" s="23">
+        <v>50.083300000000001</v>
+      </c>
+      <c r="CT46" s="23">
+        <v>49.916699999999999</v>
+      </c>
+      <c r="CU46" s="23">
+        <v>49.75</v>
+      </c>
+      <c r="CV46" s="23">
+        <v>49.5</v>
+      </c>
+      <c r="CW46" s="23">
+        <v>49.583300000000001</v>
+      </c>
+      <c r="CX46" s="23">
+        <v>49.583300000000001</v>
+      </c>
+      <c r="CY46" s="23">
+        <v>49.583300000000001</v>
+      </c>
+      <c r="CZ46" s="23">
+        <f t="shared" si="3"/>
+        <v>51.166699999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding code for comparison of algorithms using hypothesis. Adding scree plot.
</commit_message>
<xml_diff>
--- a/MasterThesis/experiments/neural.xlsx
+++ b/MasterThesis/experiments/neural.xlsx
@@ -11,13 +11,14 @@
     <sheet name="разпознаване" sheetId="2" r:id="rId2"/>
     <sheet name="експерименти" sheetId="3" r:id="rId3"/>
     <sheet name="Лист1" sheetId="4" r:id="rId4"/>
+    <sheet name="Лист2" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="54">
   <si>
     <t>Backpropagation, 6 експеримента, 82 обучаващи, 20 верифициращи, 10000 итерации в мрежата</t>
   </si>
@@ -161,6 +162,24 @@
   </si>
   <si>
     <t>Classifier: Weighted nn - new evaluation</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Number:</t>
+  </si>
+  <si>
+    <t>Alg 1</t>
+  </si>
+  <si>
+    <t>Alg 2</t>
+  </si>
+  <si>
+    <t>Delta</t>
+  </si>
+  <si>
+    <t>sD</t>
   </si>
 </sst>
 </file>
@@ -324,7 +343,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -502,8 +521,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="26">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -822,6 +865,68 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -867,7 +972,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -910,6 +1015,8 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="33" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="28" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -934,8 +1041,20 @@
     <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Акцент1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -1364,13 +1483,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="41"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="43"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -1415,12 +1534,12 @@
       <c r="E3" s="5">
         <v>0.75829999999999997</v>
       </c>
-      <c r="H3" s="39" t="s">
+      <c r="H3" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="40"/>
-      <c r="J3" s="40"/>
-      <c r="K3" s="41"/>
+      <c r="I3" s="42"/>
+      <c r="J3" s="42"/>
+      <c r="K3" s="43"/>
     </row>
     <row r="4" spans="1:15" ht="15.75" thickBot="1">
       <c r="A4" s="20" t="s">
@@ -1509,13 +1628,13 @@
       </c>
     </row>
     <row r="8" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="40"/>
-      <c r="C8" s="40"/>
-      <c r="D8" s="40"/>
-      <c r="E8" s="41"/>
+      <c r="B8" s="42"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="43"/>
       <c r="H8" s="20" t="s">
         <v>28</v>
       </c>
@@ -1599,13 +1718,13 @@
     </row>
     <row r="14" spans="1:15" ht="15.75" thickBot="1"/>
     <row r="15" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A15" s="39" t="s">
+      <c r="A15" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="40"/>
-      <c r="C15" s="40"/>
-      <c r="D15" s="40"/>
-      <c r="E15" s="41"/>
+      <c r="B15" s="42"/>
+      <c r="C15" s="42"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="43"/>
     </row>
     <row r="16" spans="1:15" ht="15.75" thickBot="1">
       <c r="A16" s="4" t="s">
@@ -1677,13 +1796,13 @@
     </row>
     <row r="22" spans="1:5" ht="15.75" thickBot="1"/>
     <row r="23" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A23" s="36" t="s">
+      <c r="A23" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="37"/>
-      <c r="C23" s="37"/>
-      <c r="D23" s="37"/>
-      <c r="E23" s="38"/>
+      <c r="B23" s="39"/>
+      <c r="C23" s="39"/>
+      <c r="D23" s="39"/>
+      <c r="E23" s="40"/>
     </row>
     <row r="24" spans="1:5" ht="15.75" thickBot="1">
       <c r="A24" s="4" t="s">
@@ -1910,20 +2029,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:CZ46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="H39" sqref="H39"/>
+    <sheetView tabSelected="1" topLeftCell="AM19" workbookViewId="0">
+      <selection activeCell="P42" sqref="P42:P44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:103">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
     </row>
     <row r="2" spans="1:103">
       <c r="A2" s="25" t="s">
@@ -3486,13 +3605,13 @@
       <c r="CY7" s="27"/>
     </row>
     <row r="8" spans="1:103">
-      <c r="A8" s="43" t="s">
+      <c r="A8" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="43"/>
-      <c r="C8" s="43"/>
-      <c r="D8" s="43"/>
-      <c r="E8" s="43"/>
+      <c r="B8" s="45"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
       <c r="CY8" s="27"/>
     </row>
     <row r="9" spans="1:103">
@@ -5056,13 +5175,13 @@
       <c r="CY14" s="27"/>
     </row>
     <row r="15" spans="1:103">
-      <c r="A15" s="43" t="s">
+      <c r="A15" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="43"/>
-      <c r="C15" s="43"/>
-      <c r="D15" s="43"/>
-      <c r="E15" s="43"/>
+      <c r="B15" s="45"/>
+      <c r="C15" s="45"/>
+      <c r="D15" s="45"/>
+      <c r="E15" s="45"/>
       <c r="CY15" s="27"/>
     </row>
     <row r="16" spans="1:103">
@@ -6623,13 +6742,13 @@
       </c>
     </row>
     <row r="23" spans="1:103">
-      <c r="A23" s="43" t="s">
+      <c r="A23" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="43"/>
-      <c r="C23" s="43"/>
-      <c r="D23" s="43"/>
-      <c r="E23" s="43"/>
+      <c r="B23" s="45"/>
+      <c r="C23" s="45"/>
+      <c r="D23" s="45"/>
+      <c r="E23" s="45"/>
     </row>
     <row r="24" spans="1:103">
       <c r="A24" s="25" t="s">
@@ -7456,13 +7575,13 @@
       </c>
     </row>
     <row r="32" spans="1:103">
-      <c r="A32" s="43" t="s">
+      <c r="A32" s="45" t="s">
         <v>42</v>
       </c>
-      <c r="B32" s="43"/>
-      <c r="C32" s="43"/>
-      <c r="D32" s="43"/>
-      <c r="E32" s="43"/>
+      <c r="B32" s="45"/>
+      <c r="C32" s="45"/>
+      <c r="D32" s="45"/>
+      <c r="E32" s="45"/>
     </row>
     <row r="33" spans="1:104">
       <c r="A33" s="25" t="s">
@@ -9009,14 +9128,14 @@
       </c>
     </row>
     <row r="41" spans="1:104">
-      <c r="A41" s="44" t="s">
+      <c r="A41" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="B41" s="44"/>
-      <c r="C41" s="44"/>
-      <c r="D41" s="45"/>
-      <c r="E41" s="45"/>
-      <c r="F41" s="45"/>
+      <c r="B41" s="36"/>
+      <c r="C41" s="36"/>
+      <c r="D41" s="37"/>
+      <c r="E41" s="37"/>
+      <c r="F41" s="37"/>
     </row>
     <row r="42" spans="1:104">
       <c r="A42" s="25" t="s">
@@ -11141,4 +11260,444 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A2:E24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="2" spans="1:5">
+      <c r="A2" s="23"/>
+      <c r="B2" s="46" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="46" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="46" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" s="46" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="46">
+        <v>1</v>
+      </c>
+      <c r="B3" s="50">
+        <v>0.6</v>
+      </c>
+      <c r="C3" s="51">
+        <v>0.66666669999999995</v>
+      </c>
+      <c r="D3" s="57">
+        <f>C3-B3</f>
+        <v>6.6666699999999968E-2</v>
+      </c>
+      <c r="E3" s="54">
+        <f>($D$23 - D3) * ($D$23 - D3)</f>
+        <v>2.7776388906250164E-6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="46">
+        <v>1</v>
+      </c>
+      <c r="B4" s="30">
+        <v>0.6</v>
+      </c>
+      <c r="C4" s="27">
+        <v>0.43333329999999998</v>
+      </c>
+      <c r="D4" s="58">
+        <f t="shared" ref="D4:D22" si="0">C4-B4</f>
+        <v>-0.1666667</v>
+      </c>
+      <c r="E4" s="55">
+        <f>($D$23 - D4) * ($D$23 - D4)</f>
+        <v>5.5225011750000615E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="46">
+        <v>1</v>
+      </c>
+      <c r="B5" s="30">
+        <v>0.6</v>
+      </c>
+      <c r="C5" s="27">
+        <v>0.7</v>
+      </c>
+      <c r="D5" s="58">
+        <f t="shared" si="0"/>
+        <v>9.9999999999999978E-2</v>
+      </c>
+      <c r="E5" s="55">
+        <f>($D$23 - D5) * ($D$23 - D5)</f>
+        <v>1.0027783055556252E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="46">
+        <v>1</v>
+      </c>
+      <c r="B6" s="30">
+        <v>0.56666669999999997</v>
+      </c>
+      <c r="C6" s="27">
+        <v>0.46666669999999999</v>
+      </c>
+      <c r="D6" s="58">
+        <f t="shared" si="0"/>
+        <v>-9.9999999999999978E-2</v>
+      </c>
+      <c r="E6" s="55">
+        <f>($D$23 - D6) * ($D$23 - D6)</f>
+        <v>2.8336108305555607E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="46">
+        <v>1</v>
+      </c>
+      <c r="B7" s="30">
+        <v>0.6</v>
+      </c>
+      <c r="C7" s="27">
+        <v>0.66666669999999995</v>
+      </c>
+      <c r="D7" s="58">
+        <f t="shared" si="0"/>
+        <v>6.6666699999999968E-2</v>
+      </c>
+      <c r="E7" s="55">
+        <f>($D$23 - D7) * ($D$23 - D7)</f>
+        <v>2.7776388906250164E-6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="46">
+        <v>1</v>
+      </c>
+      <c r="B8" s="30">
+        <v>0.4</v>
+      </c>
+      <c r="C8" s="27">
+        <v>0.6</v>
+      </c>
+      <c r="D8" s="58">
+        <f t="shared" si="0"/>
+        <v>0.19999999999999996</v>
+      </c>
+      <c r="E8" s="55">
+        <f>($D$23 - D8) * ($D$23 - D8)</f>
+        <v>1.7336113305555619E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="46">
+        <v>1</v>
+      </c>
+      <c r="B9" s="30">
+        <v>0.53333330000000001</v>
+      </c>
+      <c r="C9" s="27">
+        <v>0.56666669999999997</v>
+      </c>
+      <c r="D9" s="58">
+        <f t="shared" si="0"/>
+        <v>3.3333399999999958E-2</v>
+      </c>
+      <c r="E9" s="55">
+        <f>($D$23 - D9) * ($D$23 - D9)</f>
+        <v>1.224994750005626E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="46">
+        <v>1</v>
+      </c>
+      <c r="B10" s="30">
+        <v>0.46666669999999999</v>
+      </c>
+      <c r="C10" s="27">
+        <v>0.63333329999999999</v>
+      </c>
+      <c r="D10" s="58">
+        <f t="shared" si="0"/>
+        <v>0.1666666</v>
+      </c>
+      <c r="E10" s="55">
+        <f>($D$23 - D10) * ($D$23 - D10)</f>
+        <v>9.6694329722256302E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="46">
+        <v>1</v>
+      </c>
+      <c r="B11" s="30">
+        <v>0.43333329999999998</v>
+      </c>
+      <c r="C11" s="27">
+        <v>0.63333329999999999</v>
+      </c>
+      <c r="D11" s="58">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="E11" s="55">
+        <f>($D$23 - D11) * ($D$23 - D11)</f>
+        <v>1.7336113305555637E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="46">
+        <v>1</v>
+      </c>
+      <c r="B12" s="30">
+        <v>0.66666669999999995</v>
+      </c>
+      <c r="C12" s="27">
+        <v>0.73333329999999997</v>
+      </c>
+      <c r="D12" s="58">
+        <f t="shared" si="0"/>
+        <v>6.666660000000002E-2</v>
+      </c>
+      <c r="E12" s="55">
+        <f>($D$23 - D12) * ($D$23 - D12)</f>
+        <v>2.7779722256248408E-6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="46">
+        <v>1</v>
+      </c>
+      <c r="B13" s="30">
+        <v>0.5</v>
+      </c>
+      <c r="C13" s="27">
+        <v>0.73333329999999997</v>
+      </c>
+      <c r="D13" s="58">
+        <f t="shared" si="0"/>
+        <v>0.23333329999999997</v>
+      </c>
+      <c r="E13" s="55">
+        <f>($D$23 - D13) * ($D$23 - D13)</f>
+        <v>2.7224991750000621E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="46">
+        <v>1</v>
+      </c>
+      <c r="B14" s="30">
+        <v>0.46666669999999999</v>
+      </c>
+      <c r="C14" s="27">
+        <v>0.53333330000000001</v>
+      </c>
+      <c r="D14" s="58">
+        <f t="shared" si="0"/>
+        <v>6.666660000000002E-2</v>
+      </c>
+      <c r="E14" s="55">
+        <f>($D$23 - D14) * ($D$23 - D14)</f>
+        <v>2.7779722256248408E-6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="46">
+        <v>1</v>
+      </c>
+      <c r="B15" s="30">
+        <v>0.4</v>
+      </c>
+      <c r="C15" s="27">
+        <v>0.6</v>
+      </c>
+      <c r="D15" s="58">
+        <f t="shared" si="0"/>
+        <v>0.19999999999999996</v>
+      </c>
+      <c r="E15" s="55">
+        <f>($D$23 - D15) * ($D$23 - D15)</f>
+        <v>1.7336113305555619E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="46">
+        <v>1</v>
+      </c>
+      <c r="B16" s="30">
+        <v>0.56666669999999997</v>
+      </c>
+      <c r="C16" s="27">
+        <v>0.63333329999999999</v>
+      </c>
+      <c r="D16" s="58">
+        <f t="shared" si="0"/>
+        <v>6.666660000000002E-2</v>
+      </c>
+      <c r="E16" s="55">
+        <f>($D$23 - D16) * ($D$23 - D16)</f>
+        <v>2.7779722256248408E-6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="46">
+        <v>1</v>
+      </c>
+      <c r="B17" s="30">
+        <v>0.63333329999999999</v>
+      </c>
+      <c r="C17" s="27">
+        <v>0.5</v>
+      </c>
+      <c r="D17" s="58">
+        <f t="shared" si="0"/>
+        <v>-0.13333329999999999</v>
+      </c>
+      <c r="E17" s="55">
+        <f>($D$23 - D17) * ($D$23 - D17)</f>
+        <v>4.0669427638890608E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="46">
+        <v>1</v>
+      </c>
+      <c r="B18" s="30">
+        <v>0.56666669999999997</v>
+      </c>
+      <c r="C18" s="27">
+        <v>0.66666669999999995</v>
+      </c>
+      <c r="D18" s="58">
+        <f t="shared" si="0"/>
+        <v>9.9999999999999978E-2</v>
+      </c>
+      <c r="E18" s="55">
+        <f>($D$23 - D18) * ($D$23 - D18)</f>
+        <v>1.0027783055556252E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="46">
+        <v>1</v>
+      </c>
+      <c r="B19" s="30">
+        <v>0.36666670000000001</v>
+      </c>
+      <c r="C19" s="27">
+        <v>0.5</v>
+      </c>
+      <c r="D19" s="58">
+        <f t="shared" si="0"/>
+        <v>0.13333329999999999</v>
+      </c>
+      <c r="E19" s="55">
+        <f>($D$23 - D19) * ($D$23 - D19)</f>
+        <v>4.2249967500006267E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="46">
+        <v>1</v>
+      </c>
+      <c r="B20" s="30">
+        <v>0.6</v>
+      </c>
+      <c r="C20" s="27">
+        <v>0.6</v>
+      </c>
+      <c r="D20" s="58">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E20" s="55">
+        <f>($D$23 - D20) * ($D$23 - D20)</f>
+        <v>4.6694433055556213E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="46">
+        <v>1</v>
+      </c>
+      <c r="B21" s="30">
+        <v>0.6</v>
+      </c>
+      <c r="C21" s="27">
+        <v>0.56666669999999997</v>
+      </c>
+      <c r="D21" s="58">
+        <f t="shared" si="0"/>
+        <v>-3.333330000000001E-2</v>
+      </c>
+      <c r="E21" s="55">
+        <f>($D$23 - D21) * ($D$23 - D21)</f>
+        <v>1.0336102638890621E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="46">
+        <v>1</v>
+      </c>
+      <c r="B22" s="52">
+        <v>0.56666669999999997</v>
+      </c>
+      <c r="C22" s="53">
+        <v>0.66666669999999995</v>
+      </c>
+      <c r="D22" s="59">
+        <f t="shared" si="0"/>
+        <v>9.9999999999999978E-2</v>
+      </c>
+      <c r="E22" s="56">
+        <f>($D$23 - D22) * ($D$23 - D22)</f>
+        <v>1.0027783055556252E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="47" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" s="48">
+        <f t="shared" ref="B23:C23" si="1">AVERAGE(B3:B22)</f>
+        <v>0.53666667499999998</v>
+      </c>
+      <c r="C23" s="48">
+        <f t="shared" si="1"/>
+        <v>0.60500000000000009</v>
+      </c>
+      <c r="D23" s="48">
+        <f>AVERAGE(D3:D22)</f>
+        <v>6.8333324999999973E-2</v>
+      </c>
+      <c r="E23" s="48">
+        <f>SUM(E3:E22)/(COUNT(E3:E22) *(COUNT(E3:E22)  - 1))</f>
+        <v>6.2266072076030911E-4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="D24" t="s">
+        <v>49</v>
+      </c>
+      <c r="E24" s="49">
+        <f>$D$23/SQRT($E$23)</f>
+        <v>2.7384626273703292</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Making the recognizer to compare with nn before the PCA transformation.
</commit_message>
<xml_diff>
--- a/MasterThesis/experiments/neural.xlsx
+++ b/MasterThesis/experiments/neural.xlsx
@@ -14,11 +14,12 @@
     <sheet name="Лист2" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="66">
   <si>
     <t>Backpropagation, 6 експеримента, 82 обучаващи, 20 верифициращи, 10000 итерации в мрежата</t>
   </si>
@@ -180,6 +181,42 @@
   </si>
   <si>
     <t>sD</t>
+  </si>
+  <si>
+    <t>Classifier: Neural network - new evaluation</t>
+  </si>
+  <si>
+    <t>пол</t>
+  </si>
+  <si>
+    <t>красота А</t>
+  </si>
+  <si>
+    <t>красота Б</t>
+  </si>
+  <si>
+    <t>произволен</t>
+  </si>
+  <si>
+    <t>класификатор \ характеристики</t>
+  </si>
+  <si>
+    <t>АГК грешка</t>
+  </si>
+  <si>
+    <t>Начална прецизност</t>
+  </si>
+  <si>
+    <t>АГК прецизност</t>
+  </si>
+  <si>
+    <t>Начална грешка</t>
+  </si>
+  <si>
+    <t>Глобално подобрение</t>
+  </si>
+  <si>
+    <t>Процентно подобрение</t>
   </si>
 </sst>
 </file>
@@ -972,7 +1009,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1017,6 +1054,20 @@
     <xf numFmtId="9" fontId="0" fillId="33" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="28" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="28" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1041,20 +1092,10 @@
     <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="30" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Акцент1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -1483,13 +1524,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="43"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="57"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -1534,12 +1575,12 @@
       <c r="E3" s="5">
         <v>0.75829999999999997</v>
       </c>
-      <c r="H3" s="41" t="s">
+      <c r="H3" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="42"/>
-      <c r="J3" s="42"/>
-      <c r="K3" s="43"/>
+      <c r="I3" s="56"/>
+      <c r="J3" s="56"/>
+      <c r="K3" s="57"/>
     </row>
     <row r="4" spans="1:15" ht="15.75" thickBot="1">
       <c r="A4" s="20" t="s">
@@ -1628,13 +1669,13 @@
       </c>
     </row>
     <row r="8" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A8" s="41" t="s">
+      <c r="A8" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="42"/>
-      <c r="C8" s="42"/>
-      <c r="D8" s="42"/>
-      <c r="E8" s="43"/>
+      <c r="B8" s="56"/>
+      <c r="C8" s="56"/>
+      <c r="D8" s="56"/>
+      <c r="E8" s="57"/>
       <c r="H8" s="20" t="s">
         <v>28</v>
       </c>
@@ -1718,13 +1759,13 @@
     </row>
     <row r="14" spans="1:15" ht="15.75" thickBot="1"/>
     <row r="15" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A15" s="41" t="s">
+      <c r="A15" s="55" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="42"/>
-      <c r="C15" s="42"/>
-      <c r="D15" s="42"/>
-      <c r="E15" s="43"/>
+      <c r="B15" s="56"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="56"/>
+      <c r="E15" s="57"/>
     </row>
     <row r="16" spans="1:15" ht="15.75" thickBot="1">
       <c r="A16" s="4" t="s">
@@ -1796,13 +1837,13 @@
     </row>
     <row r="22" spans="1:5" ht="15.75" thickBot="1"/>
     <row r="23" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A23" s="38" t="s">
+      <c r="A23" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="39"/>
-      <c r="C23" s="39"/>
-      <c r="D23" s="39"/>
-      <c r="E23" s="40"/>
+      <c r="B23" s="53"/>
+      <c r="C23" s="53"/>
+      <c r="D23" s="53"/>
+      <c r="E23" s="54"/>
     </row>
     <row r="24" spans="1:5" ht="15.75" thickBot="1">
       <c r="A24" s="4" t="s">
@@ -2027,22 +2068,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:CZ46"/>
+  <dimension ref="A1:CZ53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AM19" workbookViewId="0">
-      <selection activeCell="P42" sqref="P42:P44"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="G63" sqref="G63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:103">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
     </row>
     <row r="2" spans="1:103">
       <c r="A2" s="25" t="s">
@@ -3605,13 +3646,13 @@
       <c r="CY7" s="27"/>
     </row>
     <row r="8" spans="1:103">
-      <c r="A8" s="45" t="s">
+      <c r="A8" s="59" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="45"/>
-      <c r="C8" s="45"/>
-      <c r="D8" s="45"/>
-      <c r="E8" s="45"/>
+      <c r="B8" s="59"/>
+      <c r="C8" s="59"/>
+      <c r="D8" s="59"/>
+      <c r="E8" s="59"/>
       <c r="CY8" s="27"/>
     </row>
     <row r="9" spans="1:103">
@@ -5175,13 +5216,13 @@
       <c r="CY14" s="27"/>
     </row>
     <row r="15" spans="1:103">
-      <c r="A15" s="45" t="s">
+      <c r="A15" s="59" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="45"/>
-      <c r="C15" s="45"/>
-      <c r="D15" s="45"/>
-      <c r="E15" s="45"/>
+      <c r="B15" s="59"/>
+      <c r="C15" s="59"/>
+      <c r="D15" s="59"/>
+      <c r="E15" s="59"/>
       <c r="CY15" s="27"/>
     </row>
     <row r="16" spans="1:103">
@@ -6742,13 +6783,13 @@
       </c>
     </row>
     <row r="23" spans="1:103">
-      <c r="A23" s="45" t="s">
+      <c r="A23" s="59" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="45"/>
-      <c r="C23" s="45"/>
-      <c r="D23" s="45"/>
-      <c r="E23" s="45"/>
+      <c r="B23" s="59"/>
+      <c r="C23" s="59"/>
+      <c r="D23" s="59"/>
+      <c r="E23" s="59"/>
     </row>
     <row r="24" spans="1:103">
       <c r="A24" s="25" t="s">
@@ -7575,13 +7616,13 @@
       </c>
     </row>
     <row r="32" spans="1:103">
-      <c r="A32" s="45" t="s">
+      <c r="A32" s="59" t="s">
         <v>42</v>
       </c>
-      <c r="B32" s="45"/>
-      <c r="C32" s="45"/>
-      <c r="D32" s="45"/>
-      <c r="E32" s="45"/>
+      <c r="B32" s="59"/>
+      <c r="C32" s="59"/>
+      <c r="D32" s="59"/>
+      <c r="E32" s="59"/>
     </row>
     <row r="33" spans="1:104">
       <c r="A33" s="25" t="s">
@@ -10711,8 +10752,843 @@
         <v>51.166699999999999</v>
       </c>
     </row>
+    <row r="48" spans="1:104">
+      <c r="A48" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="B48" s="59"/>
+      <c r="C48" s="59"/>
+      <c r="D48" s="59"/>
+      <c r="E48" s="59"/>
+      <c r="F48" s="59"/>
+    </row>
+    <row r="49" spans="1:54">
+      <c r="A49" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="B49" s="25">
+        <v>1</v>
+      </c>
+      <c r="C49" s="25">
+        <v>2</v>
+      </c>
+      <c r="D49" s="25">
+        <v>3</v>
+      </c>
+      <c r="E49" s="25">
+        <v>4</v>
+      </c>
+      <c r="F49" s="25">
+        <v>5</v>
+      </c>
+      <c r="G49" s="25">
+        <v>6</v>
+      </c>
+      <c r="H49" s="25">
+        <v>7</v>
+      </c>
+      <c r="I49" s="25">
+        <v>8</v>
+      </c>
+      <c r="J49" s="25">
+        <v>9</v>
+      </c>
+      <c r="K49" s="25">
+        <v>10</v>
+      </c>
+      <c r="L49" s="25">
+        <v>11</v>
+      </c>
+      <c r="M49" s="25">
+        <v>20</v>
+      </c>
+      <c r="N49" s="25">
+        <v>21</v>
+      </c>
+      <c r="O49" s="25">
+        <v>22</v>
+      </c>
+      <c r="P49" s="25">
+        <v>23</v>
+      </c>
+      <c r="Q49" s="25">
+        <v>24</v>
+      </c>
+      <c r="R49" s="25">
+        <v>25</v>
+      </c>
+      <c r="S49" s="25">
+        <v>26</v>
+      </c>
+      <c r="T49" s="25">
+        <v>27</v>
+      </c>
+      <c r="U49" s="25">
+        <v>28</v>
+      </c>
+      <c r="V49" s="25">
+        <v>29</v>
+      </c>
+      <c r="W49" s="25">
+        <v>30</v>
+      </c>
+      <c r="X49" s="25">
+        <v>31</v>
+      </c>
+      <c r="Y49" s="25">
+        <v>32</v>
+      </c>
+      <c r="Z49" s="25">
+        <v>33</v>
+      </c>
+      <c r="AA49" s="25">
+        <v>34</v>
+      </c>
+      <c r="AB49" s="25">
+        <v>35</v>
+      </c>
+      <c r="AC49" s="25">
+        <v>36</v>
+      </c>
+      <c r="AD49" s="25">
+        <v>37</v>
+      </c>
+      <c r="AE49" s="25">
+        <v>38</v>
+      </c>
+      <c r="AF49" s="25">
+        <v>39</v>
+      </c>
+      <c r="AG49" s="25">
+        <v>40</v>
+      </c>
+      <c r="AH49" s="25">
+        <v>41</v>
+      </c>
+      <c r="AI49" s="25">
+        <v>42</v>
+      </c>
+      <c r="AJ49" s="25">
+        <v>43</v>
+      </c>
+      <c r="AK49" s="25">
+        <v>44</v>
+      </c>
+      <c r="AL49" s="25">
+        <v>45</v>
+      </c>
+      <c r="AM49" s="25">
+        <v>46</v>
+      </c>
+      <c r="AN49" s="25">
+        <v>47</v>
+      </c>
+      <c r="AO49" s="25">
+        <v>48</v>
+      </c>
+      <c r="AP49" s="25">
+        <v>49</v>
+      </c>
+      <c r="AQ49" s="25">
+        <v>50</v>
+      </c>
+      <c r="AR49" s="25">
+        <v>51</v>
+      </c>
+      <c r="AS49" s="25">
+        <v>52</v>
+      </c>
+      <c r="AT49" s="25">
+        <v>53</v>
+      </c>
+      <c r="AU49" s="25">
+        <v>54</v>
+      </c>
+      <c r="AV49" s="25">
+        <v>55</v>
+      </c>
+      <c r="AW49" s="25">
+        <v>56</v>
+      </c>
+      <c r="AX49" s="25">
+        <v>57</v>
+      </c>
+      <c r="AY49" s="25">
+        <v>58</v>
+      </c>
+      <c r="AZ49" s="25">
+        <v>59</v>
+      </c>
+      <c r="BA49" s="25">
+        <v>60</v>
+      </c>
+      <c r="BB49" s="26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="50" spans="1:54">
+      <c r="A50" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="B50" s="23">
+        <v>60</v>
+      </c>
+      <c r="C50" s="23">
+        <v>54</v>
+      </c>
+      <c r="D50" s="23">
+        <v>52.083300000000001</v>
+      </c>
+      <c r="E50" s="23">
+        <v>49.5</v>
+      </c>
+      <c r="F50" s="23">
+        <v>50.916699999999999</v>
+      </c>
+      <c r="G50" s="23">
+        <v>52.416699999999999</v>
+      </c>
+      <c r="H50" s="23">
+        <v>50.666699999999999</v>
+      </c>
+      <c r="I50" s="23">
+        <v>50.583300000000001</v>
+      </c>
+      <c r="J50" s="23">
+        <v>55.5</v>
+      </c>
+      <c r="K50" s="23">
+        <v>56.166699999999999</v>
+      </c>
+      <c r="L50" s="23">
+        <v>54.416699999999999</v>
+      </c>
+      <c r="M50" s="23">
+        <v>61.416699999999999</v>
+      </c>
+      <c r="N50" s="23">
+        <v>59.916699999999999</v>
+      </c>
+      <c r="O50" s="23">
+        <v>61.333300000000001</v>
+      </c>
+      <c r="P50" s="23">
+        <v>59.166699999999999</v>
+      </c>
+      <c r="Q50" s="23">
+        <v>59.416699999999999</v>
+      </c>
+      <c r="R50" s="23">
+        <v>60.916699999999999</v>
+      </c>
+      <c r="S50" s="23">
+        <v>58.416699999999999</v>
+      </c>
+      <c r="T50" s="23">
+        <v>60.166699999999999</v>
+      </c>
+      <c r="U50" s="23">
+        <v>60</v>
+      </c>
+      <c r="V50" s="23">
+        <v>60.166699999999999</v>
+      </c>
+      <c r="W50" s="23">
+        <v>56.666699999999999</v>
+      </c>
+      <c r="X50" s="23">
+        <v>59</v>
+      </c>
+      <c r="Y50" s="23">
+        <v>56.666699999999999</v>
+      </c>
+      <c r="Z50" s="23">
+        <v>58.166699999999999</v>
+      </c>
+      <c r="AA50" s="23">
+        <v>54.666699999999999</v>
+      </c>
+      <c r="AB50" s="23">
+        <v>58.25</v>
+      </c>
+      <c r="AC50" s="23">
+        <v>57.083300000000001</v>
+      </c>
+      <c r="AD50" s="23">
+        <v>54.916699999999999</v>
+      </c>
+      <c r="AE50" s="23">
+        <v>58</v>
+      </c>
+      <c r="AF50" s="23">
+        <v>59.166699999999999</v>
+      </c>
+      <c r="AG50" s="23">
+        <v>59.833300000000001</v>
+      </c>
+      <c r="AH50" s="23">
+        <v>57.583300000000001</v>
+      </c>
+      <c r="AI50" s="23">
+        <v>58.25</v>
+      </c>
+      <c r="AJ50" s="23">
+        <v>57.916699999999999</v>
+      </c>
+      <c r="AK50" s="23">
+        <v>57.833300000000001</v>
+      </c>
+      <c r="AL50" s="23">
+        <v>57.083300000000001</v>
+      </c>
+      <c r="AM50" s="23">
+        <v>54.916699999999999</v>
+      </c>
+      <c r="AN50" s="23">
+        <v>55.666699999999999</v>
+      </c>
+      <c r="AO50" s="23">
+        <v>55.833300000000001</v>
+      </c>
+      <c r="AP50" s="23">
+        <v>56.666699999999999</v>
+      </c>
+      <c r="AQ50" s="23">
+        <v>55.583300000000001</v>
+      </c>
+      <c r="AR50" s="23">
+        <v>56.166699999999999</v>
+      </c>
+      <c r="AS50" s="23">
+        <v>54.083300000000001</v>
+      </c>
+      <c r="AT50" s="23">
+        <v>52.666699999999999</v>
+      </c>
+      <c r="AU50" s="23">
+        <v>55</v>
+      </c>
+      <c r="AV50" s="23">
+        <v>55.75</v>
+      </c>
+      <c r="AW50" s="23">
+        <v>54</v>
+      </c>
+      <c r="AX50" s="23">
+        <v>55.166699999999999</v>
+      </c>
+      <c r="AY50" s="23">
+        <v>53.083300000000001</v>
+      </c>
+      <c r="AZ50" s="23">
+        <v>52.666699999999999</v>
+      </c>
+      <c r="BA50" s="23">
+        <v>52.083300000000001</v>
+      </c>
+      <c r="BB50" s="23">
+        <f>MAX(B50:BA50)</f>
+        <v>61.416699999999999</v>
+      </c>
+    </row>
+    <row r="51" spans="1:54">
+      <c r="A51" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B51" s="23">
+        <v>81.916700000000006</v>
+      </c>
+      <c r="C51" s="23">
+        <v>79.333299999999994</v>
+      </c>
+      <c r="D51" s="23">
+        <v>77.583299999999994</v>
+      </c>
+      <c r="E51" s="23">
+        <v>76.083299999999994</v>
+      </c>
+      <c r="F51" s="23">
+        <v>81.083299999999994</v>
+      </c>
+      <c r="G51" s="23">
+        <v>76.5</v>
+      </c>
+      <c r="H51" s="23">
+        <v>74</v>
+      </c>
+      <c r="I51" s="23">
+        <v>73.583299999999994</v>
+      </c>
+      <c r="J51" s="23">
+        <v>72.083299999999994</v>
+      </c>
+      <c r="K51" s="23">
+        <v>69.166700000000006</v>
+      </c>
+      <c r="L51" s="23">
+        <v>70.75</v>
+      </c>
+      <c r="M51" s="23">
+        <v>71</v>
+      </c>
+      <c r="N51" s="23">
+        <v>70.166700000000006</v>
+      </c>
+      <c r="O51" s="23">
+        <v>71</v>
+      </c>
+      <c r="P51" s="23">
+        <v>71.166700000000006</v>
+      </c>
+      <c r="Q51" s="23">
+        <v>68.25</v>
+      </c>
+      <c r="R51" s="23">
+        <v>69.083299999999994</v>
+      </c>
+      <c r="S51" s="23">
+        <v>69.25</v>
+      </c>
+      <c r="T51" s="23">
+        <v>71.833299999999994</v>
+      </c>
+      <c r="U51" s="23">
+        <v>71.416700000000006</v>
+      </c>
+      <c r="V51" s="23">
+        <v>73.75</v>
+      </c>
+      <c r="W51" s="23">
+        <v>72.833299999999994</v>
+      </c>
+      <c r="X51" s="23">
+        <v>73.583299999999994</v>
+      </c>
+      <c r="Y51" s="23">
+        <v>73</v>
+      </c>
+      <c r="Z51" s="23">
+        <v>72.833299999999994</v>
+      </c>
+      <c r="AA51" s="23">
+        <v>74.583299999999994</v>
+      </c>
+      <c r="AB51" s="23">
+        <v>74.083299999999994</v>
+      </c>
+      <c r="AC51" s="23">
+        <v>73.583299999999994</v>
+      </c>
+      <c r="AD51" s="23">
+        <v>73.333299999999994</v>
+      </c>
+      <c r="AE51" s="23">
+        <v>73.833299999999994</v>
+      </c>
+      <c r="AF51" s="23">
+        <v>74</v>
+      </c>
+      <c r="AG51" s="23">
+        <v>73.416700000000006</v>
+      </c>
+      <c r="AH51" s="23">
+        <v>71.916700000000006</v>
+      </c>
+      <c r="AI51" s="23">
+        <v>72.583299999999994</v>
+      </c>
+      <c r="AJ51" s="23">
+        <v>73.5</v>
+      </c>
+      <c r="AK51" s="23">
+        <v>72.583299999999994</v>
+      </c>
+      <c r="AL51" s="23">
+        <v>70.833299999999994</v>
+      </c>
+      <c r="AM51" s="23">
+        <v>71.083299999999994</v>
+      </c>
+      <c r="AN51" s="23">
+        <v>74.416700000000006</v>
+      </c>
+      <c r="AO51" s="23">
+        <v>76.5</v>
+      </c>
+      <c r="AP51" s="23">
+        <v>74.916700000000006</v>
+      </c>
+      <c r="AQ51" s="23">
+        <v>75.333299999999994</v>
+      </c>
+      <c r="AR51" s="23">
+        <v>74.75</v>
+      </c>
+      <c r="AS51" s="23">
+        <v>74.916700000000006</v>
+      </c>
+      <c r="AT51" s="23">
+        <v>75.5</v>
+      </c>
+      <c r="AU51" s="23">
+        <v>74.916700000000006</v>
+      </c>
+      <c r="AV51" s="23">
+        <v>74.5</v>
+      </c>
+      <c r="AW51" s="23">
+        <v>74.666700000000006</v>
+      </c>
+      <c r="AX51" s="23">
+        <v>74.666700000000006</v>
+      </c>
+      <c r="AY51" s="23">
+        <v>75.333299999999994</v>
+      </c>
+      <c r="AZ51" s="23">
+        <v>75.333299999999994</v>
+      </c>
+      <c r="BA51" s="23">
+        <v>77.75</v>
+      </c>
+      <c r="BB51" s="23">
+        <f t="shared" ref="BB51:BB53" si="4">MAX(B51:BA51)</f>
+        <v>81.916700000000006</v>
+      </c>
+    </row>
+    <row r="52" spans="1:54">
+      <c r="A52" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="B52" s="23">
+        <v>72.083299999999994</v>
+      </c>
+      <c r="C52" s="23">
+        <v>68.5</v>
+      </c>
+      <c r="D52" s="23">
+        <v>79.416700000000006</v>
+      </c>
+      <c r="E52" s="23">
+        <v>80</v>
+      </c>
+      <c r="F52" s="23">
+        <v>78</v>
+      </c>
+      <c r="G52" s="23">
+        <v>75.916700000000006</v>
+      </c>
+      <c r="H52" s="23">
+        <v>73.583299999999994</v>
+      </c>
+      <c r="I52" s="23">
+        <v>72.083299999999994</v>
+      </c>
+      <c r="J52" s="23">
+        <v>71.333299999999994</v>
+      </c>
+      <c r="K52" s="23">
+        <v>70.416700000000006</v>
+      </c>
+      <c r="L52" s="23">
+        <v>73.166700000000006</v>
+      </c>
+      <c r="M52" s="23">
+        <v>73.166700000000006</v>
+      </c>
+      <c r="N52" s="23">
+        <v>74</v>
+      </c>
+      <c r="O52" s="23">
+        <v>73.916700000000006</v>
+      </c>
+      <c r="P52" s="23">
+        <v>70.75</v>
+      </c>
+      <c r="Q52" s="23">
+        <v>70.666700000000006</v>
+      </c>
+      <c r="R52" s="23">
+        <v>73.833299999999994</v>
+      </c>
+      <c r="S52" s="23">
+        <v>70.666700000000006</v>
+      </c>
+      <c r="T52" s="23">
+        <v>73.416700000000006</v>
+      </c>
+      <c r="U52" s="23">
+        <v>74.083299999999994</v>
+      </c>
+      <c r="V52" s="23">
+        <v>73.25</v>
+      </c>
+      <c r="W52" s="23">
+        <v>71.416700000000006</v>
+      </c>
+      <c r="X52" s="23">
+        <v>72.333299999999994</v>
+      </c>
+      <c r="Y52" s="23">
+        <v>72.083299999999994</v>
+      </c>
+      <c r="Z52" s="23">
+        <v>72.666700000000006</v>
+      </c>
+      <c r="AA52" s="23">
+        <v>71.75</v>
+      </c>
+      <c r="AB52" s="23">
+        <v>72.333299999999994</v>
+      </c>
+      <c r="AC52" s="23">
+        <v>72.083299999999994</v>
+      </c>
+      <c r="AD52" s="23">
+        <v>72</v>
+      </c>
+      <c r="AE52" s="23">
+        <v>70.833299999999994</v>
+      </c>
+      <c r="AF52" s="23">
+        <v>71.333299999999994</v>
+      </c>
+      <c r="AG52" s="23">
+        <v>72.166700000000006</v>
+      </c>
+      <c r="AH52" s="23">
+        <v>72.083299999999994</v>
+      </c>
+      <c r="AI52" s="23">
+        <v>71</v>
+      </c>
+      <c r="AJ52" s="23">
+        <v>71.5</v>
+      </c>
+      <c r="AK52" s="23">
+        <v>71.333299999999994</v>
+      </c>
+      <c r="AL52" s="23">
+        <v>70.416700000000006</v>
+      </c>
+      <c r="AM52" s="23">
+        <v>69.583299999999994</v>
+      </c>
+      <c r="AN52" s="23">
+        <v>69.833299999999994</v>
+      </c>
+      <c r="AO52" s="23">
+        <v>68.833299999999994</v>
+      </c>
+      <c r="AP52" s="23">
+        <v>69.666700000000006</v>
+      </c>
+      <c r="AQ52" s="23">
+        <v>69</v>
+      </c>
+      <c r="AR52" s="23">
+        <v>68.666700000000006</v>
+      </c>
+      <c r="AS52" s="23">
+        <v>69.916700000000006</v>
+      </c>
+      <c r="AT52" s="23">
+        <v>69.166700000000006</v>
+      </c>
+      <c r="AU52" s="23">
+        <v>69.75</v>
+      </c>
+      <c r="AV52" s="23">
+        <v>70.333299999999994</v>
+      </c>
+      <c r="AW52" s="23">
+        <v>69.416700000000006</v>
+      </c>
+      <c r="AX52" s="23">
+        <v>68.833299999999994</v>
+      </c>
+      <c r="AY52" s="23">
+        <v>69.083299999999994</v>
+      </c>
+      <c r="AZ52" s="23">
+        <v>69.333299999999994</v>
+      </c>
+      <c r="BA52" s="23">
+        <v>68.333299999999994</v>
+      </c>
+      <c r="BB52" s="23">
+        <f t="shared" si="4"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="53" spans="1:54">
+      <c r="A53" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B53" s="23">
+        <v>52.25</v>
+      </c>
+      <c r="C53" s="23">
+        <v>48.583300000000001</v>
+      </c>
+      <c r="D53" s="23">
+        <v>47.333300000000001</v>
+      </c>
+      <c r="E53" s="23">
+        <v>47.666699999999999</v>
+      </c>
+      <c r="F53" s="23">
+        <v>51.666699999999999</v>
+      </c>
+      <c r="G53" s="23">
+        <v>52</v>
+      </c>
+      <c r="H53" s="23">
+        <v>52</v>
+      </c>
+      <c r="I53" s="23">
+        <v>51</v>
+      </c>
+      <c r="J53" s="23">
+        <v>46.833300000000001</v>
+      </c>
+      <c r="K53" s="23">
+        <v>48.916699999999999</v>
+      </c>
+      <c r="L53" s="23">
+        <v>47</v>
+      </c>
+      <c r="M53" s="23">
+        <v>53.166699999999999</v>
+      </c>
+      <c r="N53" s="23">
+        <v>50.5</v>
+      </c>
+      <c r="O53" s="23">
+        <v>49.083300000000001</v>
+      </c>
+      <c r="P53" s="23">
+        <v>48.25</v>
+      </c>
+      <c r="Q53" s="23">
+        <v>47.666699999999999</v>
+      </c>
+      <c r="R53" s="23">
+        <v>48.583300000000001</v>
+      </c>
+      <c r="S53" s="23">
+        <v>47.333300000000001</v>
+      </c>
+      <c r="T53" s="23">
+        <v>48.166699999999999</v>
+      </c>
+      <c r="U53" s="23">
+        <v>49.75</v>
+      </c>
+      <c r="V53" s="23">
+        <v>49.75</v>
+      </c>
+      <c r="W53" s="23">
+        <v>47.166699999999999</v>
+      </c>
+      <c r="X53" s="23">
+        <v>47.333300000000001</v>
+      </c>
+      <c r="Y53" s="23">
+        <v>48.25</v>
+      </c>
+      <c r="Z53" s="23">
+        <v>46.833300000000001</v>
+      </c>
+      <c r="AA53" s="23">
+        <v>47.083300000000001</v>
+      </c>
+      <c r="AB53" s="23">
+        <v>47.75</v>
+      </c>
+      <c r="AC53" s="23">
+        <v>48.666699999999999</v>
+      </c>
+      <c r="AD53" s="23">
+        <v>46.666699999999999</v>
+      </c>
+      <c r="AE53" s="23">
+        <v>47.166699999999999</v>
+      </c>
+      <c r="AF53" s="23">
+        <v>50.75</v>
+      </c>
+      <c r="AG53" s="23">
+        <v>48.083300000000001</v>
+      </c>
+      <c r="AH53" s="23">
+        <v>47.666699999999999</v>
+      </c>
+      <c r="AI53" s="23">
+        <v>48.75</v>
+      </c>
+      <c r="AJ53" s="23">
+        <v>47.666699999999999</v>
+      </c>
+      <c r="AK53" s="23">
+        <v>47.833300000000001</v>
+      </c>
+      <c r="AL53" s="23">
+        <v>46.583300000000001</v>
+      </c>
+      <c r="AM53" s="23">
+        <v>46.833300000000001</v>
+      </c>
+      <c r="AN53" s="23">
+        <v>46.75</v>
+      </c>
+      <c r="AO53" s="23">
+        <v>48.25</v>
+      </c>
+      <c r="AP53" s="23">
+        <v>46.416699999999999</v>
+      </c>
+      <c r="AQ53" s="23">
+        <v>43.416699999999999</v>
+      </c>
+      <c r="AR53" s="23">
+        <v>45</v>
+      </c>
+      <c r="AS53" s="23">
+        <v>43.833300000000001</v>
+      </c>
+      <c r="AT53" s="23">
+        <v>43.25</v>
+      </c>
+      <c r="AU53" s="23">
+        <v>42.583300000000001</v>
+      </c>
+      <c r="AV53" s="23">
+        <v>42.916699999999999</v>
+      </c>
+      <c r="AW53" s="23">
+        <v>42.666699999999999</v>
+      </c>
+      <c r="AX53" s="23">
+        <v>43.166699999999999</v>
+      </c>
+      <c r="AY53" s="23">
+        <v>41.166699999999999</v>
+      </c>
+      <c r="AZ53" s="23">
+        <v>42.25</v>
+      </c>
+      <c r="BA53" s="23">
+        <v>45.166699999999999</v>
+      </c>
+      <c r="BB53" s="23">
+        <f t="shared" si="4"/>
+        <v>53.166699999999999</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="A48:F48"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A8:E8"/>
     <mergeCell ref="A15:E15"/>
@@ -11264,50 +12140,59 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:E24"/>
+  <dimension ref="A2:O24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="H6" sqref="H6:N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="8" max="8" width="15" customWidth="1"/>
+    <col min="9" max="9" width="15" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="8.28515625" customWidth="1"/>
+    <col min="11" max="11" width="11.85546875" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" customWidth="1"/>
+    <col min="13" max="13" width="13.140625" customWidth="1"/>
+    <col min="14" max="14" width="12.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:15">
       <c r="A2" s="23"/>
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="46" t="s">
+      <c r="C2" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="D2" s="46" t="s">
+      <c r="D2" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="E2" s="46" t="s">
+      <c r="E2" s="38" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="46">
+    <row r="3" spans="1:15">
+      <c r="A3" s="38">
         <v>1</v>
       </c>
-      <c r="B3" s="50">
+      <c r="B3" s="42">
         <v>0.6</v>
       </c>
-      <c r="C3" s="51">
+      <c r="C3" s="43">
         <v>0.66666669999999995</v>
       </c>
-      <c r="D3" s="57">
+      <c r="D3" s="49">
         <f>C3-B3</f>
         <v>6.6666699999999968E-2</v>
       </c>
-      <c r="E3" s="54">
-        <f>($D$23 - D3) * ($D$23 - D3)</f>
+      <c r="E3" s="46">
+        <f t="shared" ref="E3:E22" si="0">($D$23 - D3) * ($D$23 - D3)</f>
         <v>2.7776388906250164E-6</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="46">
+    <row r="4" spans="1:15">
+      <c r="A4" s="38">
         <v>1</v>
       </c>
       <c r="B4" s="30">
@@ -11316,17 +12201,17 @@
       <c r="C4" s="27">
         <v>0.43333329999999998</v>
       </c>
-      <c r="D4" s="58">
-        <f t="shared" ref="D4:D22" si="0">C4-B4</f>
+      <c r="D4" s="50">
+        <f t="shared" ref="D4:D22" si="1">C4-B4</f>
         <v>-0.1666667</v>
       </c>
-      <c r="E4" s="55">
-        <f>($D$23 - D4) * ($D$23 - D4)</f>
+      <c r="E4" s="47">
+        <f t="shared" si="0"/>
         <v>5.5225011750000615E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="46">
+    <row r="5" spans="1:15">
+      <c r="A5" s="38">
         <v>1</v>
       </c>
       <c r="B5" s="30">
@@ -11335,17 +12220,17 @@
       <c r="C5" s="27">
         <v>0.7</v>
       </c>
-      <c r="D5" s="58">
+      <c r="D5" s="50">
+        <f t="shared" si="1"/>
+        <v>9.9999999999999978E-2</v>
+      </c>
+      <c r="E5" s="47">
         <f t="shared" si="0"/>
-        <v>9.9999999999999978E-2</v>
-      </c>
-      <c r="E5" s="55">
-        <f>($D$23 - D5) * ($D$23 - D5)</f>
         <v>1.0027783055556252E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="46">
+    <row r="6" spans="1:15" ht="29.25" customHeight="1">
+      <c r="A6" s="38">
         <v>1</v>
       </c>
       <c r="B6" s="30">
@@ -11354,17 +12239,39 @@
       <c r="C6" s="27">
         <v>0.46666669999999999</v>
       </c>
-      <c r="D6" s="58">
+      <c r="D6" s="50">
+        <f t="shared" si="1"/>
+        <v>-9.9999999999999978E-2</v>
+      </c>
+      <c r="E6" s="47">
         <f t="shared" si="0"/>
-        <v>-9.9999999999999978E-2</v>
-      </c>
-      <c r="E6" s="55">
-        <f>($D$23 - D6) * ($D$23 - D6)</f>
         <v>2.8336108305555607E-2</v>
       </c>
+      <c r="H6" s="60" t="s">
+        <v>59</v>
+      </c>
+      <c r="I6" s="60" t="s">
+        <v>61</v>
+      </c>
+      <c r="J6" s="60" t="s">
+        <v>63</v>
+      </c>
+      <c r="K6" s="60" t="s">
+        <v>62</v>
+      </c>
+      <c r="L6" s="60" t="s">
+        <v>60</v>
+      </c>
+      <c r="M6" s="60" t="s">
+        <v>64</v>
+      </c>
+      <c r="N6" s="60" t="s">
+        <v>65</v>
+      </c>
+      <c r="O6" s="60"/>
     </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="46">
+    <row r="7" spans="1:15">
+      <c r="A7" s="38">
         <v>1</v>
       </c>
       <c r="B7" s="30">
@@ -11373,17 +12280,42 @@
       <c r="C7" s="27">
         <v>0.66666669999999995</v>
       </c>
-      <c r="D7" s="58">
+      <c r="D7" s="50">
+        <f t="shared" si="1"/>
+        <v>6.6666699999999968E-2</v>
+      </c>
+      <c r="E7" s="47">
         <f t="shared" si="0"/>
-        <v>6.6666699999999968E-2</v>
-      </c>
-      <c r="E7" s="55">
-        <f>($D$23 - D7) * ($D$23 - D7)</f>
         <v>2.7776388906250164E-6</v>
       </c>
+      <c r="H7" t="s">
+        <v>55</v>
+      </c>
+      <c r="I7">
+        <v>84.33</v>
+      </c>
+      <c r="J7">
+        <f xml:space="preserve"> 100 - I7</f>
+        <v>15.670000000000002</v>
+      </c>
+      <c r="K7">
+        <v>85.33</v>
+      </c>
+      <c r="L7">
+        <f xml:space="preserve"> 100 - K7</f>
+        <v>14.670000000000002</v>
+      </c>
+      <c r="M7">
+        <f xml:space="preserve"> J7 - L7</f>
+        <v>1</v>
+      </c>
+      <c r="N7" s="61">
+        <f xml:space="preserve"> M7  / J7</f>
+        <v>6.3816209317166556E-2</v>
+      </c>
     </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="46">
+    <row r="8" spans="1:15">
+      <c r="A8" s="38">
         <v>1</v>
       </c>
       <c r="B8" s="30">
@@ -11392,17 +12324,42 @@
       <c r="C8" s="27">
         <v>0.6</v>
       </c>
-      <c r="D8" s="58">
+      <c r="D8" s="50">
+        <f t="shared" si="1"/>
+        <v>0.19999999999999996</v>
+      </c>
+      <c r="E8" s="47">
         <f t="shared" si="0"/>
-        <v>0.19999999999999996</v>
-      </c>
-      <c r="E8" s="55">
-        <f>($D$23 - D8) * ($D$23 - D8)</f>
         <v>1.7336113305555619E-2</v>
       </c>
+      <c r="H8" t="s">
+        <v>56</v>
+      </c>
+      <c r="I8">
+        <v>53.67</v>
+      </c>
+      <c r="J8">
+        <f t="shared" ref="J8:J10" si="2" xml:space="preserve"> 100 - I8</f>
+        <v>46.33</v>
+      </c>
+      <c r="K8">
+        <v>60.5</v>
+      </c>
+      <c r="L8">
+        <f t="shared" ref="L8:L10" si="3" xml:space="preserve"> 100 - K8</f>
+        <v>39.5</v>
+      </c>
+      <c r="M8">
+        <f t="shared" ref="M8:M10" si="4" xml:space="preserve"> J8 - L8</f>
+        <v>6.8299999999999983</v>
+      </c>
+      <c r="N8" s="61">
+        <f t="shared" ref="N8:N10" si="5" xml:space="preserve"> M8  / J8</f>
+        <v>0.14742067774660045</v>
+      </c>
     </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="46">
+    <row r="9" spans="1:15">
+      <c r="A9" s="38">
         <v>1</v>
       </c>
       <c r="B9" s="30">
@@ -11411,17 +12368,42 @@
       <c r="C9" s="27">
         <v>0.56666669999999997</v>
       </c>
-      <c r="D9" s="58">
+      <c r="D9" s="50">
+        <f t="shared" si="1"/>
+        <v>3.3333399999999958E-2</v>
+      </c>
+      <c r="E9" s="47">
         <f t="shared" si="0"/>
-        <v>3.3333399999999958E-2</v>
-      </c>
-      <c r="E9" s="55">
-        <f>($D$23 - D9) * ($D$23 - D9)</f>
         <v>1.224994750005626E-3</v>
       </c>
+      <c r="H9" t="s">
+        <v>57</v>
+      </c>
+      <c r="I9">
+        <v>82.44</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="2"/>
+        <v>17.560000000000002</v>
+      </c>
+      <c r="K9">
+        <v>83.89</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="3"/>
+        <v>16.11</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="4"/>
+        <v>1.4500000000000028</v>
+      </c>
+      <c r="N9" s="61">
+        <f t="shared" si="5"/>
+        <v>8.2574031890660746E-2</v>
+      </c>
     </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="46">
+    <row r="10" spans="1:15">
+      <c r="A10" s="38">
         <v>1</v>
       </c>
       <c r="B10" s="30">
@@ -11430,17 +12412,42 @@
       <c r="C10" s="27">
         <v>0.63333329999999999</v>
       </c>
-      <c r="D10" s="58">
+      <c r="D10" s="50">
+        <f t="shared" si="1"/>
+        <v>0.1666666</v>
+      </c>
+      <c r="E10" s="47">
         <f t="shared" si="0"/>
-        <v>0.1666666</v>
-      </c>
-      <c r="E10" s="55">
-        <f>($D$23 - D10) * ($D$23 - D10)</f>
         <v>9.6694329722256302E-3</v>
       </c>
+      <c r="H10" t="s">
+        <v>58</v>
+      </c>
+      <c r="I10">
+        <v>48.78</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="2"/>
+        <v>51.22</v>
+      </c>
+      <c r="K10">
+        <v>50.67</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="3"/>
+        <v>49.33</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="4"/>
+        <v>1.8900000000000006</v>
+      </c>
+      <c r="N10" s="61">
+        <f t="shared" si="5"/>
+        <v>3.6899648574775491E-2</v>
+      </c>
     </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="46">
+    <row r="11" spans="1:15">
+      <c r="A11" s="38">
         <v>1</v>
       </c>
       <c r="B11" s="30">
@@ -11449,17 +12456,17 @@
       <c r="C11" s="27">
         <v>0.63333329999999999</v>
       </c>
-      <c r="D11" s="58">
+      <c r="D11" s="50">
+        <f t="shared" si="1"/>
+        <v>0.2</v>
+      </c>
+      <c r="E11" s="47">
         <f t="shared" si="0"/>
-        <v>0.2</v>
-      </c>
-      <c r="E11" s="55">
-        <f>($D$23 - D11) * ($D$23 - D11)</f>
         <v>1.7336113305555637E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="46">
+    <row r="12" spans="1:15">
+      <c r="A12" s="38">
         <v>1</v>
       </c>
       <c r="B12" s="30">
@@ -11468,17 +12475,17 @@
       <c r="C12" s="27">
         <v>0.73333329999999997</v>
       </c>
-      <c r="D12" s="58">
+      <c r="D12" s="50">
+        <f t="shared" si="1"/>
+        <v>6.666660000000002E-2</v>
+      </c>
+      <c r="E12" s="47">
         <f t="shared" si="0"/>
-        <v>6.666660000000002E-2</v>
-      </c>
-      <c r="E12" s="55">
-        <f>($D$23 - D12) * ($D$23 - D12)</f>
         <v>2.7779722256248408E-6</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="46">
+    <row r="13" spans="1:15">
+      <c r="A13" s="38">
         <v>1</v>
       </c>
       <c r="B13" s="30">
@@ -11487,17 +12494,17 @@
       <c r="C13" s="27">
         <v>0.73333329999999997</v>
       </c>
-      <c r="D13" s="58">
+      <c r="D13" s="50">
+        <f t="shared" si="1"/>
+        <v>0.23333329999999997</v>
+      </c>
+      <c r="E13" s="47">
         <f t="shared" si="0"/>
-        <v>0.23333329999999997</v>
-      </c>
-      <c r="E13" s="55">
-        <f>($D$23 - D13) * ($D$23 - D13)</f>
         <v>2.7224991750000621E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="46">
+    <row r="14" spans="1:15">
+      <c r="A14" s="38">
         <v>1</v>
       </c>
       <c r="B14" s="30">
@@ -11506,17 +12513,17 @@
       <c r="C14" s="27">
         <v>0.53333330000000001</v>
       </c>
-      <c r="D14" s="58">
+      <c r="D14" s="50">
+        <f t="shared" si="1"/>
+        <v>6.666660000000002E-2</v>
+      </c>
+      <c r="E14" s="47">
         <f t="shared" si="0"/>
-        <v>6.666660000000002E-2</v>
-      </c>
-      <c r="E14" s="55">
-        <f>($D$23 - D14) * ($D$23 - D14)</f>
         <v>2.7779722256248408E-6</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="46">
+    <row r="15" spans="1:15">
+      <c r="A15" s="38">
         <v>1</v>
       </c>
       <c r="B15" s="30">
@@ -11525,17 +12532,17 @@
       <c r="C15" s="27">
         <v>0.6</v>
       </c>
-      <c r="D15" s="58">
+      <c r="D15" s="50">
+        <f t="shared" si="1"/>
+        <v>0.19999999999999996</v>
+      </c>
+      <c r="E15" s="47">
         <f t="shared" si="0"/>
-        <v>0.19999999999999996</v>
-      </c>
-      <c r="E15" s="55">
-        <f>($D$23 - D15) * ($D$23 - D15)</f>
         <v>1.7336113305555619E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="46">
+    <row r="16" spans="1:15">
+      <c r="A16" s="38">
         <v>1</v>
       </c>
       <c r="B16" s="30">
@@ -11544,17 +12551,17 @@
       <c r="C16" s="27">
         <v>0.63333329999999999</v>
       </c>
-      <c r="D16" s="58">
+      <c r="D16" s="50">
+        <f t="shared" si="1"/>
+        <v>6.666660000000002E-2</v>
+      </c>
+      <c r="E16" s="47">
         <f t="shared" si="0"/>
-        <v>6.666660000000002E-2</v>
-      </c>
-      <c r="E16" s="55">
-        <f>($D$23 - D16) * ($D$23 - D16)</f>
         <v>2.7779722256248408E-6</v>
       </c>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="46">
+      <c r="A17" s="38">
         <v>1</v>
       </c>
       <c r="B17" s="30">
@@ -11563,17 +12570,17 @@
       <c r="C17" s="27">
         <v>0.5</v>
       </c>
-      <c r="D17" s="58">
+      <c r="D17" s="50">
+        <f t="shared" si="1"/>
+        <v>-0.13333329999999999</v>
+      </c>
+      <c r="E17" s="47">
         <f t="shared" si="0"/>
-        <v>-0.13333329999999999</v>
-      </c>
-      <c r="E17" s="55">
-        <f>($D$23 - D17) * ($D$23 - D17)</f>
         <v>4.0669427638890608E-2</v>
       </c>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="46">
+      <c r="A18" s="38">
         <v>1</v>
       </c>
       <c r="B18" s="30">
@@ -11582,17 +12589,17 @@
       <c r="C18" s="27">
         <v>0.66666669999999995</v>
       </c>
-      <c r="D18" s="58">
+      <c r="D18" s="50">
+        <f t="shared" si="1"/>
+        <v>9.9999999999999978E-2</v>
+      </c>
+      <c r="E18" s="47">
         <f t="shared" si="0"/>
-        <v>9.9999999999999978E-2</v>
-      </c>
-      <c r="E18" s="55">
-        <f>($D$23 - D18) * ($D$23 - D18)</f>
         <v>1.0027783055556252E-3</v>
       </c>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="46">
+      <c r="A19" s="38">
         <v>1</v>
       </c>
       <c r="B19" s="30">
@@ -11601,17 +12608,17 @@
       <c r="C19" s="27">
         <v>0.5</v>
       </c>
-      <c r="D19" s="58">
+      <c r="D19" s="50">
+        <f t="shared" si="1"/>
+        <v>0.13333329999999999</v>
+      </c>
+      <c r="E19" s="47">
         <f t="shared" si="0"/>
-        <v>0.13333329999999999</v>
-      </c>
-      <c r="E19" s="55">
-        <f>($D$23 - D19) * ($D$23 - D19)</f>
         <v>4.2249967500006267E-3</v>
       </c>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="46">
+      <c r="A20" s="38">
         <v>1</v>
       </c>
       <c r="B20" s="30">
@@ -11620,17 +12627,17 @@
       <c r="C20" s="27">
         <v>0.6</v>
       </c>
-      <c r="D20" s="58">
+      <c r="D20" s="50">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E20" s="47">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E20" s="55">
-        <f>($D$23 - D20) * ($D$23 - D20)</f>
         <v>4.6694433055556213E-3</v>
       </c>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="46">
+      <c r="A21" s="38">
         <v>1</v>
       </c>
       <c r="B21" s="30">
@@ -11639,51 +12646,51 @@
       <c r="C21" s="27">
         <v>0.56666669999999997</v>
       </c>
-      <c r="D21" s="58">
+      <c r="D21" s="50">
+        <f t="shared" si="1"/>
+        <v>-3.333330000000001E-2</v>
+      </c>
+      <c r="E21" s="47">
         <f t="shared" si="0"/>
-        <v>-3.333330000000001E-2</v>
-      </c>
-      <c r="E21" s="55">
-        <f>($D$23 - D21) * ($D$23 - D21)</f>
         <v>1.0336102638890621E-2</v>
       </c>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="46">
+      <c r="A22" s="38">
         <v>1</v>
       </c>
-      <c r="B22" s="52">
+      <c r="B22" s="44">
         <v>0.56666669999999997</v>
       </c>
-      <c r="C22" s="53">
+      <c r="C22" s="45">
         <v>0.66666669999999995</v>
       </c>
-      <c r="D22" s="59">
+      <c r="D22" s="51">
+        <f t="shared" si="1"/>
+        <v>9.9999999999999978E-2</v>
+      </c>
+      <c r="E22" s="48">
         <f t="shared" si="0"/>
-        <v>9.9999999999999978E-2</v>
-      </c>
-      <c r="E22" s="56">
-        <f>($D$23 - D22) * ($D$23 - D22)</f>
         <v>1.0027783055556252E-3</v>
       </c>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="47" t="s">
+      <c r="A23" s="39" t="s">
         <v>48</v>
       </c>
-      <c r="B23" s="48">
-        <f t="shared" ref="B23:C23" si="1">AVERAGE(B3:B22)</f>
+      <c r="B23" s="40">
+        <f t="shared" ref="B23:C23" si="6">AVERAGE(B3:B22)</f>
         <v>0.53666667499999998</v>
       </c>
-      <c r="C23" s="48">
-        <f t="shared" si="1"/>
+      <c r="C23" s="40">
+        <f t="shared" si="6"/>
         <v>0.60500000000000009</v>
       </c>
-      <c r="D23" s="48">
+      <c r="D23" s="40">
         <f>AVERAGE(D3:D22)</f>
         <v>6.8333324999999973E-2</v>
       </c>
-      <c r="E23" s="48">
+      <c r="E23" s="40">
         <f>SUM(E3:E22)/(COUNT(E3:E22) *(COUNT(E3:E22)  - 1))</f>
         <v>6.2266072076030911E-4</v>
       </c>
@@ -11692,12 +12699,13 @@
       <c r="D24" t="s">
         <v>49</v>
       </c>
-      <c r="E24" s="49">
+      <c r="E24" s="41">
         <f>$D$23/SQRT($E$23)</f>
         <v>2.7384626273703292</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>